<commit_message>
corrected a bug in create.climate.data
</commit_message>
<xml_diff>
--- a/for_development/dev_documentation/soil-root-calibration_V3.xlsx
+++ b/for_development/dev_documentation/soil-root-calibration_V3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jruffault/Dropbox/Mon Mac (MacBook-Pro-de-Julien.local)/Desktop/SurEau-Ecos/for_development/dev_documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AFC141A-80FF-AB4A-9672-AB7D04491BA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBCF6A83-8C74-4548-BC01-F69A26918516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8000" yWindow="500" windowWidth="31000" windowHeight="17440" activeTab="2" xr2:uid="{D9106142-DCBD-4E45-A888-1E539F445614}"/>
+    <workbookView xWindow="7400" yWindow="500" windowWidth="31000" windowHeight="17440" xr2:uid="{D9106142-DCBD-4E45-A888-1E539F445614}"/>
   </bookViews>
   <sheets>
     <sheet name="WorkSheet" sheetId="1" r:id="rId1"/>
@@ -1267,7 +1267,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="54">
+  <fonts count="54" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2685,157 +2685,157 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>4.5925888793794001E-4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.3151616380458741</c:v>
+                  <c:v>1.3616134230305676E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.63198540354745669</c:v>
+                  <c:v>2.8715960862765442E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.0674570918195458</c:v>
+                  <c:v>5.3370317102745014E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.6601715815122597</c:v>
+                  <c:v>9.1935735207933876E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.4496312980403321</c:v>
+                  <c:v>1.5003057720066113E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.4792992790446222</c:v>
+                  <c:v>2.3480243747916522E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.797472666616958</c:v>
+                  <c:v>3.5520236959888214E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.4577430798151498</c:v>
+                  <c:v>5.2228000126832846E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8.5193428946556011</c:v>
+                  <c:v>7.4950331077162757E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>11.047455427394711</c:v>
+                  <c:v>0.10531049791441752</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>14.113515381749325</c:v>
+                  <c:v>0.14524568383104364</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>17.795510444050191</c:v>
+                  <c:v>0.19704739054208348</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>22.178289437616584</c:v>
+                  <c:v>0.26340495830866423</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>27.353880277730777</c:v>
+                  <c:v>0.34745237470956025</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>33.421820043549261</c:v>
+                  <c:v>0.45281856168104484</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>40.489499080792143</c:v>
+                  <c:v>0.58368135024671663</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>48.672520887942895</c:v>
+                  <c:v>0.74482537467739096</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>58.095079500288271</c:v>
+                  <c:v>0.94170414265257341</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>68.890356117025519</c:v>
+                  <c:v>1.1805065655457774</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>81.200936791782354</c:v>
+                  <c:v>1.4682282635072366</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>95.179253114226654</c:v>
+                  <c:v>1.812747993913171</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>110.98804794451044</c:v>
+                  <c:v>2.2229095893939594</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>128.80086842093311</c:v>
+                  <c:v>2.7086098335157511</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>148.80258864436263</c:v>
+                  <c:v>3.2808927488128257</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>171.18996465163156</c:v>
+                  <c:v>3.9520508238798979</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>196.17222452644145</c:v>
+                  <c:v>4.7357337643565272</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>223.97169676289931</c:v>
+                  <c:v>5.6470654177066297</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>254.82448029719598</c:v>
+                  <c:v>6.7027695946832884</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>288.98115996122215</c:v>
+                  <c:v>7.9213055923924749</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>326.70757149298095</c:v>
+                  <c:v>9.3230143162290542</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>368.28562066833882</c:v>
+                  <c:v>10.930276002175972</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>414.01416160356581</c:v>
+                  <c:v>12.767680658793845</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>464.20993982626999</c:v>
+                  <c:v>14.862212481749824</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>519.20860633287589</c:v>
+                  <c:v>17.243449645369402</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>579.36580955449483</c:v>
+                  <c:v>19.94378104827738</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>645.0583729527134</c:v>
+                  <c:v>22.998641787083621</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>716.68556687722617</c:v>
+                  <c:v>26.446769357223328</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>794.6704843560924</c:v>
+                  <c:v>30.330482838165832</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>879.46153167748651</c:v>
+                  <c:v>34.695987616838806</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>971.53404598375982</c:v>
+                  <c:v>39.59370854492181</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>1071.3920536639166</c:v>
+                  <c:v>45.078654820580034</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>1179.570185134248</c:v>
+                  <c:v>51.210820342780124</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>1296.6357636807979</c:v>
+                  <c:v>58.055623818019448</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>1423.1910884521617</c:v>
+                  <c:v>65.684393518993474</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>1559.8759344976083</c:v>
+                  <c:v>74.174902319225055</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>1707.3702960174396</c:v>
+                  <c:v>83.611959477491524</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>1866.3974028194343</c:v>
+                  <c:v>94.088066646031905</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>2037.7270444667847</c:v>
+                  <c:v>105.70414675778086</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>2222.179241892828</c:v>
+                  <c:v>118.57035584815631</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>2420.6283125120053</c:v>
+                  <c:v>132.80698953325199</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3096,157 +3096,157 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>4.5910480274279379E-4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.25616308056217729</c:v>
+                  <c:v>1.3602598950913313E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.43231966606274191</c:v>
+                  <c:v>2.8655825797312406E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.599666355615326</c:v>
+                  <c:v>5.316296878539792E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.75011127189451954</c:v>
+                  <c:v>9.1322182127808633E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.87795320772144447</c:v>
+                  <c:v>1.4840347305453874E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.98212304083342128</c:v>
+                  <c:v>2.3084141026052558E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.064700517580168</c:v>
+                  <c:v>3.4621539051072632E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.1291256461405335</c:v>
+                  <c:v>5.0307869269171697E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.1790115489589372</c:v>
+                  <c:v>7.1058269614329539E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.2175718763409391</c:v>
+                  <c:v>9.778499721024439E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.2474392613862997</c:v>
+                  <c:v>0.13130813576865469</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.2706769055200273</c:v>
+                  <c:v>0.17224423734157626</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.2888635744675236</c:v>
+                  <c:v>0.22088591565340021</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.3031929951786028</c:v>
+                  <c:v>0.27709424360789786</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.3145635734887848</c:v>
+                  <c:v>0.34023115666120018</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.3236513896316358</c:v>
+                  <c:v>0.409156639513995</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.3309666240786677</c:v>
+                  <c:v>0.48230315270739788</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.3368960200306046</c:v>
+                  <c:v>0.55782005427798043</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.3417344023301796</c:v>
+                  <c:v>0.63376089545272862</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.3457079317850806</c:v>
+                  <c:v>0.70827490266880677</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.3489912386390328</c:v>
+                  <c:v>0.77976550527831168</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1.3517200665445663</c:v>
+                  <c:v>0.84699176825559819</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1.3540006360667187</c:v>
+                  <c:v>0.90910640943844057</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1.3559166114295176</c:v>
+                  <c:v>0.96563940463757103</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1.3575343122340857</c:v>
+                  <c:v>1.0164447024421746</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1.3589066352184731</c:v>
+                  <c:v>1.0616289552302225</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1.3600760233933222</c:v>
+                  <c:v>1.1014777167099887</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1.3610767279048599</c:v>
+                  <c:v>1.1363891703321813</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1.3619365417824301</c:v>
+                  <c:v>1.166820321044034</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1.3626781370146528</c:v>
+                  <c:v>1.1932467762058712</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1.3633201018994123</c:v>
+                  <c:v>1.2161349505004408</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1.3638777505661861</c:v>
+                  <c:v>1.2359244757316503</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>1.3643637582986048</c:v>
+                  <c:v>1.253018363735048</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1.3647886628885679</c:v>
+                  <c:v>1.2677786885825035</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1.3651612623773528</c:v>
+                  <c:v>1.2805259605188766</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1.3654889322183295</c:v>
+                  <c:v>1.2915408019288817</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>1.3657778794388025</c:v>
+                  <c:v>1.3010669269379471</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>1.3660333472879647</c:v>
+                  <c:v>1.3093147422195068</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1.366259780774854</c:v>
+                  <c:v>1.3164651252438047</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1.3664609611637988</c:v>
+                  <c:v>1.3226731077108129</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>1.3666401157148349</c:v>
+                  <c:v>1.3280713101470438</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>1.3668000075934463</c:v>
+                  <c:v>1.3327730520587682</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>1.3669430098247448</c:v>
+                  <c:v>1.3368751119396871</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>1.3670711663556274</c:v>
+                  <c:v>1.3404601416348407</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>1.3671862426576684</c:v>
+                  <c:v>1.3435987565710525</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>1.367289767810949</c:v>
+                  <c:v>1.346351331808286</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>1.3673830696226883</c:v>
+                  <c:v>1.3487695369447354</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>1.3674673040301519</c:v>
+                  <c:v>1.3508976427741337</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>1.3675434797965111</c:v>
+                  <c:v>1.3527736306600466</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>1.3676124793169921</c:v>
+                  <c:v>1.3544301327622559</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3754,7 +3754,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.28000000000000003</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3766,7 +3766,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.28000000000000003</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4296,58 +4296,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>-3.5944401511222881</c:v>
+                  <c:v>-40.03627388240605</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1.7888543819998328</c:v>
+                  <c:v>-15.812802138851525</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-1.1832159566199236</c:v>
+                  <c:v>-8.573309019436488</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.87749643873921235</c:v>
+                  <c:v>-5.4251618951836793</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.69166465863162352</c:v>
+                  <c:v>-3.7628840854179857</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.56568542494923824</c:v>
+                  <c:v>-2.7733271364219005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.47380354147934278</c:v>
+                  <c:v>-2.1340109821626103</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.40311288741492773</c:v>
+                  <c:v>-1.695629994580736</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.34641016151377546</c:v>
+                  <c:v>-1.3810808706842324</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.29933259094191533</c:v>
+                  <c:v>-1.1471658159994846</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.25905103361409115</c:v>
+                  <c:v>-0.968101443057651</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.22360679774997907</c:v>
+                  <c:v>-0.82769874290523227</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-0.19153691689213431</c:v>
+                  <c:v>-0.71536206370457789</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-0.16162440712835383</c:v>
+                  <c:v>-0.62391201418098852</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-0.13266499161421605</c:v>
+                  <c:v>-0.54833885676102501</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-0.10307764064044152</c:v>
+                  <c:v>-0.48505736422050805</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-6.9600938624701389E-2</c:v>
+                  <c:v>-0.43144475917474873</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>-0.38554494183855909</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4374,7 +4374,7 @@
         <c:axId val="1290916927"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="0.28000000000000003"/>
+          <c:max val="0.5"/>
           <c:min val="0.1"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -4424,6 +4424,7 @@
         <c:axId val="1290897999"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="-7"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -6575,8 +6576,8 @@
       <xdr:rowOff>244474</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1451615" cy="443455"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="ZoneTexte 2">
@@ -6618,6 +6619,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -6809,7 +6811,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="ZoneTexte 2">
@@ -7283,11 +7285,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B673C9AC-1A9D-EA45-B245-5C46BCC162EE}">
   <dimension ref="A1:AE67"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" zoomScale="62" zoomScaleNormal="64" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="64" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.1640625" style="1" customWidth="1"/>
@@ -7315,28 +7317,28 @@
     <col min="30" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:31" ht="20">
+    <row r="1" spans="2:31" ht="20" x14ac:dyDescent="0.2">
       <c r="B1" s="13" t="s">
         <v>50</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
     </row>
-    <row r="2" spans="2:31">
+    <row r="2" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B2" s="14" t="s">
         <v>27</v>
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
     </row>
-    <row r="3" spans="2:31">
+    <row r="3" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B3" s="19" t="s">
         <v>44</v>
       </c>
       <c r="C3" s="14"/>
       <c r="D3" s="14"/>
     </row>
-    <row r="5" spans="2:31" ht="34">
+    <row r="5" spans="2:31" ht="34" x14ac:dyDescent="0.2">
       <c r="B5" s="38" t="s">
         <v>28</v>
       </c>
@@ -7367,7 +7369,7 @@
       <c r="AD5" s="152"/>
       <c r="AE5" s="152"/>
     </row>
-    <row r="6" spans="2:31" ht="18" customHeight="1" thickBot="1">
+    <row r="6" spans="2:31" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="62" t="s">
         <v>14</v>
       </c>
@@ -7452,7 +7454,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="7" spans="2:31" ht="18" customHeight="1">
+    <row r="7" spans="2:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="25" t="s">
         <v>67</v>
       </c>
@@ -7538,7 +7540,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="8" spans="2:31" ht="18" customHeight="1">
+    <row r="8" spans="2:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="29" t="s">
         <v>68</v>
       </c>
@@ -7577,7 +7579,7 @@
       </c>
       <c r="O8" s="147">
         <f>1-(1/n)</f>
-        <v>0.5</v>
+        <v>0.35483870967741937</v>
       </c>
       <c r="Q8" s="114">
         <v>0.01</v>
@@ -7631,11 +7633,11 @@
         <v>0</v>
       </c>
       <c r="AE8" s="157" t="e">
-        <f>(-1 * ((((1 / AD8)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
+        <f t="shared" ref="AE8:AE35" si="12">(-1 * ((((1 / AD8)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="2:31" ht="18" customHeight="1">
+    <row r="9" spans="2:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="29" t="s">
         <v>69</v>
       </c>
@@ -7726,11 +7728,11 @@
         <v>0</v>
       </c>
       <c r="AE9" s="160" t="e">
-        <f>(-1 * ((((1 / AD9)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
+        <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="2:31" ht="18" customHeight="1">
+    <row r="10" spans="2:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="29" t="s">
         <v>60</v>
       </c>
@@ -7747,7 +7749,7 @@
         <v>32</v>
       </c>
       <c r="G10" s="138">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="I10" s="73" t="s">
         <v>80</v>
@@ -7821,11 +7823,11 @@
         <v>0</v>
       </c>
       <c r="AE10" s="160" t="e">
-        <f>(-1 * ((((1 / AD10)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
+        <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="11" spans="2:31" ht="18" customHeight="1">
+    <row r="11" spans="2:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="29" t="s">
         <v>61</v>
       </c>
@@ -7842,7 +7844,7 @@
         <v>32</v>
       </c>
       <c r="G11" s="138">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="I11" s="73" t="s">
         <v>81</v>
@@ -7916,11 +7918,11 @@
         <v>0</v>
       </c>
       <c r="AE11" s="160" t="e">
-        <f>(-1 * ((((1 / AD11)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
+        <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="2:31" ht="18" customHeight="1">
+    <row r="12" spans="2:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="33" t="s">
         <v>62</v>
       </c>
@@ -7937,7 +7939,7 @@
         <v>32</v>
       </c>
       <c r="G12" s="138">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="I12" s="73" t="s">
         <v>19</v>
@@ -8011,11 +8013,11 @@
         <v>0</v>
       </c>
       <c r="AE12" s="160" t="e">
-        <f>(-1 * ((((1 / AD12)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
+        <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="2:31" ht="18" customHeight="1">
+    <row r="13" spans="2:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="64"/>
       <c r="C13" s="64"/>
       <c r="D13" s="65"/>
@@ -8096,11 +8098,11 @@
         <v>0</v>
       </c>
       <c r="AE13" s="160" t="e">
-        <f>(-1 * ((((1 / AD13)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
+        <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="2:31" ht="18" customHeight="1">
+    <row r="14" spans="2:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="10" t="s">
         <v>31</v>
       </c>
@@ -8183,11 +8185,11 @@
         <v>0</v>
       </c>
       <c r="AE14" s="160" t="e">
-        <f>(-1 * ((((1 / AD14)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
+        <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="2:31" ht="18" customHeight="1">
+    <row r="15" spans="2:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="40" t="s">
         <v>14</v>
       </c>
@@ -8280,11 +8282,11 @@
         <v>0</v>
       </c>
       <c r="AE15" s="160" t="e">
-        <f>(-1 * ((((1 / AD15)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
+        <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="2:31" ht="18" customHeight="1">
+    <row r="16" spans="2:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="42" t="s">
         <v>38</v>
       </c>
@@ -8299,7 +8301,7 @@
       </c>
       <c r="F16" s="45"/>
       <c r="G16" s="139">
-        <v>5.0000000000000001E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="I16" s="73" t="s">
         <v>73</v>
@@ -8319,7 +8321,7 @@
       <c r="N16" s="8"/>
       <c r="O16" s="149">
         <f>La_1/(depth1*(1-(RFC_1/100)))</f>
-        <v>12444.876068816591</v>
+        <v>29867.70256515982</v>
       </c>
       <c r="Q16" s="118">
         <v>0.09</v>
@@ -8373,11 +8375,11 @@
         <v>0</v>
       </c>
       <c r="AE16" s="160" t="e">
-        <f>(-1 * ((((1 / AD16)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
+        <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:31" ht="18" customHeight="1">
+    <row r="17" spans="1:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="46" t="s">
         <v>37</v>
       </c>
@@ -8392,7 +8394,7 @@
       </c>
       <c r="F17" s="49"/>
       <c r="G17" s="139">
-        <v>2</v>
+        <v>1.55</v>
       </c>
       <c r="I17" s="73" t="s">
         <v>74</v>
@@ -8414,26 +8416,26 @@
       </c>
       <c r="O17" s="149">
         <f>La_2/((depth2-depth1)*(1-(RFC_2/100)))</f>
-        <v>5427.5931421969171</v>
+        <v>10855.186284393834</v>
       </c>
       <c r="Q17" s="118">
         <v>0.1</v>
       </c>
       <c r="R17" s="117">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.2345679012345689E-2</v>
       </c>
       <c r="S17" s="129">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4.5925888793794001E-4</v>
       </c>
       <c r="T17" s="129">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>8.4783936930846957E-5</v>
       </c>
       <c r="U17" s="129">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1.8205099893128233E-5</v>
       </c>
       <c r="V17" s="129">
         <f t="shared" si="6"/>
@@ -8447,17 +8449,17 @@
         <f t="shared" si="8"/>
         <v>8.3207940750375742E-2</v>
       </c>
-      <c r="Y17" s="129" t="e">
+      <c r="Y17" s="129">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Z17" s="129" t="e">
+        <v>4.5910480274279379E-4</v>
+      </c>
+      <c r="Z17" s="129">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AA17" s="135" t="e">
+        <v>8.475985404246421E-5</v>
+      </c>
+      <c r="AA17" s="135">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
+        <v>1.8201117663040167E-5</v>
       </c>
       <c r="AC17" s="158">
         <f t="shared" si="0"/>
@@ -8465,14 +8467,14 @@
       </c>
       <c r="AD17" s="159">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AE17" s="160" t="e">
-        <f>(-1 * ((((1 / AD17)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
-        <v>#DIV/0!</v>
+        <v>1.2345679012345689E-2</v>
+      </c>
+      <c r="AE17" s="160">
+        <f t="shared" si="12"/>
+        <v>-295.10161713880905</v>
       </c>
     </row>
-    <row r="18" spans="1:31" ht="18" customHeight="1">
+    <row r="18" spans="1:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="46" t="s">
         <v>36</v>
       </c>
@@ -8509,26 +8511,26 @@
       </c>
       <c r="O18" s="149">
         <f>La_3/((depth3-depth2)*(1-(RFC_3/100)))</f>
-        <v>378.3701449977101</v>
+        <v>1513.4805799908388</v>
       </c>
       <c r="Q18" s="118">
         <v>0.11</v>
       </c>
       <c r="R18" s="117">
         <f t="shared" si="2"/>
-        <v>5.5555555555555525E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
       <c r="S18" s="129">
         <f t="shared" si="3"/>
-        <v>0.3151616380458741</v>
+        <v>1.3616134230305676E-3</v>
       </c>
       <c r="T18" s="129">
         <f t="shared" si="4"/>
-        <v>6.0903284244074471E-2</v>
+        <v>2.5136790950471092E-4</v>
       </c>
       <c r="U18" s="129">
         <f t="shared" si="5"/>
-        <v>1.243866491344923E-2</v>
+        <v>5.3974586084538481E-5</v>
       </c>
       <c r="V18" s="129">
         <f t="shared" si="6"/>
@@ -8544,15 +8546,15 @@
       </c>
       <c r="Y18" s="129">
         <f t="shared" si="9"/>
-        <v>0.25616308056217729</v>
+        <v>1.3602598950913313E-3</v>
       </c>
       <c r="Z18" s="129">
         <f t="shared" si="10"/>
-        <v>5.057987274967559E-2</v>
+        <v>2.511563372239747E-4</v>
       </c>
       <c r="AA18" s="135">
         <f t="shared" si="11"/>
-        <v>1.0821039449845448E-2</v>
+        <v>5.3939597027041723E-5</v>
       </c>
       <c r="AC18" s="158">
         <f t="shared" si="0"/>
@@ -8560,14 +8562,14 @@
       </c>
       <c r="AD18" s="159">
         <f t="shared" si="1"/>
-        <v>5.5555555555555525E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
       <c r="AE18" s="160">
-        <f>(-1 * ((((1 / AD18)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
-        <v>-3.5944401511222881</v>
+        <f t="shared" si="12"/>
+        <v>-40.03627388240605</v>
       </c>
     </row>
-    <row r="19" spans="1:31" ht="18" customHeight="1">
+    <row r="19" spans="1:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="46" t="s">
         <v>9</v>
       </c>
@@ -8582,7 +8584,7 @@
       </c>
       <c r="F19" s="49"/>
       <c r="G19" s="139">
-        <v>5</v>
+        <v>1.69</v>
       </c>
       <c r="I19" s="73" t="s">
         <v>76</v>
@@ -8596,26 +8598,26 @@
       <c r="N19" s="8"/>
       <c r="O19" s="149">
         <f>2*PI()*La_1/LN((1/SQRT(PI()*Lv_1))/root_radius)</f>
-        <v>7261.8849375360205</v>
+        <v>8400.1862183303838</v>
       </c>
       <c r="Q19" s="118">
         <v>0.12</v>
       </c>
       <c r="R19" s="117">
         <f t="shared" si="2"/>
-        <v>0.11111111111111105</v>
+        <v>6.1728395061728378E-2</v>
       </c>
       <c r="S19" s="129">
         <f t="shared" si="3"/>
-        <v>0.63198540354745669</v>
+        <v>2.8715960862765442E-3</v>
       </c>
       <c r="T19" s="129">
         <f t="shared" si="4"/>
-        <v>0.12212776564117986</v>
+        <v>5.3012631407720761E-4</v>
       </c>
       <c r="U19" s="129">
         <f t="shared" si="5"/>
-        <v>2.4942929963365553E-2</v>
+        <v>1.1383055391286166E-4</v>
       </c>
       <c r="V19" s="129">
         <f t="shared" si="6"/>
@@ -8631,15 +8633,15 @@
       </c>
       <c r="Y19" s="129">
         <f t="shared" si="9"/>
-        <v>0.43231966606274191</v>
+        <v>2.8655825797312406E-3</v>
       </c>
       <c r="Z19" s="129">
         <f t="shared" si="10"/>
-        <v>8.6659764735813702E-2</v>
+        <v>5.2918617383178876E-4</v>
       </c>
       <c r="AA19" s="135">
         <f t="shared" si="11"/>
-        <v>1.9190320196551064E-2</v>
+        <v>1.1367504359663485E-4</v>
       </c>
       <c r="AC19" s="158">
         <f t="shared" si="0"/>
@@ -8647,14 +8649,14 @@
       </c>
       <c r="AD19" s="159">
         <f t="shared" si="1"/>
-        <v>0.11111111111111105</v>
+        <v>6.1728395061728378E-2</v>
       </c>
       <c r="AE19" s="160">
-        <f>(-1 * ((((1 / AD19)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
-        <v>-1.7888543819998328</v>
+        <f t="shared" si="12"/>
+        <v>-15.812802138851525</v>
       </c>
     </row>
-    <row r="20" spans="1:31" ht="18" customHeight="1">
+    <row r="20" spans="1:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="46" t="s">
         <v>34</v>
       </c>
@@ -8671,7 +8673,7 @@
         <v>142</v>
       </c>
       <c r="G20" s="139">
-        <v>0.28000000000000003</v>
+        <v>0.5</v>
       </c>
       <c r="I20" s="73" t="s">
         <v>77</v>
@@ -8687,26 +8689,26 @@
       </c>
       <c r="O20" s="149">
         <f>2*PI()*La_2/LN((1/SQRT(PI()*Lv_2))/root_radius)</f>
-        <v>1403.3200399667398</v>
+        <v>1550.7611877476247</v>
       </c>
       <c r="Q20" s="118">
         <v>0.13</v>
       </c>
       <c r="R20" s="117">
         <f t="shared" si="2"/>
-        <v>0.16666666666666663</v>
+        <v>8.6419753086419762E-2</v>
       </c>
       <c r="S20" s="129">
         <f t="shared" si="3"/>
-        <v>1.0674570918195458</v>
+        <v>5.3370317102745014E-3</v>
       </c>
       <c r="T20" s="129">
         <f t="shared" si="4"/>
-        <v>0.20628031725097196</v>
+        <v>9.8527120934671923E-4</v>
       </c>
       <c r="U20" s="129">
         <f t="shared" si="5"/>
-        <v>4.2129940550365036E-2</v>
+        <v>2.1156083849480076E-4</v>
       </c>
       <c r="V20" s="129">
         <f t="shared" si="6"/>
@@ -8722,15 +8724,15 @@
       </c>
       <c r="Y20" s="129">
         <f t="shared" si="9"/>
-        <v>0.599666355615326</v>
+        <v>5.316296878539792E-3</v>
       </c>
       <c r="Z20" s="129">
         <f t="shared" si="10"/>
-        <v>0.12196599568983096</v>
+        <v>9.8202867373347116E-4</v>
       </c>
       <c r="AA20" s="135">
         <f t="shared" si="11"/>
-        <v>2.7968763798713641E-2</v>
+        <v>2.1102429742787839E-4</v>
       </c>
       <c r="AC20" s="158">
         <f t="shared" si="0"/>
@@ -8738,14 +8740,14 @@
       </c>
       <c r="AD20" s="159">
         <f t="shared" si="1"/>
-        <v>0.16666666666666663</v>
+        <v>8.6419753086419762E-2</v>
       </c>
       <c r="AE20" s="160">
-        <f>(-1 * ((((1 / AD20)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
-        <v>-1.1832159566199236</v>
+        <f t="shared" si="12"/>
+        <v>-8.573309019436488</v>
       </c>
     </row>
-    <row r="21" spans="1:31" ht="18" customHeight="1" thickBot="1">
+    <row r="21" spans="1:31" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B21" s="50" t="s">
         <v>35</v>
       </c>
@@ -8762,7 +8764,7 @@
         <v>141</v>
       </c>
       <c r="G21" s="140">
-        <v>0.1</v>
+        <v>9.5000000000000001E-2</v>
       </c>
       <c r="I21" s="73" t="s">
         <v>78</v>
@@ -8778,26 +8780,26 @@
       </c>
       <c r="O21" s="149">
         <f>2*PI()*La_3/LN((1/SQRT(PI()*Lv_3))/root_radius)</f>
-        <v>286.6089729007146</v>
+        <v>332.98480060389988</v>
       </c>
       <c r="Q21" s="118">
         <v>0.14000000000000001</v>
       </c>
       <c r="R21" s="117">
         <f t="shared" si="2"/>
-        <v>0.22222222222222224</v>
+        <v>0.11111111111111113</v>
       </c>
       <c r="S21" s="129">
         <f t="shared" si="3"/>
-        <v>1.6601715815122597</v>
+        <v>9.1935735207933876E-3</v>
       </c>
       <c r="T21" s="129">
         <f t="shared" si="4"/>
-        <v>0.32081919090691652</v>
+        <v>1.6972286830546463E-3</v>
       </c>
       <c r="U21" s="129">
         <f t="shared" si="5"/>
-        <v>6.5522942859740627E-2</v>
+        <v>3.6443480728777771E-4</v>
       </c>
       <c r="V21" s="129">
         <f t="shared" si="6"/>
@@ -8813,15 +8815,15 @@
       </c>
       <c r="Y21" s="129">
         <f t="shared" si="9"/>
-        <v>0.75011127189451954</v>
+        <v>9.1322182127808633E-3</v>
       </c>
       <c r="Z21" s="129">
         <f t="shared" si="10"/>
-        <v>0.15460120651536211</v>
+        <v>1.6876297639314931E-3</v>
       </c>
       <c r="AA21" s="135">
         <f t="shared" si="11"/>
-        <v>3.6657007710352352E-2</v>
+        <v>3.6284561315662317E-4</v>
       </c>
       <c r="AC21" s="158">
         <f t="shared" si="0"/>
@@ -8829,14 +8831,14 @@
       </c>
       <c r="AD21" s="159">
         <f t="shared" si="1"/>
-        <v>0.22222222222222224</v>
+        <v>0.11111111111111113</v>
       </c>
       <c r="AE21" s="160">
-        <f>(-1 * ((((1 / AD21)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
-        <v>-0.87749643873921235</v>
+        <f t="shared" si="12"/>
+        <v>-5.4251618951836793</v>
       </c>
     </row>
-    <row r="22" spans="1:31" ht="18" customHeight="1">
+    <row r="22" spans="1:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="39"/>
       <c r="C22" s="39"/>
       <c r="D22" s="39"/>
@@ -8866,19 +8868,19 @@
       </c>
       <c r="R22" s="117">
         <f t="shared" si="2"/>
-        <v>0.27777777777777768</v>
+        <v>0.13580246913580243</v>
       </c>
       <c r="S22" s="129">
         <f t="shared" si="3"/>
-        <v>2.4496312980403321</v>
+        <v>1.5003057720066113E-2</v>
       </c>
       <c r="T22" s="129">
         <f t="shared" si="4"/>
-        <v>0.47337801695273485</v>
+        <v>2.7697195044373989E-3</v>
       </c>
       <c r="U22" s="129">
         <f t="shared" si="5"/>
-        <v>9.6681001744845049E-2</v>
+        <v>5.9472374225032069E-4</v>
       </c>
       <c r="V22" s="129">
         <f t="shared" si="6"/>
@@ -8894,15 +8896,15 @@
       </c>
       <c r="Y22" s="129">
         <f t="shared" si="9"/>
-        <v>0.87795320772144447</v>
+        <v>1.4840347305453874E-2</v>
       </c>
       <c r="Z22" s="129">
         <f t="shared" si="10"/>
-        <v>0.18302578785393944</v>
+        <v>2.7442474570888195E-3</v>
       </c>
       <c r="AA22" s="135">
         <f t="shared" si="11"/>
-        <v>4.4719964180598634E-2</v>
+        <v>5.9050315652386866E-4</v>
       </c>
       <c r="AC22" s="158">
         <f t="shared" si="0"/>
@@ -8910,14 +8912,14 @@
       </c>
       <c r="AD22" s="159">
         <f t="shared" si="1"/>
-        <v>0.27777777777777768</v>
+        <v>0.13580246913580243</v>
       </c>
       <c r="AE22" s="160">
-        <f>(-1 * ((((1 / AD22)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
-        <v>-0.69166465863162352</v>
+        <f t="shared" si="12"/>
+        <v>-3.7628840854179857</v>
       </c>
     </row>
-    <row r="23" spans="1:31" ht="18" customHeight="1">
+    <row r="23" spans="1:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="11" t="s">
         <v>39</v>
       </c>
@@ -8949,19 +8951,19 @@
       </c>
       <c r="R23" s="117">
         <f t="shared" si="2"/>
-        <v>0.33333333333333326</v>
+        <v>0.16049382716049382</v>
       </c>
       <c r="S23" s="129">
         <f t="shared" si="3"/>
-        <v>3.4792992790446222</v>
+        <v>2.3480243747916522E-2</v>
       </c>
       <c r="T23" s="129">
         <f t="shared" si="4"/>
-        <v>0.67235579265206846</v>
+        <v>4.3346956527780455E-3</v>
       </c>
       <c r="U23" s="129">
         <f t="shared" si="5"/>
-        <v>0.13731949781065084</v>
+        <v>9.3076082830994232E-4</v>
       </c>
       <c r="V23" s="129">
         <f t="shared" si="6"/>
@@ -8977,15 +8979,15 @@
       </c>
       <c r="Y23" s="129">
         <f t="shared" si="9"/>
-        <v>0.98212304083342128</v>
+        <v>2.3084141026052558E-2</v>
       </c>
       <c r="Z23" s="129">
         <f t="shared" si="10"/>
-        <v>0.2066738248877879</v>
+        <v>4.2726289629593092E-3</v>
       </c>
       <c r="AA23" s="135">
         <f t="shared" si="11"/>
-        <v>5.1812476090307681E-2</v>
+        <v>9.2046454724948354E-4</v>
       </c>
       <c r="AC23" s="158">
         <f t="shared" si="0"/>
@@ -8993,14 +8995,14 @@
       </c>
       <c r="AD23" s="159">
         <f t="shared" si="1"/>
-        <v>0.33333333333333326</v>
+        <v>0.16049382716049382</v>
       </c>
       <c r="AE23" s="160">
-        <f>(-1 * ((((1 / AD23)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
-        <v>-0.56568542494923824</v>
+        <f t="shared" si="12"/>
+        <v>-2.7733271364219005</v>
       </c>
     </row>
-    <row r="24" spans="1:31" ht="18" customHeight="1" thickBot="1">
+    <row r="24" spans="1:31" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="56" t="s">
         <v>14</v>
       </c>
@@ -9042,19 +9044,19 @@
       </c>
       <c r="R24" s="117">
         <f t="shared" si="2"/>
-        <v>0.3888888888888889</v>
+        <v>0.1851851851851852</v>
       </c>
       <c r="S24" s="129">
         <f t="shared" si="3"/>
-        <v>4.797472666616958</v>
+        <v>3.5520236959888214E-2</v>
       </c>
       <c r="T24" s="129">
         <f t="shared" si="4"/>
-        <v>0.92708567984286638</v>
+        <v>6.5574028271889514E-3</v>
       </c>
       <c r="U24" s="129">
         <f t="shared" si="5"/>
-        <v>0.1893446020317805</v>
+        <v>1.4080281929562412E-3</v>
       </c>
       <c r="V24" s="129">
         <f t="shared" si="6"/>
@@ -9070,15 +9072,15 @@
       </c>
       <c r="Y24" s="129">
         <f t="shared" si="9"/>
-        <v>1.064700517580168</v>
+        <v>3.4621539051072632E-2</v>
       </c>
       <c r="Z24" s="129">
         <f t="shared" si="10"/>
-        <v>0.22573958281708073</v>
+        <v>6.4163999152732796E-3</v>
       </c>
       <c r="AA24" s="135">
         <f t="shared" si="11"/>
-        <v>5.7805274045292558E-2</v>
+        <v>1.3845982964849576E-3</v>
       </c>
       <c r="AC24" s="158">
         <f t="shared" si="0"/>
@@ -9086,14 +9088,14 @@
       </c>
       <c r="AD24" s="159">
         <f t="shared" si="1"/>
-        <v>0.3888888888888889</v>
+        <v>0.1851851851851852</v>
       </c>
       <c r="AE24" s="160">
-        <f>(-1 * ((((1 / AD24)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
-        <v>-0.47380354147934278</v>
+        <f t="shared" si="12"/>
+        <v>-2.1340109821626103</v>
       </c>
     </row>
-    <row r="25" spans="1:31" ht="18" customHeight="1">
+    <row r="25" spans="1:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="58" t="s">
         <v>59</v>
       </c>
@@ -9115,19 +9117,19 @@
       </c>
       <c r="R25" s="117">
         <f t="shared" si="2"/>
-        <v>0.44444444444444431</v>
+        <v>0.2098765432098765</v>
       </c>
       <c r="S25" s="129">
         <f t="shared" si="3"/>
-        <v>6.4577430798151498</v>
+        <v>5.2228000126832846E-2</v>
       </c>
       <c r="T25" s="129">
         <f t="shared" si="4"/>
-        <v>1.2479239694392614</v>
+        <v>9.6418285744227887E-3</v>
       </c>
       <c r="U25" s="129">
         <f t="shared" si="5"/>
-        <v>0.25487144553828683</v>
+        <v>2.0703267470694882E-3</v>
       </c>
       <c r="V25" s="129">
         <f t="shared" si="6"/>
@@ -9143,15 +9145,15 @@
       </c>
       <c r="Y25" s="129">
         <f t="shared" si="9"/>
-        <v>1.1291256461405335</v>
+        <v>5.0307869269171697E-2</v>
       </c>
       <c r="Z25" s="129">
         <f t="shared" si="10"/>
-        <v>0.24081500396044364</v>
+        <v>9.3400331729721342E-3</v>
       </c>
       <c r="AA25" s="135">
         <f t="shared" si="11"/>
-        <v>6.2728841211291478E-2</v>
+        <v>2.0200647874235593E-3</v>
       </c>
       <c r="AC25" s="158">
         <f t="shared" si="0"/>
@@ -9159,14 +9161,14 @@
       </c>
       <c r="AD25" s="159">
         <f t="shared" si="1"/>
-        <v>0.44444444444444431</v>
+        <v>0.2098765432098765</v>
       </c>
       <c r="AE25" s="160">
-        <f>(-1 * ((((1 / AD25)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
-        <v>-0.40311288741492773</v>
+        <f t="shared" si="12"/>
+        <v>-1.695629994580736</v>
       </c>
     </row>
-    <row r="26" spans="1:31" ht="18" customHeight="1">
+    <row r="26" spans="1:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="69" t="s">
         <v>51</v>
       </c>
@@ -9190,19 +9192,19 @@
       </c>
       <c r="R26" s="117">
         <f t="shared" si="2"/>
-        <v>0.49999999999999994</v>
+        <v>0.23456790123456789</v>
       </c>
       <c r="S26" s="129">
         <f t="shared" si="3"/>
-        <v>8.5193428946556011</v>
+        <v>7.4950331077162757E-2</v>
       </c>
       <c r="T26" s="129">
         <f t="shared" si="4"/>
-        <v>1.646316998169755</v>
+        <v>1.383660569210577E-2</v>
       </c>
       <c r="U26" s="129">
         <f t="shared" si="5"/>
-        <v>0.33623778644649327</v>
+        <v>2.971043784060995E-3</v>
       </c>
       <c r="V26" s="129">
         <f t="shared" si="6"/>
@@ -9218,15 +9220,15 @@
       </c>
       <c r="Y26" s="129">
         <f t="shared" si="9"/>
-        <v>1.1790115489589372</v>
+        <v>7.1058269614329539E-2</v>
       </c>
       <c r="Z26" s="129">
         <f t="shared" si="10"/>
-        <v>0.25261132263598535</v>
+        <v>1.3223438704391598E-2</v>
       </c>
       <c r="AA26" s="135">
         <f t="shared" si="11"/>
-        <v>6.6701487221363084E-2</v>
+        <v>2.8686162465993508E-3</v>
       </c>
       <c r="AC26" s="158">
         <f t="shared" si="0"/>
@@ -9234,14 +9236,14 @@
       </c>
       <c r="AD26" s="159">
         <f t="shared" si="1"/>
-        <v>0.49999999999999994</v>
+        <v>0.23456790123456789</v>
       </c>
       <c r="AE26" s="160">
-        <f>(-1 * ((((1 / AD26)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
-        <v>-0.34641016151377546</v>
+        <f t="shared" si="12"/>
+        <v>-1.3810808706842324</v>
       </c>
     </row>
-    <row r="27" spans="1:31">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B27" s="102" t="s">
         <v>56</v>
       </c>
@@ -9265,19 +9267,19 @@
       </c>
       <c r="R27" s="117">
         <f t="shared" si="2"/>
-        <v>0.55555555555555547</v>
+        <v>0.25925925925925924</v>
       </c>
       <c r="S27" s="129">
         <f t="shared" si="3"/>
-        <v>11.047455427394711</v>
+        <v>0.10531049791441752</v>
       </c>
       <c r="T27" s="129">
         <f t="shared" si="4"/>
-        <v>2.134861089820927</v>
+        <v>1.9441406247838581E-2</v>
       </c>
       <c r="U27" s="129">
         <f t="shared" si="5"/>
-        <v>0.43601625204025313</v>
+        <v>4.1745259257478205E-3</v>
       </c>
       <c r="V27" s="129">
         <f t="shared" si="6"/>
@@ -9293,15 +9295,15 @@
       </c>
       <c r="Y27" s="129">
         <f t="shared" si="9"/>
-        <v>1.2175718763409391</v>
+        <v>9.778499721024439E-2</v>
       </c>
       <c r="Z27" s="129">
         <f t="shared" si="10"/>
-        <v>0.26180417009858881</v>
+        <v>1.8252224407377643E-2</v>
       </c>
       <c r="AA27" s="135">
         <f t="shared" si="11"/>
-        <v>6.9873505452385146E-2</v>
+        <v>3.9750961388852991E-3</v>
       </c>
       <c r="AC27" s="158">
         <f t="shared" si="0"/>
@@ -9309,14 +9311,14 @@
       </c>
       <c r="AD27" s="159">
         <f t="shared" si="1"/>
-        <v>0.55555555555555547</v>
+        <v>0.25925925925925924</v>
       </c>
       <c r="AE27" s="160">
-        <f>(-1 * ((((1 / AD27)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
-        <v>-0.29933259094191533</v>
+        <f t="shared" si="12"/>
+        <v>-1.1471658159994846</v>
       </c>
     </row>
-    <row r="28" spans="1:31">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B28" s="102" t="s">
         <v>0</v>
       </c>
@@ -9340,19 +9342,19 @@
       </c>
       <c r="R28" s="117">
         <f t="shared" si="2"/>
-        <v>0.61111111111111094</v>
+        <v>0.2839506172839506</v>
       </c>
       <c r="S28" s="129">
         <f t="shared" si="3"/>
-        <v>14.113515381749325</v>
+        <v>0.14524568383104364</v>
       </c>
       <c r="T28" s="129">
         <f t="shared" si="4"/>
-        <v>2.7273606150399594</v>
+        <v>2.6813854278794076E-2</v>
       </c>
       <c r="U28" s="129">
         <f t="shared" si="5"/>
-        <v>0.55702619669351472</v>
+        <v>5.7575634410959604E-3</v>
       </c>
       <c r="V28" s="129">
         <f t="shared" si="6"/>
@@ -9368,15 +9370,15 @@
       </c>
       <c r="Y28" s="129">
         <f t="shared" si="9"/>
-        <v>1.2474392613862997</v>
+        <v>0.13130813576865469</v>
       </c>
       <c r="Z28" s="129">
         <f t="shared" si="10"/>
-        <v>0.26896982587731033</v>
+        <v>2.4603037429826512E-2</v>
       </c>
       <c r="AA28" s="135">
         <f t="shared" si="11"/>
-        <v>7.2393832287556054E-2</v>
+        <v>5.3849523141258904E-3</v>
       </c>
       <c r="AC28" s="158">
         <f t="shared" si="0"/>
@@ -9384,14 +9386,14 @@
       </c>
       <c r="AD28" s="159">
         <f t="shared" si="1"/>
-        <v>0.61111111111111094</v>
+        <v>0.2839506172839506</v>
       </c>
       <c r="AE28" s="160">
-        <f>(-1 * ((((1 / AD28)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
-        <v>-0.25905103361409115</v>
+        <f t="shared" si="12"/>
+        <v>-0.968101443057651</v>
       </c>
     </row>
-    <row r="29" spans="1:31">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
       <c r="B29" s="107" t="s">
         <v>82</v>
@@ -9420,19 +9422,19 @@
       </c>
       <c r="R29" s="117">
         <f t="shared" si="2"/>
-        <v>0.66666666666666652</v>
+        <v>0.30864197530864196</v>
       </c>
       <c r="S29" s="129">
         <f t="shared" si="3"/>
-        <v>17.795510444050191</v>
+        <v>0.19704739054208348</v>
       </c>
       <c r="T29" s="129">
         <f t="shared" si="4"/>
-        <v>3.4388862729690115</v>
+        <v>3.6376984683126112E-2</v>
       </c>
       <c r="U29" s="129">
         <f t="shared" si="5"/>
-        <v>0.70234560509901578</v>
+        <v>7.8109918451564767E-3</v>
       </c>
       <c r="V29" s="129">
         <f t="shared" si="6"/>
@@ -9448,15 +9450,15 @@
       </c>
       <c r="Y29" s="129">
         <f t="shared" si="9"/>
-        <v>1.2706769055200273</v>
+        <v>0.17224423734157626</v>
       </c>
       <c r="Z29" s="129">
         <f t="shared" si="10"/>
-        <v>0.2745724397439403</v>
+        <v>3.242421945137737E-2</v>
       </c>
       <c r="AA29" s="135">
         <f t="shared" si="11"/>
-        <v>7.4394332256721971E-2</v>
+        <v>7.1406742324876607E-3</v>
       </c>
       <c r="AC29" s="158">
         <f t="shared" si="0"/>
@@ -9464,14 +9466,14 @@
       </c>
       <c r="AD29" s="159">
         <f t="shared" si="1"/>
-        <v>0.66666666666666652</v>
+        <v>0.30864197530864196</v>
       </c>
       <c r="AE29" s="160">
-        <f>(-1 * ((((1 / AD29)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
-        <v>-0.22360679774997907</v>
+        <f t="shared" si="12"/>
+        <v>-0.82769874290523227</v>
       </c>
     </row>
-    <row r="30" spans="1:31" ht="17" thickBot="1">
+    <row r="30" spans="1:31" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -9505,19 +9507,19 @@
       </c>
       <c r="R30" s="117">
         <f t="shared" si="2"/>
-        <v>0.72222222222222221</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="S30" s="129">
         <f t="shared" si="3"/>
-        <v>22.178289437616584</v>
+        <v>0.26340495830866423</v>
       </c>
       <c r="T30" s="129">
         <f t="shared" si="4"/>
-        <v>4.2858346404136558</v>
+        <v>4.8627277466063906E-2</v>
       </c>
       <c r="U30" s="129">
         <f t="shared" si="5"/>
-        <v>0.87532325437351743</v>
+        <v>1.0441417040147742E-2</v>
       </c>
       <c r="V30" s="129">
         <f t="shared" si="6"/>
@@ -9533,15 +9535,15 @@
       </c>
       <c r="Y30" s="129">
         <f t="shared" si="9"/>
-        <v>1.2888635744675236</v>
+        <v>0.22088591565340021</v>
       </c>
       <c r="Z30" s="129">
         <f t="shared" si="10"/>
-        <v>0.27897418259339202</v>
+        <v>4.1813320236684465E-2</v>
       </c>
       <c r="AA30" s="135">
         <f t="shared" si="11"/>
-        <v>7.5984846250020804E-2</v>
+        <v>9.2772532660602303E-3</v>
       </c>
       <c r="AC30" s="158">
         <f t="shared" si="0"/>
@@ -9549,14 +9551,14 @@
       </c>
       <c r="AD30" s="159">
         <f t="shared" si="1"/>
-        <v>0.72222222222222221</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="AE30" s="160">
-        <f>(-1 * ((((1 / AD30)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
-        <v>-0.19153691689213431</v>
+        <f t="shared" si="12"/>
+        <v>-0.71536206370457789</v>
       </c>
     </row>
-    <row r="31" spans="1:31" ht="17" thickBot="1">
+    <row r="31" spans="1:31" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -9584,26 +9586,26 @@
       </c>
       <c r="O31" s="151">
         <f>1000*(sc_vg-rc_vg)*((depth1*(1-RFC_1/100)+(depth2-depth1)*(1-RFC_2/100))+((depth3-depth2)*(1-RFC_3/100)))</f>
-        <v>189</v>
+        <v>141.75000000000006</v>
       </c>
       <c r="Q31" s="118">
         <v>0.24</v>
       </c>
       <c r="R31" s="117">
         <f t="shared" si="2"/>
-        <v>0.77777777777777757</v>
+        <v>0.35802469135802462</v>
       </c>
       <c r="S31" s="129">
         <f t="shared" si="3"/>
-        <v>27.353880277730777</v>
+        <v>0.34745237470956025</v>
       </c>
       <c r="T31" s="129">
         <f t="shared" si="4"/>
-        <v>5.2859896149242953</v>
+        <v>6.4143299122888395E-2</v>
       </c>
       <c r="U31" s="129">
         <f t="shared" si="5"/>
-        <v>1.0795912629689259</v>
+        <v>1.3773070823066846E-2</v>
       </c>
       <c r="V31" s="129">
         <f t="shared" si="6"/>
@@ -9619,15 +9621,15 @@
       </c>
       <c r="Y31" s="129">
         <f t="shared" si="9"/>
-        <v>1.3031929951786028</v>
+        <v>0.27709424360789786</v>
       </c>
       <c r="Z31" s="129">
         <f t="shared" si="10"/>
-        <v>0.28245287149060611</v>
+        <v>5.279461056652044E-2</v>
       </c>
       <c r="AA31" s="135">
         <f t="shared" si="11"/>
-        <v>7.7253721499302555E-2</v>
+        <v>1.1817043794481364E-2</v>
       </c>
       <c r="AC31" s="158">
         <f t="shared" si="0"/>
@@ -9635,14 +9637,14 @@
       </c>
       <c r="AD31" s="159">
         <f t="shared" si="1"/>
-        <v>0.77777777777777757</v>
+        <v>0.35802469135802462</v>
       </c>
       <c r="AE31" s="160">
-        <f>(-1 * ((((1 / AD31)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
-        <v>-0.16162440712835383</v>
+        <f t="shared" si="12"/>
+        <v>-0.62391201418098852</v>
       </c>
     </row>
-    <row r="32" spans="1:31">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -9655,19 +9657,19 @@
       </c>
       <c r="R32" s="117">
         <f t="shared" si="2"/>
-        <v>0.83333333333333326</v>
+        <v>0.38271604938271603</v>
       </c>
       <c r="S32" s="129">
         <f t="shared" si="3"/>
-        <v>33.421820043549261</v>
+        <v>0.45281856168104484</v>
       </c>
       <c r="T32" s="129">
         <f t="shared" si="4"/>
-        <v>6.4585861994101714</v>
+        <v>8.3594986146180897E-2</v>
       </c>
       <c r="U32" s="129">
         <f t="shared" si="5"/>
-        <v>1.3190781178094997</v>
+        <v>1.7949804272443467E-2</v>
       </c>
       <c r="V32" s="129">
         <f t="shared" si="6"/>
@@ -9683,15 +9685,15 @@
       </c>
       <c r="Y32" s="129">
         <f t="shared" si="9"/>
-        <v>1.3145635734887848</v>
+        <v>0.34023115666120018</v>
       </c>
       <c r="Z32" s="129">
         <f t="shared" si="10"/>
-        <v>0.28521988097386514</v>
+        <v>6.5301114844674199E-2</v>
       </c>
       <c r="AA32" s="135">
         <f t="shared" si="11"/>
-        <v>7.8270601923069408E-2</v>
+        <v>1.4764724639180103E-2</v>
       </c>
       <c r="AC32" s="158">
         <f t="shared" si="0"/>
@@ -9699,14 +9701,14 @@
       </c>
       <c r="AD32" s="159">
         <f t="shared" si="1"/>
-        <v>0.83333333333333326</v>
+        <v>0.38271604938271603</v>
       </c>
       <c r="AE32" s="160">
-        <f>(-1 * ((((1 / AD32)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
-        <v>-0.13266499161421605</v>
+        <f t="shared" si="12"/>
+        <v>-0.54833885676102501</v>
       </c>
     </row>
-    <row r="33" spans="1:31">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
       <c r="B33" s="9"/>
       <c r="C33" s="3"/>
@@ -9727,19 +9729,19 @@
       </c>
       <c r="R33" s="117">
         <f t="shared" si="2"/>
-        <v>0.88888888888888884</v>
+        <v>0.40740740740740738</v>
       </c>
       <c r="S33" s="129">
         <f t="shared" si="3"/>
-        <v>40.489499080792143</v>
+        <v>0.58368135024671663</v>
       </c>
       <c r="T33" s="129">
         <f t="shared" si="4"/>
-        <v>7.8243769981254498</v>
+        <v>0.10775360931875183</v>
       </c>
       <c r="U33" s="129">
         <f t="shared" si="5"/>
-        <v>1.5980222551898156</v>
+        <v>2.313722731574732E-2</v>
       </c>
       <c r="V33" s="129">
         <f t="shared" si="6"/>
@@ -9755,15 +9757,15 @@
       </c>
       <c r="Y33" s="129">
         <f t="shared" si="9"/>
-        <v>1.3236513896316358</v>
+        <v>0.409156639513995</v>
       </c>
       <c r="Z33" s="129">
         <f t="shared" si="10"/>
-        <v>0.2874356134612927</v>
+        <v>7.9166121704973627E-2</v>
       </c>
       <c r="AA33" s="135">
         <f t="shared" si="11"/>
-        <v>7.9089788803880276E-2</v>
+        <v>1.8103324059064261E-2</v>
       </c>
       <c r="AC33" s="158">
         <f t="shared" si="0"/>
@@ -9771,14 +9773,14 @@
       </c>
       <c r="AD33" s="159">
         <f t="shared" si="1"/>
-        <v>0.88888888888888884</v>
+        <v>0.40740740740740738</v>
       </c>
       <c r="AE33" s="160">
-        <f>(-1 * ((((1 / AD33)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
-        <v>-0.10307764064044152</v>
+        <f t="shared" si="12"/>
+        <v>-0.48505736422050805</v>
       </c>
     </row>
-    <row r="34" spans="1:31">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
@@ -9791,19 +9793,19 @@
       </c>
       <c r="R34" s="117">
         <f t="shared" si="2"/>
-        <v>0.94444444444444442</v>
+        <v>0.4320987654320988</v>
       </c>
       <c r="S34" s="129">
         <f t="shared" si="3"/>
-        <v>48.672520887942895</v>
+        <v>0.74482537467739096</v>
       </c>
       <c r="T34" s="129">
         <f t="shared" si="4"/>
-        <v>9.4057017627334449</v>
+        <v>0.13750246157386459</v>
       </c>
       <c r="U34" s="129">
         <f t="shared" si="5"/>
-        <v>1.9209862646095797</v>
+        <v>2.9525003663665384E-2</v>
       </c>
       <c r="V34" s="129">
         <f t="shared" si="6"/>
@@ -9819,15 +9821,15 @@
       </c>
       <c r="Y34" s="129">
         <f t="shared" si="9"/>
-        <v>1.3309666240786677</v>
+        <v>0.48230315270739788</v>
       </c>
       <c r="Z34" s="129">
         <f t="shared" si="10"/>
-        <v>0.2892219030070502</v>
+        <v>9.4127999941968729E-2</v>
       </c>
       <c r="AA34" s="135">
         <f t="shared" si="11"/>
-        <v>7.9753404565508085E-2</v>
+        <v>2.1792340901502321E-2</v>
       </c>
       <c r="AC34" s="158">
         <f t="shared" si="0"/>
@@ -9835,14 +9837,14 @@
       </c>
       <c r="AD34" s="159">
         <f t="shared" si="1"/>
-        <v>0.94444444444444442</v>
+        <v>0.4320987654320988</v>
       </c>
       <c r="AE34" s="160">
-        <f>(-1 * ((((1 / AD34)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
-        <v>-6.9600938624701389E-2</v>
+        <f t="shared" si="12"/>
+        <v>-0.43144475917474873</v>
       </c>
     </row>
-    <row r="35" spans="1:31">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
       <c r="B35" s="9"/>
       <c r="C35" s="9"/>
@@ -9855,19 +9857,19 @@
       </c>
       <c r="R35" s="117">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.45679012345679015</v>
       </c>
       <c r="S35" s="129">
         <f t="shared" si="3"/>
-        <v>58.095079500288271</v>
+        <v>0.94170414265257341</v>
       </c>
       <c r="T35" s="129">
         <f t="shared" si="4"/>
-        <v>11.22656031973394</v>
+        <v>0.17384831678850846</v>
       </c>
       <c r="U35" s="129">
         <f t="shared" si="5"/>
-        <v>2.292871783205721</v>
+        <v>3.7329311281787181E-2</v>
       </c>
       <c r="V35" s="129">
         <f t="shared" si="6"/>
@@ -9883,15 +9885,15 @@
       </c>
       <c r="Y35" s="129">
         <f t="shared" si="9"/>
-        <v>1.3368960200306046</v>
+        <v>0.55782005427798043</v>
       </c>
       <c r="Z35" s="129">
         <f t="shared" si="10"/>
-        <v>0.29067158267529458</v>
+        <v>0.10984936746062583</v>
       </c>
       <c r="AA35" s="135">
         <f t="shared" si="11"/>
-        <v>8.0294081701744777E-2</v>
+        <v>2.5768756704014472E-2</v>
       </c>
       <c r="AC35" s="158">
         <f t="shared" si="0"/>
@@ -9899,14 +9901,14 @@
       </c>
       <c r="AD35" s="159">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.45679012345679015</v>
       </c>
       <c r="AE35" s="160">
-        <f>(-1 * ((((1 / AD35)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>-0.38554494183855909</v>
       </c>
     </row>
-    <row r="36" spans="1:31">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
@@ -9919,19 +9921,19 @@
       </c>
       <c r="R36" s="117">
         <f t="shared" si="2"/>
-        <v>1.0555555555555554</v>
+        <v>0.4814814814814814</v>
       </c>
       <c r="S36" s="129">
         <f t="shared" si="3"/>
-        <v>68.890356117025519</v>
+        <v>1.1805065655457774</v>
       </c>
       <c r="T36" s="129">
         <f t="shared" si="4"/>
-        <v>13.312689216509312</v>
+        <v>0.21793371196162661</v>
       </c>
       <c r="U36" s="129">
         <f t="shared" si="5"/>
-        <v>2.7189351496616445</v>
+        <v>4.679547966235275E-2</v>
       </c>
       <c r="V36" s="129">
         <f t="shared" si="6"/>
@@ -9947,15 +9949,15 @@
       </c>
       <c r="Y36" s="129">
         <f t="shared" si="9"/>
-        <v>1.3417344023301796</v>
+        <v>0.63376089545272862</v>
       </c>
       <c r="Z36" s="129">
         <f t="shared" si="10"/>
-        <v>0.29185571273234956</v>
+        <v>0.1259479864149449</v>
       </c>
       <c r="AA36" s="135">
         <f t="shared" si="11"/>
-        <v>8.0737131380358873E-2</v>
+        <v>2.9951177336478972E-2</v>
       </c>
       <c r="AC36" s="158">
         <f t="shared" si="0"/>
@@ -9963,14 +9965,14 @@
       </c>
       <c r="AD36" s="159">
         <f t="shared" si="1"/>
-        <v>1.0555555555555554</v>
-      </c>
-      <c r="AE36" s="160" t="e">
+        <v>0.4814814814814814</v>
+      </c>
+      <c r="AE36" s="160">
         <f>MAX(0,(-1*((((1/AD36)^(1/m))-1)^(1/n))/alpha/10000))</f>
-        <v>#NUM!</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:31">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="B37" s="9"/>
       <c r="C37" s="9"/>
@@ -9983,19 +9985,19 @@
       </c>
       <c r="R37" s="117">
         <f t="shared" si="2"/>
-        <v>1.1111111111111109</v>
+        <v>0.50617283950617276</v>
       </c>
       <c r="S37" s="129">
         <f t="shared" si="3"/>
-        <v>81.200936791782354</v>
+        <v>1.4682282635072366</v>
       </c>
       <c r="T37" s="129">
         <f t="shared" si="4"/>
-        <v>15.691642437761432</v>
+        <v>0.27105011086928787</v>
       </c>
       <c r="U37" s="129">
         <f t="shared" si="5"/>
-        <v>3.2048038894382649</v>
+        <v>5.8200816369775706E-2</v>
       </c>
       <c r="V37" s="129">
         <f t="shared" si="6"/>
@@ -10011,15 +10013,15 @@
       </c>
       <c r="Y37" s="129">
         <f t="shared" si="9"/>
-        <v>1.3457079317850806</v>
+        <v>0.70827490266880677</v>
       </c>
       <c r="Z37" s="129">
         <f t="shared" si="10"/>
-        <v>0.29282898413942537</v>
+        <v>0.14203357119272955</v>
       </c>
       <c r="AA37" s="135">
         <f t="shared" si="11"/>
-        <v>8.1102242303566677E-2</v>
+        <v>3.4246606636992194E-2</v>
       </c>
       <c r="AC37" s="158">
         <f t="shared" si="0"/>
@@ -10027,14 +10029,14 @@
       </c>
       <c r="AD37" s="159">
         <f t="shared" si="1"/>
-        <v>1.1111111111111109</v>
-      </c>
-      <c r="AE37" s="160" t="e">
-        <f>(-1 * ((((1 / AD37)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
-        <v>#NUM!</v>
+        <v>0.50617283950617276</v>
+      </c>
+      <c r="AE37" s="160">
+        <f t="shared" ref="AE37:AE67" si="13">(-1 * ((((1 / AD37)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
+        <v>-0.3112880463053686</v>
       </c>
     </row>
-    <row r="38" spans="1:31">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
@@ -10047,19 +10049,19 @@
       </c>
       <c r="R38" s="117">
         <f t="shared" si="2"/>
-        <v>1.1666666666666665</v>
+        <v>0.53086419753086411</v>
       </c>
       <c r="S38" s="129">
         <f t="shared" si="3"/>
-        <v>95.179253114226654</v>
+        <v>1.812747993913171</v>
       </c>
       <c r="T38" s="129">
         <f t="shared" si="4"/>
-        <v>18.392876564852411</v>
+        <v>0.33465201354627272</v>
       </c>
       <c r="U38" s="129">
         <f t="shared" si="5"/>
-        <v>3.7564941074075415</v>
+        <v>7.1857636677282052E-2</v>
       </c>
       <c r="V38" s="129">
         <f t="shared" si="6"/>
@@ -10075,15 +10077,15 @@
       </c>
       <c r="Y38" s="129">
         <f t="shared" si="9"/>
-        <v>1.3489912386390328</v>
+        <v>0.77976550527831168</v>
       </c>
       <c r="Z38" s="129">
         <f t="shared" si="10"/>
-        <v>0.29363374007015125</v>
+        <v>0.15774331273883432</v>
       </c>
       <c r="AA38" s="135">
         <f t="shared" si="11"/>
-        <v>8.1404790058712165E-2</v>
+        <v>3.8558692872341267E-2</v>
       </c>
       <c r="AC38" s="158">
         <f t="shared" si="0"/>
@@ -10091,14 +10093,14 @@
       </c>
       <c r="AD38" s="159">
         <f t="shared" si="1"/>
-        <v>1.1666666666666665</v>
-      </c>
-      <c r="AE38" s="160" t="e">
-        <f>(-1 * ((((1 / AD38)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
-        <v>#NUM!</v>
+        <v>0.53086419753086411</v>
+      </c>
+      <c r="AE38" s="160">
+        <f t="shared" si="13"/>
+        <v>-0.28089442929918113</v>
       </c>
     </row>
-    <row r="39" spans="1:31">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
@@ -10111,19 +10113,19 @@
       </c>
       <c r="R39" s="117">
         <f t="shared" si="2"/>
-        <v>1.2222222222222221</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="S39" s="129">
         <f t="shared" si="3"/>
-        <v>110.98804794451044</v>
+        <v>2.2229095893939594</v>
       </c>
       <c r="T39" s="129">
         <f t="shared" si="4"/>
-        <v>21.44784077647034</v>
+        <v>0.41037208289286298</v>
       </c>
       <c r="U39" s="129">
         <f t="shared" si="5"/>
-        <v>4.3804288692605882</v>
+        <v>8.8116511604187417E-2</v>
       </c>
       <c r="V39" s="129">
         <f t="shared" si="6"/>
@@ -10139,15 +10141,15 @@
       </c>
       <c r="Y39" s="129">
         <f t="shared" si="9"/>
-        <v>1.3517200665445663</v>
+        <v>0.84699176825559819</v>
       </c>
       <c r="Z39" s="129">
         <f t="shared" si="10"/>
-        <v>0.29430296712706111</v>
+        <v>0.17276984062906914</v>
       </c>
       <c r="AA39" s="135">
         <f t="shared" si="11"/>
-        <v>8.1656837535976662E-2</v>
+        <v>4.2795954552460234E-2</v>
       </c>
       <c r="AC39" s="158">
         <f t="shared" si="0"/>
@@ -10155,14 +10157,14 @@
       </c>
       <c r="AD39" s="159">
         <f t="shared" si="1"/>
-        <v>1.2222222222222221</v>
-      </c>
-      <c r="AE39" s="160" t="e">
-        <f>(-1 * ((((1 / AD39)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
-        <v>#NUM!</v>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="AE39" s="160">
+        <f t="shared" si="13"/>
+        <v>-0.25398636654803403</v>
       </c>
     </row>
-    <row r="40" spans="1:31">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
       <c r="B40" s="9"/>
       <c r="C40" s="9"/>
@@ -10174,44 +10176,44 @@
         <v>0.33</v>
       </c>
       <c r="R40" s="117">
-        <f t="shared" ref="R40:R66" si="12">MAX((Q40-rc_vg)/(sc_vg-rc_vg),0)</f>
-        <v>1.2777777777777777</v>
+        <f t="shared" ref="R40:R66" si="14">MAX((Q40-rc_vg)/(sc_vg-rc_vg),0)</f>
+        <v>0.58024691358024694</v>
       </c>
       <c r="S40" s="129">
-        <f t="shared" ref="S40:S67" si="13">Bgc_1*Ksat*R40^I*(1-(1-Q40^(1/m))^m)^2</f>
-        <v>128.80086842093311</v>
+        <f t="shared" ref="S40:S67" si="15">Bgc_1*Ksat*R40^I*(1-(1-Q40^(1/m))^m)^2</f>
+        <v>2.7086098335157511</v>
       </c>
       <c r="T40" s="129">
-        <f t="shared" ref="T40:T67" si="14">Bgc_2*Ksat*R40^I*(1-(1-Q40^(1/m))^m)^2</f>
-        <v>24.890072119697244</v>
+        <f t="shared" ref="T40:T67" si="16">Bgc_2*Ksat*R40^I*(1-(1-Q40^(1/m))^m)^2</f>
+        <v>0.5000373674338201</v>
       </c>
       <c r="U40" s="129">
-        <f t="shared" ref="U40:U67" si="15">Bgc_3*Ksat*R40^I*(1-(1-Q40^(1/m))^m)^2</f>
-        <v>5.083457659323539</v>
+        <f t="shared" ref="U40:U67" si="17">Bgc_3*Ksat*R40^I*(1-(1-Q40^(1/m))^m)^2</f>
+        <v>0.10736975132275949</v>
       </c>
       <c r="V40" s="129">
-        <f t="shared" ref="V40:V67" si="16">kroot1</f>
+        <f t="shared" ref="V40:V67" si="18">kroot1</f>
         <v>1.368385593142037</v>
       </c>
       <c r="W40" s="129">
-        <f t="shared" ref="W40:W67" si="17">kroot2</f>
+        <f t="shared" ref="W40:W67" si="19">kroot2</f>
         <v>0.29839751798850311</v>
       </c>
       <c r="X40" s="129">
-        <f t="shared" ref="X40:X67" si="18">kroot3</f>
+        <f t="shared" ref="X40:X67" si="20">kroot3</f>
         <v>8.3207940750375742E-2</v>
       </c>
       <c r="Y40" s="129">
-        <f t="shared" ref="Y40:Y67" si="19">1/((1/kroot1)+(1/S40))</f>
-        <v>1.3540006360667187</v>
+        <f t="shared" ref="Y40:Y67" si="21">1/((1/kroot1)+(1/S40))</f>
+        <v>0.90910640943844057</v>
       </c>
       <c r="Z40" s="129">
-        <f t="shared" ref="Z40:Z67" si="20">1/((1/kroot2)+(1/T40))</f>
-        <v>0.29486252439728944</v>
+        <f t="shared" ref="Z40:Z67" si="22">1/((1/kroot2)+(1/T40))</f>
+        <v>0.18687799351957696</v>
       </c>
       <c r="AA40" s="135">
-        <f t="shared" ref="AA40:AA67" si="21">1/((1/kroot3)+(1/U40))</f>
-        <v>8.1867896331046769E-2</v>
+        <f t="shared" ref="AA40:AA67" si="23">1/((1/kroot3)+(1/U40))</f>
+        <v>4.6878602680413779E-2</v>
       </c>
       <c r="AC40" s="158">
         <f t="shared" si="0"/>
@@ -10219,14 +10221,14 @@
       </c>
       <c r="AD40" s="159">
         <f t="shared" si="1"/>
-        <v>1.2777777777777777</v>
-      </c>
-      <c r="AE40" s="160" t="e">
-        <f>(-1 * ((((1 / AD40)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
-        <v>#NUM!</v>
+        <v>0.58024691358024694</v>
+      </c>
+      <c r="AE40" s="160">
+        <f t="shared" si="13"/>
+        <v>-0.22999826025010989</v>
       </c>
     </row>
-    <row r="41" spans="1:31">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
       <c r="B41" s="12"/>
       <c r="C41" s="9"/>
@@ -10238,44 +10240,44 @@
         <v>0.34</v>
       </c>
       <c r="R41" s="117">
-        <f t="shared" si="12"/>
-        <v>1.3333333333333333</v>
+        <f t="shared" si="14"/>
+        <v>0.60493827160493829</v>
       </c>
       <c r="S41" s="129">
-        <f t="shared" si="13"/>
-        <v>148.80258864436263</v>
+        <f t="shared" si="15"/>
+        <v>3.2808927488128257</v>
       </c>
       <c r="T41" s="129">
-        <f t="shared" si="14"/>
-        <v>28.75529651595027</v>
+        <f t="shared" si="16"/>
+        <v>0.60568670786358014</v>
       </c>
       <c r="U41" s="129">
-        <f t="shared" si="15"/>
-        <v>5.8728770096430303</v>
+        <f t="shared" si="17"/>
+        <v>0.13005514275174745</v>
       </c>
       <c r="V41" s="129">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.368385593142037</v>
       </c>
       <c r="W41" s="129">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.29839751798850311</v>
       </c>
       <c r="X41" s="129">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>8.3207940750375742E-2</v>
       </c>
       <c r="Y41" s="129">
-        <f t="shared" si="19"/>
-        <v>1.3559166114295176</v>
+        <f t="shared" si="21"/>
+        <v>0.96563940463757103</v>
       </c>
       <c r="Z41" s="129">
-        <f t="shared" si="20"/>
-        <v>0.29533281032559155</v>
+        <f t="shared" si="22"/>
+        <v>0.1999099255766574</v>
       </c>
       <c r="AA41" s="135">
-        <f t="shared" si="21"/>
-        <v>8.2045505784860237E-2</v>
+        <f t="shared" si="23"/>
+        <v>5.0743056110136957E-2</v>
       </c>
       <c r="AC41" s="158">
         <f t="shared" si="0"/>
@@ -10283,14 +10285,14 @@
       </c>
       <c r="AD41" s="159">
         <f t="shared" si="1"/>
-        <v>1.3333333333333333</v>
-      </c>
-      <c r="AE41" s="160" t="e">
-        <f>(-1 * ((((1 / AD41)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
-        <v>#NUM!</v>
+        <v>0.60493827160493829</v>
+      </c>
+      <c r="AE41" s="160">
+        <f t="shared" si="13"/>
+        <v>-0.20847238432764578</v>
       </c>
     </row>
-    <row r="42" spans="1:31">
+    <row r="42" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A42" s="99"/>
       <c r="B42" s="12"/>
       <c r="C42" s="12"/>
@@ -10302,44 +10304,44 @@
         <v>0.35</v>
       </c>
       <c r="R42" s="117">
-        <f t="shared" si="12"/>
-        <v>1.3888888888888886</v>
+        <f t="shared" si="14"/>
+        <v>0.62962962962962965</v>
       </c>
       <c r="S42" s="129">
-        <f t="shared" si="13"/>
-        <v>171.18996465163156</v>
+        <f t="shared" si="15"/>
+        <v>3.9520508238798979</v>
       </c>
       <c r="T42" s="129">
-        <f t="shared" si="14"/>
-        <v>33.081536006592884</v>
+        <f t="shared" si="16"/>
+        <v>0.72958942461362519</v>
       </c>
       <c r="U42" s="129">
-        <f t="shared" si="15"/>
-        <v>6.7564524034391438</v>
+        <f t="shared" si="17"/>
+        <v>0.15665996221541953</v>
       </c>
       <c r="V42" s="129">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.368385593142037</v>
       </c>
       <c r="W42" s="129">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.29839751798850311</v>
       </c>
       <c r="X42" s="129">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>8.3207940750375742E-2</v>
       </c>
       <c r="Y42" s="129">
-        <f t="shared" si="19"/>
-        <v>1.3575343122340857</v>
+        <f t="shared" si="21"/>
+        <v>1.0164447024421746</v>
       </c>
       <c r="Z42" s="129">
-        <f t="shared" si="20"/>
-        <v>0.29573001481099892</v>
+        <f t="shared" si="22"/>
+        <v>0.2117805824500899</v>
       </c>
       <c r="AA42" s="135">
-        <f t="shared" si="21"/>
-        <v>8.2195673904435093E-2</v>
+        <f t="shared" si="23"/>
+        <v>5.4343881331365744E-2</v>
       </c>
       <c r="AC42" s="158">
         <f t="shared" si="0"/>
@@ -10347,14 +10349,14 @@
       </c>
       <c r="AD42" s="159">
         <f t="shared" si="1"/>
-        <v>1.3888888888888886</v>
-      </c>
-      <c r="AE42" s="160" t="e">
-        <f>(-1 * ((((1 / AD42)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
-        <v>#NUM!</v>
+        <v>0.62962962962962965</v>
+      </c>
+      <c r="AE42" s="160">
+        <f t="shared" si="13"/>
+        <v>-0.18903439682681863</v>
       </c>
     </row>
-    <row r="43" spans="1:31">
+    <row r="43" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A43" s="99"/>
       <c r="B43" s="12"/>
       <c r="C43" s="12"/>
@@ -10366,44 +10368,44 @@
         <v>0.36</v>
       </c>
       <c r="R43" s="117">
-        <f t="shared" si="12"/>
-        <v>1.4444444444444444</v>
+        <f t="shared" si="14"/>
+        <v>0.65432098765432101</v>
       </c>
       <c r="S43" s="129">
-        <f t="shared" si="13"/>
-        <v>196.17222452644145</v>
+        <f t="shared" si="15"/>
+        <v>4.7357337643565272</v>
       </c>
       <c r="T43" s="129">
-        <f t="shared" si="14"/>
-        <v>37.909222788679656</v>
+        <f t="shared" si="16"/>
+        <v>0.87426539440809503</v>
       </c>
       <c r="U43" s="129">
-        <f t="shared" si="15"/>
-        <v>7.7424415653505205</v>
+        <f t="shared" si="17"/>
+        <v>0.18772528635095465</v>
       </c>
       <c r="V43" s="129">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.368385593142037</v>
       </c>
       <c r="W43" s="129">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.29839751798850311</v>
       </c>
       <c r="X43" s="129">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>8.3207940750375742E-2</v>
       </c>
       <c r="Y43" s="129">
-        <f t="shared" si="19"/>
-        <v>1.3589066352184731</v>
+        <f t="shared" si="21"/>
+        <v>1.0616289552302225</v>
       </c>
       <c r="Z43" s="129">
-        <f t="shared" si="20"/>
-        <v>0.29606706458609217</v>
+        <f t="shared" si="22"/>
+        <v>0.22246684959231097</v>
       </c>
       <c r="AA43" s="135">
-        <f t="shared" si="21"/>
-        <v>8.2323214006797416E-2</v>
+        <f t="shared" si="23"/>
+        <v>5.7653447202308299E-2</v>
       </c>
       <c r="AC43" s="158">
         <f t="shared" si="0"/>
@@ -10411,14 +10413,14 @@
       </c>
       <c r="AD43" s="159">
         <f t="shared" si="1"/>
-        <v>1.4444444444444444</v>
-      </c>
-      <c r="AE43" s="160" t="e">
-        <f>(-1 * ((((1 / AD43)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
-        <v>#NUM!</v>
+        <v>0.65432098765432101</v>
+      </c>
+      <c r="AE43" s="160">
+        <f t="shared" si="13"/>
+        <v>-0.17137497238380819</v>
       </c>
     </row>
-    <row r="44" spans="1:31">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A44" s="99"/>
       <c r="B44" s="12"/>
       <c r="C44" s="12"/>
@@ -10430,44 +10432,44 @@
         <v>0.37</v>
       </c>
       <c r="R44" s="117">
-        <f t="shared" si="12"/>
-        <v>1.5</v>
+        <f t="shared" si="14"/>
+        <v>0.67901234567901236</v>
       </c>
       <c r="S44" s="129">
-        <f t="shared" si="13"/>
-        <v>223.97169676289931</v>
+        <f t="shared" si="15"/>
+        <v>5.6470654177066297</v>
       </c>
       <c r="T44" s="129">
-        <f t="shared" si="14"/>
-        <v>43.281320642815736</v>
+        <f t="shared" si="16"/>
+        <v>1.0425066357864452</v>
       </c>
       <c r="U44" s="129">
-        <f t="shared" si="15"/>
-        <v>8.8396192614180311</v>
+        <f t="shared" si="17"/>
+        <v>0.22385062702645242</v>
       </c>
       <c r="V44" s="129">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.368385593142037</v>
       </c>
       <c r="W44" s="129">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.29839751798850311</v>
       </c>
       <c r="X44" s="129">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>8.3207940750375742E-2</v>
       </c>
       <c r="Y44" s="129">
-        <f t="shared" si="19"/>
-        <v>1.3600760233933222</v>
+        <f t="shared" si="21"/>
+        <v>1.1014777167099887</v>
       </c>
       <c r="Z44" s="129">
-        <f t="shared" si="20"/>
-        <v>0.29635434096718444</v>
+        <f t="shared" si="22"/>
+        <v>0.23199375714472595</v>
       </c>
       <c r="AA44" s="135">
-        <f t="shared" si="21"/>
-        <v>8.2432002670768473E-2</v>
+        <f t="shared" si="23"/>
+        <v>6.0659925060580294E-2</v>
       </c>
       <c r="AC44" s="158">
         <f t="shared" si="0"/>
@@ -10475,14 +10477,14 @@
       </c>
       <c r="AD44" s="159">
         <f t="shared" si="1"/>
-        <v>1.5</v>
-      </c>
-      <c r="AE44" s="160" t="e">
-        <f>(-1 * ((((1 / AD44)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
-        <v>#NUM!</v>
+        <v>0.67901234567901236</v>
+      </c>
+      <c r="AE44" s="160">
+        <f t="shared" si="13"/>
+        <v>-0.15523581232288602</v>
       </c>
     </row>
-    <row r="45" spans="1:31">
+    <row r="45" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A45" s="99"/>
       <c r="B45" s="12"/>
       <c r="C45" s="12"/>
@@ -10494,44 +10496,44 @@
         <v>0.38</v>
       </c>
       <c r="R45" s="117">
-        <f t="shared" si="12"/>
-        <v>1.5555555555555556</v>
+        <f t="shared" si="14"/>
+        <v>0.70370370370370372</v>
       </c>
       <c r="S45" s="129">
-        <f t="shared" si="13"/>
-        <v>254.82448029719598</v>
+        <f t="shared" si="15"/>
+        <v>6.7027695946832884</v>
       </c>
       <c r="T45" s="129">
-        <f t="shared" si="14"/>
-        <v>49.243454413159519</v>
+        <f t="shared" si="16"/>
+        <v>1.2374005370461543</v>
       </c>
       <c r="U45" s="129">
-        <f t="shared" si="15"/>
-        <v>10.057303743608848</v>
+        <f t="shared" si="17"/>
+        <v>0.26569891892505126</v>
       </c>
       <c r="V45" s="129">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.368385593142037</v>
       </c>
       <c r="W45" s="129">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.29839751798850311</v>
       </c>
       <c r="X45" s="129">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>8.3207940750375742E-2</v>
       </c>
       <c r="Y45" s="129">
-        <f t="shared" si="19"/>
-        <v>1.3610767279048599</v>
+        <f t="shared" si="21"/>
+        <v>1.1363891703321813</v>
       </c>
       <c r="Z45" s="129">
-        <f t="shared" si="20"/>
-        <v>0.29660022791413437</v>
+        <f t="shared" si="22"/>
+        <v>0.24042044317075323</v>
       </c>
       <c r="AA45" s="135">
-        <f t="shared" si="21"/>
-        <v>8.252517822128197E-2</v>
+        <f t="shared" si="23"/>
+        <v>6.3364360115822638E-2</v>
       </c>
       <c r="AC45" s="158">
         <f t="shared" si="0"/>
@@ -10539,14 +10541,14 @@
       </c>
       <c r="AD45" s="159">
         <f t="shared" si="1"/>
-        <v>1.5555555555555556</v>
-      </c>
-      <c r="AE45" s="160" t="e">
-        <f>(-1 * ((((1 / AD45)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
-        <v>#NUM!</v>
+        <v>0.70370370370370372</v>
+      </c>
+      <c r="AE45" s="160">
+        <f t="shared" si="13"/>
+        <v>-0.14039880681261674</v>
       </c>
     </row>
-    <row r="46" spans="1:31">
+    <row r="46" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A46" s="99"/>
       <c r="B46" s="12"/>
       <c r="C46" s="12"/>
@@ -10558,44 +10560,44 @@
         <v>0.39</v>
       </c>
       <c r="R46" s="117">
-        <f t="shared" si="12"/>
-        <v>1.6111111111111112</v>
+        <f t="shared" si="14"/>
+        <v>0.72839506172839508</v>
       </c>
       <c r="S46" s="129">
-        <f t="shared" si="13"/>
-        <v>288.98115996122215</v>
+        <f t="shared" si="15"/>
+        <v>7.9213055923924749</v>
       </c>
       <c r="T46" s="129">
-        <f t="shared" si="14"/>
-        <v>55.84404826496958</v>
+        <f t="shared" si="16"/>
+        <v>1.4623548752008533</v>
       </c>
       <c r="U46" s="129">
-        <f t="shared" si="15"/>
-        <v>11.405384987034182</v>
+        <f t="shared" si="17"/>
+        <v>0.31400189170206605</v>
       </c>
       <c r="V46" s="129">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.368385593142037</v>
       </c>
       <c r="W46" s="129">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.29839751798850311</v>
       </c>
       <c r="X46" s="129">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>8.3207940750375742E-2</v>
       </c>
       <c r="Y46" s="129">
-        <f t="shared" si="19"/>
-        <v>1.3619365417824301</v>
+        <f t="shared" si="21"/>
+        <v>1.166820321044034</v>
       </c>
       <c r="Z46" s="129">
-        <f t="shared" si="20"/>
-        <v>0.29681153295525531</v>
+        <f t="shared" si="22"/>
+        <v>0.24782761441426257</v>
       </c>
       <c r="AA46" s="135">
-        <f t="shared" si="21"/>
-        <v>8.2605294155841627E-2</v>
+        <f t="shared" si="23"/>
+        <v>6.5777452282427248E-2</v>
       </c>
       <c r="AC46" s="158">
         <f t="shared" si="0"/>
@@ -10603,14 +10605,14 @@
       </c>
       <c r="AD46" s="159">
         <f t="shared" si="1"/>
-        <v>1.6111111111111112</v>
-      </c>
-      <c r="AE46" s="160" t="e">
-        <f>(-1 * ((((1 / AD46)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
-        <v>#NUM!</v>
+        <v>0.72839506172839508</v>
+      </c>
+      <c r="AE46" s="160">
+        <f t="shared" si="13"/>
+        <v>-0.12667746234775107</v>
       </c>
     </row>
-    <row r="47" spans="1:31">
+    <row r="47" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A47" s="99"/>
       <c r="B47" s="3"/>
       <c r="C47" s="12"/>
@@ -10622,44 +10624,44 @@
         <v>0.4</v>
       </c>
       <c r="R47" s="117">
-        <f t="shared" si="12"/>
-        <v>1.6666666666666667</v>
+        <f t="shared" si="14"/>
+        <v>0.75308641975308654</v>
       </c>
       <c r="S47" s="129">
-        <f t="shared" si="13"/>
-        <v>326.70757149298095</v>
+        <f t="shared" si="15"/>
+        <v>9.3230143162290542</v>
       </c>
       <c r="T47" s="129">
-        <f t="shared" si="14"/>
-        <v>63.13447351873473</v>
+        <f t="shared" si="16"/>
+        <v>1.7211247915998102</v>
       </c>
       <c r="U47" s="129">
-        <f t="shared" si="15"/>
-        <v>12.894354883053472</v>
+        <f t="shared" si="17"/>
+        <v>0.36956586228321364</v>
       </c>
       <c r="V47" s="129">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.368385593142037</v>
       </c>
       <c r="W47" s="129">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.29839751798850311</v>
       </c>
       <c r="X47" s="129">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>8.3207940750375742E-2</v>
       </c>
       <c r="Y47" s="129">
-        <f t="shared" si="19"/>
-        <v>1.3626781370146528</v>
+        <f t="shared" si="21"/>
+        <v>1.1932467762058712</v>
       </c>
       <c r="Z47" s="129">
-        <f t="shared" si="20"/>
-        <v>0.29699381234998407</v>
+        <f t="shared" si="22"/>
+        <v>0.25430734957642431</v>
       </c>
       <c r="AA47" s="135">
-        <f t="shared" si="21"/>
-        <v>8.2674438312520568E-2</v>
+        <f t="shared" si="23"/>
+        <v>6.7916505253158135E-2</v>
       </c>
       <c r="AC47" s="158">
         <f t="shared" si="0"/>
@@ -10667,14 +10669,14 @@
       </c>
       <c r="AD47" s="159">
         <f t="shared" si="1"/>
-        <v>1.6666666666666667</v>
-      </c>
-      <c r="AE47" s="160" t="e">
-        <f>(-1 * ((((1 / AD47)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
-        <v>#NUM!</v>
+        <v>0.75308641975308654</v>
+      </c>
+      <c r="AE47" s="160">
+        <f t="shared" si="13"/>
+        <v>-0.1139099244926758</v>
       </c>
     </row>
-    <row r="48" spans="1:31">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
@@ -10685,44 +10687,44 @@
         <v>0.41</v>
       </c>
       <c r="R48" s="117">
-        <f t="shared" si="12"/>
-        <v>1.7222222222222217</v>
+        <f t="shared" si="14"/>
+        <v>0.77777777777777757</v>
       </c>
       <c r="S48" s="129">
-        <f t="shared" si="13"/>
-        <v>368.28562066833882</v>
+        <f t="shared" si="15"/>
+        <v>10.930276002175972</v>
       </c>
       <c r="T48" s="129">
-        <f t="shared" si="14"/>
-        <v>71.1692069429605</v>
+        <f t="shared" si="16"/>
+        <v>2.0178419090943427</v>
       </c>
       <c r="U48" s="129">
-        <f t="shared" si="15"/>
-        <v>14.535339568416456</v>
+        <f t="shared" si="17"/>
+        <v>0.43327798700319359</v>
       </c>
       <c r="V48" s="129">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.368385593142037</v>
       </c>
       <c r="W48" s="129">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.29839751798850311</v>
       </c>
       <c r="X48" s="129">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>8.3207940750375742E-2</v>
       </c>
       <c r="Y48" s="129">
-        <f t="shared" si="19"/>
-        <v>1.3633201018994123</v>
+        <f t="shared" si="21"/>
+        <v>1.2161349505004408</v>
       </c>
       <c r="Z48" s="129">
-        <f t="shared" si="20"/>
-        <v>0.29715162372055748</v>
+        <f t="shared" si="22"/>
+        <v>0.25995543048210035</v>
       </c>
       <c r="AA48" s="135">
-        <f t="shared" si="21"/>
-        <v>8.273432588545318E-2</v>
+        <f t="shared" si="23"/>
+        <v>6.980280997743922E-2</v>
       </c>
       <c r="AC48" s="158">
         <f t="shared" si="0"/>
@@ -10730,56 +10732,56 @@
       </c>
       <c r="AD48" s="159">
         <f t="shared" si="1"/>
-        <v>1.7222222222222217</v>
-      </c>
-      <c r="AE48" s="160" t="e">
-        <f>(-1 * ((((1 / AD48)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
-        <v>#NUM!</v>
+        <v>0.77777777777777757</v>
+      </c>
+      <c r="AE48" s="160">
+        <f t="shared" si="13"/>
+        <v>-0.10195304955261535</v>
       </c>
     </row>
-    <row r="49" spans="17:31">
+    <row r="49" spans="17:31" x14ac:dyDescent="0.2">
       <c r="Q49" s="118">
         <v>0.42</v>
       </c>
       <c r="R49" s="117">
-        <f t="shared" si="12"/>
-        <v>1.7777777777777772</v>
+        <f t="shared" si="14"/>
+        <v>0.80246913580246892</v>
       </c>
       <c r="S49" s="129">
-        <f t="shared" si="13"/>
-        <v>414.01416160356581</v>
+        <f t="shared" si="15"/>
+        <v>12.767680658793845</v>
       </c>
       <c r="T49" s="129">
-        <f t="shared" si="14"/>
-        <v>80.006000481390913</v>
+        <f t="shared" si="16"/>
+        <v>2.3570457973905348</v>
       </c>
       <c r="U49" s="129">
-        <f t="shared" si="15"/>
-        <v>16.340134089732661</v>
+        <f t="shared" si="17"/>
+        <v>0.50611301795494612</v>
       </c>
       <c r="V49" s="129">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.368385593142037</v>
       </c>
       <c r="W49" s="129">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.29839751798850311</v>
       </c>
       <c r="X49" s="129">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>8.3207940750375742E-2</v>
       </c>
       <c r="Y49" s="129">
-        <f t="shared" si="19"/>
-        <v>1.3638777505661861</v>
+        <f t="shared" si="21"/>
+        <v>1.2359244757316503</v>
       </c>
       <c r="Z49" s="129">
-        <f t="shared" si="20"/>
-        <v>0.29728872343976137</v>
+        <f t="shared" si="22"/>
+        <v>0.26486598740526063</v>
       </c>
       <c r="AA49" s="135">
-        <f t="shared" si="21"/>
-        <v>8.2786372388037113E-2</v>
+        <f t="shared" si="23"/>
+        <v>7.1459569507770701E-2</v>
       </c>
       <c r="AC49" s="158">
         <f t="shared" si="0"/>
@@ -10787,56 +10789,56 @@
       </c>
       <c r="AD49" s="159">
         <f t="shared" si="1"/>
-        <v>1.7777777777777772</v>
-      </c>
-      <c r="AE49" s="160" t="e">
-        <f>(-1 * ((((1 / AD49)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
-        <v>#NUM!</v>
+        <v>0.80246913580246892</v>
+      </c>
+      <c r="AE49" s="160">
+        <f t="shared" si="13"/>
+        <v>-9.0677015761655322E-2</v>
       </c>
     </row>
-    <row r="50" spans="17:31">
+    <row r="50" spans="17:31" x14ac:dyDescent="0.2">
       <c r="Q50" s="118">
         <v>0.43</v>
       </c>
       <c r="R50" s="117">
-        <f t="shared" si="12"/>
-        <v>1.8333333333333328</v>
+        <f t="shared" si="14"/>
+        <v>0.82716049382716039</v>
       </c>
       <c r="S50" s="129">
-        <f t="shared" si="13"/>
-        <v>464.20993982626999</v>
+        <f t="shared" si="15"/>
+        <v>14.862212481749824</v>
       </c>
       <c r="T50" s="129">
-        <f t="shared" si="14"/>
-        <v>89.706063496372735</v>
+        <f t="shared" si="16"/>
+        <v>2.7437180178770948</v>
       </c>
       <c r="U50" s="129">
-        <f t="shared" si="15"/>
-        <v>18.321239624192245</v>
+        <f t="shared" si="17"/>
+        <v>0.58914061321272659</v>
       </c>
       <c r="V50" s="129">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.368385593142037</v>
       </c>
       <c r="W50" s="129">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.29839751798850311</v>
       </c>
       <c r="X50" s="129">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>8.3207940750375742E-2</v>
       </c>
       <c r="Y50" s="129">
-        <f t="shared" si="19"/>
-        <v>1.3643637582986048</v>
+        <f t="shared" si="21"/>
+        <v>1.253018363735048</v>
       </c>
       <c r="Z50" s="129">
-        <f t="shared" si="20"/>
-        <v>0.29740822170542786</v>
+        <f t="shared" si="22"/>
+        <v>0.26912805807091206</v>
       </c>
       <c r="AA50" s="135">
-        <f t="shared" si="21"/>
-        <v>8.2831751170140466E-2</v>
+        <f t="shared" si="23"/>
+        <v>7.2910363157462535E-2</v>
       </c>
       <c r="AC50" s="158">
         <f t="shared" si="0"/>
@@ -10844,56 +10846,56 @@
       </c>
       <c r="AD50" s="159">
         <f t="shared" si="1"/>
-        <v>1.8333333333333328</v>
-      </c>
-      <c r="AE50" s="160" t="e">
-        <f>(-1 * ((((1 / AD50)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
-        <v>#NUM!</v>
+        <v>0.82716049382716039</v>
+      </c>
+      <c r="AE50" s="160">
+        <f t="shared" si="13"/>
+        <v>-7.9959889996252656E-2</v>
       </c>
     </row>
-    <row r="51" spans="17:31">
+    <row r="51" spans="17:31" x14ac:dyDescent="0.2">
       <c r="Q51" s="118">
         <v>0.44</v>
       </c>
       <c r="R51" s="117">
-        <f t="shared" si="12"/>
-        <v>1.8888888888888884</v>
+        <f t="shared" si="14"/>
+        <v>0.85185185185185175</v>
       </c>
       <c r="S51" s="129">
-        <f t="shared" si="13"/>
-        <v>519.20860633287589</v>
+        <f t="shared" si="15"/>
+        <v>17.243449645369402</v>
       </c>
       <c r="T51" s="129">
-        <f t="shared" si="14"/>
-        <v>100.33425872998592</v>
+        <f t="shared" si="16"/>
+        <v>3.1833190072105726</v>
       </c>
       <c r="U51" s="129">
-        <f t="shared" si="15"/>
-        <v>20.491903501953399</v>
+        <f t="shared" si="17"/>
+        <v>0.6835332566029656</v>
       </c>
       <c r="V51" s="129">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.368385593142037</v>
       </c>
       <c r="W51" s="129">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.29839751798850311</v>
       </c>
       <c r="X51" s="129">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>8.3207940750375742E-2</v>
       </c>
       <c r="Y51" s="129">
-        <f t="shared" si="19"/>
-        <v>1.3647886628885679</v>
+        <f t="shared" si="21"/>
+        <v>1.2677786885825035</v>
       </c>
       <c r="Z51" s="129">
-        <f t="shared" si="20"/>
-        <v>0.29751270502557897</v>
+        <f t="shared" si="22"/>
+        <v>0.27282361554777873</v>
       </c>
       <c r="AA51" s="135">
-        <f t="shared" si="21"/>
-        <v>8.2871438981080431E-2</v>
+        <f t="shared" si="23"/>
+        <v>7.4178086312115504E-2</v>
       </c>
       <c r="AC51" s="158">
         <f t="shared" si="0"/>
@@ -10901,56 +10903,56 @@
       </c>
       <c r="AD51" s="159">
         <f t="shared" si="1"/>
-        <v>1.8888888888888884</v>
-      </c>
-      <c r="AE51" s="160" t="e">
-        <f>(-1 * ((((1 / AD51)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
-        <v>#NUM!</v>
+        <v>0.85185185185185175</v>
+      </c>
+      <c r="AE51" s="160">
+        <f t="shared" si="13"/>
+        <v>-6.9681292615027479E-2</v>
       </c>
     </row>
-    <row r="52" spans="17:31">
+    <row r="52" spans="17:31" x14ac:dyDescent="0.2">
       <c r="Q52" s="118">
         <v>0.45</v>
       </c>
       <c r="R52" s="117">
-        <f t="shared" si="12"/>
-        <v>1.9444444444444442</v>
+        <f t="shared" si="14"/>
+        <v>0.87654320987654311</v>
       </c>
       <c r="S52" s="129">
-        <f t="shared" si="13"/>
-        <v>579.36580955449483</v>
+        <f t="shared" si="15"/>
+        <v>19.94378104827738</v>
       </c>
       <c r="T52" s="129">
-        <f t="shared" si="14"/>
-        <v>111.95931332054977</v>
+        <f t="shared" si="16"/>
+        <v>3.6818280908006389</v>
       </c>
       <c r="U52" s="129">
-        <f t="shared" si="15"/>
-        <v>22.866162303384904</v>
+        <f t="shared" si="17"/>
+        <v>0.79057484953808987</v>
       </c>
       <c r="V52" s="129">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.368385593142037</v>
       </c>
       <c r="W52" s="129">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.29839751798850311</v>
       </c>
       <c r="X52" s="129">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>8.3207940750375742E-2</v>
       </c>
       <c r="Y52" s="129">
-        <f t="shared" si="19"/>
-        <v>1.3651612623773528</v>
+        <f t="shared" si="21"/>
+        <v>1.2805259605188766</v>
       </c>
       <c r="Z52" s="129">
-        <f t="shared" si="20"/>
-        <v>0.29760433346624104</v>
+        <f t="shared" si="22"/>
+        <v>0.27602665575770935</v>
       </c>
       <c r="AA52" s="135">
-        <f t="shared" si="21"/>
-        <v>8.2906252236474701E-2</v>
+        <f t="shared" si="23"/>
+        <v>7.5284276561896665E-2</v>
       </c>
       <c r="AC52" s="158">
         <f t="shared" si="0"/>
@@ -10958,56 +10960,56 @@
       </c>
       <c r="AD52" s="159">
         <f t="shared" si="1"/>
-        <v>1.9444444444444442</v>
-      </c>
-      <c r="AE52" s="160" t="e">
-        <f>(-1 * ((((1 / AD52)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
-        <v>#NUM!</v>
+        <v>0.87654320987654311</v>
+      </c>
+      <c r="AE52" s="160">
+        <f t="shared" si="13"/>
+        <v>-5.9713577299716769E-2</v>
       </c>
     </row>
-    <row r="53" spans="17:31">
+    <row r="53" spans="17:31" x14ac:dyDescent="0.2">
       <c r="Q53" s="118">
         <v>0.46</v>
       </c>
       <c r="R53" s="117">
-        <f t="shared" si="12"/>
-        <v>1.9999999999999998</v>
+        <f t="shared" si="14"/>
+        <v>0.90123456790123446</v>
       </c>
       <c r="S53" s="129">
-        <f t="shared" si="13"/>
-        <v>645.0583729527134</v>
+        <f t="shared" si="15"/>
+        <v>22.998641787083621</v>
       </c>
       <c r="T53" s="129">
-        <f t="shared" si="14"/>
-        <v>124.65404636664859</v>
+        <f t="shared" si="16"/>
+        <v>4.2457869536859842</v>
       </c>
       <c r="U53" s="129">
-        <f t="shared" si="15"/>
-        <v>25.458888335913716</v>
+        <f t="shared" si="17"/>
+        <v>0.91167004523319917</v>
       </c>
       <c r="V53" s="129">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.368385593142037</v>
       </c>
       <c r="W53" s="129">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.29839751798850311</v>
       </c>
       <c r="X53" s="129">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>8.3207940750375742E-2</v>
       </c>
       <c r="Y53" s="129">
-        <f t="shared" si="19"/>
-        <v>1.3654889322183295</v>
+        <f t="shared" si="21"/>
+        <v>1.2915408019288817</v>
       </c>
       <c r="Z53" s="129">
-        <f t="shared" si="20"/>
-        <v>0.29768491825076682</v>
+        <f t="shared" si="22"/>
+        <v>0.27880300564052873</v>
       </c>
       <c r="AA53" s="135">
-        <f t="shared" si="21"/>
-        <v>8.2936876021430864E-2</v>
+        <f t="shared" si="23"/>
+        <v>7.6248734192927256E-2</v>
       </c>
       <c r="AC53" s="158">
         <f t="shared" si="0"/>
@@ -11015,56 +11017,56 @@
       </c>
       <c r="AD53" s="159">
         <f t="shared" si="1"/>
-        <v>1.9999999999999998</v>
-      </c>
-      <c r="AE53" s="160" t="e">
-        <f>(-1 * ((((1 / AD53)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
-        <v>#NUM!</v>
+        <v>0.90123456790123446</v>
+      </c>
+      <c r="AE53" s="160">
+        <f t="shared" si="13"/>
+        <v>-4.9906980966632077E-2</v>
       </c>
     </row>
-    <row r="54" spans="17:31">
+    <row r="54" spans="17:31" x14ac:dyDescent="0.2">
       <c r="Q54" s="118">
         <v>0.47</v>
       </c>
       <c r="R54" s="117">
-        <f t="shared" si="12"/>
-        <v>2.0555555555555554</v>
+        <f t="shared" si="14"/>
+        <v>0.92592592592592582</v>
       </c>
       <c r="S54" s="129">
-        <f t="shared" si="13"/>
-        <v>716.68556687722617</v>
+        <f t="shared" si="15"/>
+        <v>26.446769357223328</v>
       </c>
       <c r="T54" s="129">
-        <f t="shared" si="14"/>
-        <v>138.49561470674928</v>
+        <f t="shared" si="16"/>
+        <v>4.882346937857144</v>
       </c>
       <c r="U54" s="129">
-        <f t="shared" si="15"/>
-        <v>28.285839831158757</v>
+        <f t="shared" si="17"/>
+        <v>1.0483544045506517</v>
       </c>
       <c r="V54" s="129">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.368385593142037</v>
       </c>
       <c r="W54" s="129">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.29839751798850311</v>
       </c>
       <c r="X54" s="129">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>8.3207940750375742E-2</v>
       </c>
       <c r="Y54" s="129">
-        <f t="shared" si="19"/>
-        <v>1.3657778794388025</v>
+        <f t="shared" si="21"/>
+        <v>1.3010669269379471</v>
       </c>
       <c r="Z54" s="129">
-        <f t="shared" si="20"/>
-        <v>0.29775598398199621</v>
+        <f t="shared" si="22"/>
+        <v>0.28121059060758774</v>
       </c>
       <c r="AA54" s="135">
-        <f t="shared" si="21"/>
-        <v>8.2963887391250532E-2</v>
+        <f t="shared" si="23"/>
+        <v>7.708935485657227E-2</v>
       </c>
       <c r="AC54" s="158">
         <f t="shared" si="0"/>
@@ -11072,56 +11074,56 @@
       </c>
       <c r="AD54" s="159">
         <f t="shared" si="1"/>
-        <v>2.0555555555555554</v>
-      </c>
-      <c r="AE54" s="160" t="e">
-        <f>(-1 * ((((1 / AD54)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
-        <v>#NUM!</v>
+        <v>0.92592592592592582</v>
+      </c>
+      <c r="AE54" s="160">
+        <f t="shared" si="13"/>
+        <v>-4.0059166658069092E-2</v>
       </c>
     </row>
-    <row r="55" spans="17:31">
+    <row r="55" spans="17:31" x14ac:dyDescent="0.2">
       <c r="Q55" s="118">
         <v>0.48</v>
       </c>
       <c r="R55" s="117">
-        <f t="shared" si="12"/>
-        <v>2.1111111111111107</v>
+        <f t="shared" si="14"/>
+        <v>0.95061728395061729</v>
       </c>
       <c r="S55" s="129">
-        <f t="shared" si="13"/>
-        <v>794.6704843560924</v>
+        <f t="shared" si="15"/>
+        <v>30.330482838165832</v>
       </c>
       <c r="T55" s="129">
-        <f t="shared" si="14"/>
-        <v>153.56577878323736</v>
+        <f t="shared" si="16"/>
+        <v>5.5993205827312851</v>
       </c>
       <c r="U55" s="129">
-        <f t="shared" si="15"/>
-        <v>31.36371524403312</v>
+        <f t="shared" si="17"/>
+        <v>1.2023054629488972</v>
       </c>
       <c r="V55" s="129">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.368385593142037</v>
       </c>
       <c r="W55" s="129">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.29839751798850311</v>
       </c>
       <c r="X55" s="129">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>8.3207940750375742E-2</v>
       </c>
       <c r="Y55" s="129">
-        <f t="shared" si="19"/>
-        <v>1.3660333472879647</v>
+        <f t="shared" si="21"/>
+        <v>1.3093147422195068</v>
       </c>
       <c r="Z55" s="129">
-        <f t="shared" si="20"/>
-        <v>0.29781881876895649</v>
+        <f t="shared" si="22"/>
+        <v>0.28329997056065431</v>
       </c>
       <c r="AA55" s="135">
-        <f t="shared" si="21"/>
-        <v>8.2987774174357001E-2</v>
+        <f t="shared" si="23"/>
+        <v>7.782210705623116E-2</v>
       </c>
       <c r="AC55" s="158">
         <f t="shared" si="0"/>
@@ -11129,56 +11131,56 @@
       </c>
       <c r="AD55" s="159">
         <f t="shared" si="1"/>
-        <v>2.1111111111111107</v>
-      </c>
-      <c r="AE55" s="160" t="e">
-        <f>(-1 * ((((1 / AD55)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
-        <v>#NUM!</v>
+        <v>0.95061728395061729</v>
+      </c>
+      <c r="AE55" s="160">
+        <f t="shared" si="13"/>
+        <v>-2.9836323237022209E-2</v>
       </c>
     </row>
-    <row r="56" spans="17:31">
+    <row r="56" spans="17:31" x14ac:dyDescent="0.2">
       <c r="Q56" s="118">
         <v>0.49</v>
       </c>
       <c r="R56" s="117">
-        <f t="shared" si="12"/>
-        <v>2.1666666666666665</v>
+        <f t="shared" si="14"/>
+        <v>0.97530864197530864</v>
       </c>
       <c r="S56" s="129">
-        <f t="shared" si="13"/>
-        <v>879.46153167748651</v>
+        <f t="shared" si="15"/>
+        <v>34.695987616838806</v>
       </c>
       <c r="T56" s="129">
-        <f t="shared" si="14"/>
-        <v>169.95119068928912</v>
+        <f t="shared" si="16"/>
+        <v>6.4052378802454824</v>
       </c>
       <c r="U56" s="129">
-        <f t="shared" si="15"/>
-        <v>34.710212082387926</v>
+        <f t="shared" si="17"/>
+        <v>1.3753548097704866</v>
       </c>
       <c r="V56" s="129">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.368385593142037</v>
       </c>
       <c r="W56" s="129">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.29839751798850311</v>
       </c>
       <c r="X56" s="129">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>8.3207940750375742E-2</v>
       </c>
       <c r="Y56" s="129">
-        <f t="shared" si="19"/>
-        <v>1.366259780774854</v>
+        <f t="shared" si="21"/>
+        <v>1.3164651252438047</v>
       </c>
       <c r="Z56" s="129">
-        <f t="shared" si="20"/>
-        <v>0.29787451479255239</v>
+        <f t="shared" si="22"/>
+        <v>0.28511501178818738</v>
       </c>
       <c r="AA56" s="135">
-        <f t="shared" si="21"/>
-        <v>8.3008950211379759E-2</v>
+        <f t="shared" si="23"/>
+        <v>7.8461102534847768E-2</v>
       </c>
       <c r="AC56" s="158">
         <f t="shared" si="0"/>
@@ -11186,56 +11188,56 @@
       </c>
       <c r="AD56" s="159">
         <f t="shared" si="1"/>
-        <v>2.1666666666666665</v>
-      </c>
-      <c r="AE56" s="160" t="e">
-        <f>(-1 * ((((1 / AD56)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
-        <v>#NUM!</v>
+        <v>0.97530864197530864</v>
+      </c>
+      <c r="AE56" s="160">
+        <f t="shared" si="13"/>
+        <v>-1.8478166964546325E-2</v>
       </c>
     </row>
-    <row r="57" spans="17:31">
+    <row r="57" spans="17:31" x14ac:dyDescent="0.2">
       <c r="Q57" s="118">
         <v>0.5</v>
       </c>
       <c r="R57" s="117">
-        <f t="shared" si="12"/>
-        <v>2.2222222222222219</v>
+        <f t="shared" si="14"/>
+        <v>1</v>
       </c>
       <c r="S57" s="129">
-        <f t="shared" si="13"/>
-        <v>971.53404598375982</v>
+        <f t="shared" si="15"/>
+        <v>39.59370854492181</v>
       </c>
       <c r="T57" s="129">
-        <f t="shared" si="14"/>
-        <v>187.74370676018657</v>
+        <f t="shared" si="16"/>
+        <v>7.3094077791361309</v>
       </c>
       <c r="U57" s="129">
-        <f t="shared" si="15"/>
-        <v>38.344090749523787</v>
+        <f t="shared" si="17"/>
+        <v>1.569501294653463</v>
       </c>
       <c r="V57" s="129">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.368385593142037</v>
       </c>
       <c r="W57" s="129">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.29839751798850311</v>
       </c>
       <c r="X57" s="129">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>8.3207940750375742E-2</v>
       </c>
       <c r="Y57" s="129">
-        <f t="shared" si="19"/>
-        <v>1.3664609611637988</v>
+        <f t="shared" si="21"/>
+        <v>1.3226731077108129</v>
       </c>
       <c r="Z57" s="129">
-        <f t="shared" si="20"/>
-        <v>0.29792400127753299</v>
+        <f t="shared" si="22"/>
+        <v>0.28669360664164567</v>
       </c>
       <c r="AA57" s="135">
-        <f t="shared" si="21"/>
-        <v>8.3027767757740428E-2</v>
+        <f t="shared" si="23"/>
+        <v>7.9018721463883237E-2</v>
       </c>
       <c r="AC57" s="158">
         <f t="shared" si="0"/>
@@ -11243,56 +11245,56 @@
       </c>
       <c r="AD57" s="159">
         <f t="shared" si="1"/>
-        <v>2.2222222222222219</v>
-      </c>
-      <c r="AE57" s="160" t="e">
-        <f>(-1 * ((((1 / AD57)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
-        <v>#NUM!</v>
+        <v>1</v>
+      </c>
+      <c r="AE57" s="160">
+        <f t="shared" si="13"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="58" spans="17:31">
+    <row r="58" spans="17:31" x14ac:dyDescent="0.2">
       <c r="Q58" s="118">
         <v>0.51</v>
       </c>
       <c r="R58" s="117">
-        <f t="shared" si="12"/>
-        <v>2.2777777777777777</v>
+        <f t="shared" si="14"/>
+        <v>1.0246913580246915</v>
       </c>
       <c r="S58" s="129">
-        <f t="shared" si="13"/>
-        <v>1071.3920536639166</v>
+        <f t="shared" si="15"/>
+        <v>45.078654820580034</v>
       </c>
       <c r="T58" s="129">
-        <f t="shared" si="14"/>
-        <v>207.04072737316591</v>
+        <f t="shared" si="16"/>
+        <v>8.3219855458778635</v>
       </c>
       <c r="U58" s="129">
-        <f t="shared" si="15"/>
-        <v>42.285243943674004</v>
+        <f t="shared" si="17"/>
+        <v>1.7869254915049195</v>
       </c>
       <c r="V58" s="129">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.368385593142037</v>
       </c>
       <c r="W58" s="129">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.29839751798850311</v>
       </c>
       <c r="X58" s="129">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>8.3207940750375742E-2</v>
       </c>
       <c r="Y58" s="129">
-        <f t="shared" si="19"/>
-        <v>1.3666401157148349</v>
+        <f t="shared" si="21"/>
+        <v>1.3280713101470438</v>
       </c>
       <c r="Z58" s="129">
-        <f t="shared" si="20"/>
-        <v>0.29796807140533438</v>
+        <f t="shared" si="22"/>
+        <v>0.28806838550308861</v>
       </c>
       <c r="AA58" s="135">
-        <f t="shared" si="21"/>
-        <v>8.3044527618765351E-2</v>
+        <f t="shared" si="23"/>
+        <v>7.9505765662489875E-2</v>
       </c>
       <c r="AC58" s="158">
         <f t="shared" si="0"/>
@@ -11300,56 +11302,56 @@
       </c>
       <c r="AD58" s="159">
         <f t="shared" si="1"/>
-        <v>2.2777777777777777</v>
+        <v>1.0246913580246915</v>
       </c>
       <c r="AE58" s="160" t="e">
-        <f>(-1 * ((((1 / AD58)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
+        <f t="shared" si="13"/>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="59" spans="17:31">
+    <row r="59" spans="17:31" x14ac:dyDescent="0.2">
       <c r="Q59" s="118">
         <v>0.52</v>
       </c>
       <c r="R59" s="117">
-        <f t="shared" si="12"/>
-        <v>2.3333333333333335</v>
+        <f t="shared" si="14"/>
+        <v>1.0493827160493827</v>
       </c>
       <c r="S59" s="129">
-        <f t="shared" si="13"/>
-        <v>1179.570185134248</v>
+        <f t="shared" si="15"/>
+        <v>51.210820342780124</v>
       </c>
       <c r="T59" s="129">
-        <f t="shared" si="14"/>
-        <v>227.94556696843242</v>
+        <f t="shared" si="16"/>
+        <v>9.4540466742277243</v>
       </c>
       <c r="U59" s="129">
-        <f t="shared" si="15"/>
-        <v>46.554772229748735</v>
+        <f t="shared" si="17"/>
+        <v>2.0300055686137046</v>
       </c>
       <c r="V59" s="129">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.368385593142037</v>
       </c>
       <c r="W59" s="129">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.29839751798850311</v>
       </c>
       <c r="X59" s="129">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>8.3207940750375742E-2</v>
       </c>
       <c r="Y59" s="129">
-        <f t="shared" si="19"/>
-        <v>1.3668000075934463</v>
+        <f t="shared" si="21"/>
+        <v>1.3327730520587682</v>
       </c>
       <c r="Z59" s="129">
-        <f t="shared" si="20"/>
-        <v>0.29800740437063789</v>
+        <f t="shared" si="22"/>
+        <v>0.28926738845515332</v>
       </c>
       <c r="AA59" s="135">
-        <f t="shared" si="21"/>
-        <v>8.3059487464478568E-2</v>
+        <f t="shared" si="23"/>
+        <v>7.9931621829813129E-2</v>
       </c>
       <c r="AC59" s="158">
         <f t="shared" si="0"/>
@@ -11357,56 +11359,56 @@
       </c>
       <c r="AD59" s="159">
         <f t="shared" si="1"/>
-        <v>2.3333333333333335</v>
+        <v>1.0493827160493827</v>
       </c>
       <c r="AE59" s="160" t="e">
-        <f>(-1 * ((((1 / AD59)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
+        <f t="shared" si="13"/>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="60" spans="17:31">
+    <row r="60" spans="17:31" x14ac:dyDescent="0.2">
       <c r="Q60" s="118">
         <v>0.53</v>
       </c>
       <c r="R60" s="117">
-        <f t="shared" si="12"/>
-        <v>2.3888888888888888</v>
+        <f t="shared" si="14"/>
+        <v>1.0740740740740742</v>
       </c>
       <c r="S60" s="129">
-        <f t="shared" si="13"/>
-        <v>1296.6357636807979</v>
+        <f t="shared" si="15"/>
+        <v>58.055623818019448</v>
       </c>
       <c r="T60" s="129">
-        <f t="shared" si="14"/>
-        <v>250.56785770668458</v>
+        <f t="shared" si="16"/>
+        <v>10.71766813347568</v>
       </c>
       <c r="U60" s="129">
-        <f t="shared" si="15"/>
-        <v>51.175066480877277</v>
+        <f t="shared" si="17"/>
+        <v>2.3013347345555122</v>
       </c>
       <c r="V60" s="129">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.368385593142037</v>
       </c>
       <c r="W60" s="129">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.29839751798850311</v>
       </c>
       <c r="X60" s="129">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>8.3207940750375742E-2</v>
       </c>
       <c r="Y60" s="129">
-        <f t="shared" si="19"/>
-        <v>1.3669430098247448</v>
+        <f t="shared" si="21"/>
+        <v>1.3368751119396871</v>
       </c>
       <c r="Z60" s="129">
-        <f t="shared" si="20"/>
-        <v>0.29804258352885665</v>
+        <f t="shared" si="22"/>
+        <v>0.29031467956334678</v>
       </c>
       <c r="AA60" s="135">
-        <f t="shared" si="21"/>
-        <v>8.3072868676997549E-2</v>
+        <f t="shared" si="23"/>
+        <v>8.0304423243384646E-2</v>
       </c>
       <c r="AC60" s="158">
         <f t="shared" si="0"/>
@@ -11414,56 +11416,56 @@
       </c>
       <c r="AD60" s="159">
         <f t="shared" si="1"/>
-        <v>2.3888888888888888</v>
+        <v>1.0740740740740742</v>
       </c>
       <c r="AE60" s="160" t="e">
-        <f>(-1 * ((((1 / AD60)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
+        <f t="shared" si="13"/>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="61" spans="17:31">
+    <row r="61" spans="17:31" x14ac:dyDescent="0.2">
       <c r="Q61" s="118">
         <v>0.54</v>
       </c>
       <c r="R61" s="117">
-        <f t="shared" si="12"/>
-        <v>2.4444444444444446</v>
+        <f t="shared" si="14"/>
+        <v>1.0987654320987654</v>
       </c>
       <c r="S61" s="129">
-        <f t="shared" si="13"/>
-        <v>1423.1910884521617</v>
+        <f t="shared" si="15"/>
+        <v>65.684393518993474</v>
       </c>
       <c r="T61" s="129">
-        <f t="shared" si="14"/>
-        <v>275.02399064514083</v>
+        <f t="shared" si="16"/>
+        <v>12.126017859904362</v>
       </c>
       <c r="U61" s="129">
-        <f t="shared" si="15"/>
-        <v>56.169897982592602</v>
+        <f t="shared" si="17"/>
+        <v>2.6037404541083355</v>
       </c>
       <c r="V61" s="129">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.368385593142037</v>
       </c>
       <c r="W61" s="129">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.29839751798850311</v>
       </c>
       <c r="X61" s="129">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>8.3207940750375742E-2</v>
       </c>
       <c r="Y61" s="129">
-        <f t="shared" si="19"/>
-        <v>1.3670711663556274</v>
+        <f t="shared" si="21"/>
+        <v>1.3404601416348407</v>
       </c>
       <c r="Z61" s="129">
-        <f t="shared" si="20"/>
-        <v>0.29807411138384682</v>
+        <f t="shared" si="22"/>
+        <v>0.29123089678070507</v>
       </c>
       <c r="AA61" s="135">
-        <f t="shared" si="21"/>
-        <v>8.3084862010272875E-2</v>
+        <f t="shared" si="23"/>
+        <v>8.0631202984527403E-2</v>
       </c>
       <c r="AC61" s="158">
         <f t="shared" si="0"/>
@@ -11471,56 +11473,56 @@
       </c>
       <c r="AD61" s="159">
         <f t="shared" si="1"/>
-        <v>2.4444444444444446</v>
+        <v>1.0987654320987654</v>
       </c>
       <c r="AE61" s="160" t="e">
-        <f>(-1 * ((((1 / AD61)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
+        <f t="shared" si="13"/>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="62" spans="17:31">
+    <row r="62" spans="17:31" x14ac:dyDescent="0.2">
       <c r="Q62" s="118">
         <v>0.55000000000000004</v>
       </c>
       <c r="R62" s="117">
-        <f t="shared" si="12"/>
-        <v>2.5</v>
+        <f t="shared" si="14"/>
+        <v>1.1234567901234569</v>
       </c>
       <c r="S62" s="129">
-        <f t="shared" si="13"/>
-        <v>1559.8759344976083</v>
+        <f t="shared" si="15"/>
+        <v>74.174902319225055</v>
       </c>
       <c r="T62" s="129">
-        <f t="shared" si="14"/>
-        <v>301.43759885640316</v>
+        <f t="shared" si="16"/>
+        <v>13.693453529710952</v>
       </c>
       <c r="U62" s="129">
-        <f t="shared" si="15"/>
-        <v>61.56451710326818</v>
+        <f t="shared" si="17"/>
+        <v>2.9403056571155499</v>
       </c>
       <c r="V62" s="129">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.368385593142037</v>
       </c>
       <c r="W62" s="129">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.29839751798850311</v>
       </c>
       <c r="X62" s="129">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>8.3207940750375742E-2</v>
       </c>
       <c r="Y62" s="129">
-        <f t="shared" si="19"/>
-        <v>1.3671862426576684</v>
+        <f t="shared" si="21"/>
+        <v>1.3435987565710525</v>
       </c>
       <c r="Z62" s="129">
-        <f t="shared" si="20"/>
-        <v>0.29810242201118653</v>
+        <f t="shared" si="22"/>
+        <v>0.29203373678198868</v>
       </c>
       <c r="AA62" s="135">
-        <f t="shared" si="21"/>
-        <v>8.3095632284832618E-2</v>
+        <f t="shared" si="23"/>
+        <v>8.0918034923987248E-2</v>
       </c>
       <c r="AC62" s="158">
         <f t="shared" si="0"/>
@@ -11528,56 +11530,56 @@
       </c>
       <c r="AD62" s="159">
         <f t="shared" si="1"/>
-        <v>2.5</v>
+        <v>1.1234567901234569</v>
       </c>
       <c r="AE62" s="160" t="e">
-        <f>(-1 * ((((1 / AD62)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
+        <f t="shared" si="13"/>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="63" spans="17:31">
+    <row r="63" spans="17:31" x14ac:dyDescent="0.2">
       <c r="Q63" s="118">
         <v>0.56000000000000005</v>
       </c>
       <c r="R63" s="117">
-        <f t="shared" si="12"/>
-        <v>2.5555555555555558</v>
+        <f t="shared" si="14"/>
+        <v>1.1481481481481484</v>
       </c>
       <c r="S63" s="129">
-        <f t="shared" si="13"/>
-        <v>1707.3702960174396</v>
+        <f t="shared" si="15"/>
+        <v>83.611959477491524</v>
       </c>
       <c r="T63" s="129">
-        <f t="shared" si="14"/>
-        <v>329.94008754677179</v>
+        <f t="shared" si="16"/>
+        <v>15.435631808528241</v>
       </c>
       <c r="U63" s="129">
-        <f t="shared" si="15"/>
-        <v>67.385761563551384</v>
+        <f t="shared" si="17"/>
+        <v>3.3143921969205619</v>
       </c>
       <c r="V63" s="129">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.368385593142037</v>
       </c>
       <c r="W63" s="129">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.29839751798850311</v>
       </c>
       <c r="X63" s="129">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>8.3207940750375742E-2</v>
       </c>
       <c r="Y63" s="129">
-        <f t="shared" si="19"/>
-        <v>1.367289767810949</v>
+        <f t="shared" si="21"/>
+        <v>1.346351331808286</v>
       </c>
       <c r="Z63" s="129">
-        <f t="shared" si="20"/>
-        <v>0.29812789139206253</v>
+        <f t="shared" si="22"/>
+        <v>0.29273837773307998</v>
       </c>
       <c r="AA63" s="135">
-        <f t="shared" si="21"/>
-        <v>8.3105322295480316E-2</v>
+        <f t="shared" si="23"/>
+        <v>8.1170160810602091E-2</v>
       </c>
       <c r="AC63" s="158">
         <f t="shared" si="0"/>
@@ -11585,56 +11587,56 @@
       </c>
       <c r="AD63" s="159">
         <f t="shared" si="1"/>
-        <v>2.5555555555555558</v>
+        <v>1.1481481481481484</v>
       </c>
       <c r="AE63" s="160" t="e">
-        <f>(-1 * ((((1 / AD63)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
+        <f t="shared" si="13"/>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="64" spans="17:31">
+    <row r="64" spans="17:31" x14ac:dyDescent="0.2">
       <c r="Q64" s="118">
         <v>0.56999999999999995</v>
       </c>
       <c r="R64" s="117">
-        <f t="shared" si="12"/>
-        <v>2.6111111111111107</v>
+        <f t="shared" si="14"/>
+        <v>1.1728395061728394</v>
       </c>
       <c r="S64" s="129">
-        <f t="shared" si="13"/>
-        <v>1866.3974028194343</v>
+        <f t="shared" si="15"/>
+        <v>94.088066646031905</v>
       </c>
       <c r="T64" s="129">
-        <f t="shared" si="14"/>
-        <v>360.67121697015966</v>
+        <f t="shared" si="16"/>
+        <v>17.369629457319185</v>
       </c>
       <c r="U64" s="129">
-        <f t="shared" si="15"/>
-        <v>73.662175488577972</v>
+        <f t="shared" si="17"/>
+        <v>3.7296668546429541</v>
       </c>
       <c r="V64" s="129">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.368385593142037</v>
       </c>
       <c r="W64" s="129">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.29839751798850311</v>
       </c>
       <c r="X64" s="129">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>8.3207940750375742E-2</v>
       </c>
       <c r="Y64" s="129">
-        <f t="shared" si="19"/>
-        <v>1.3673830696226883</v>
+        <f t="shared" si="21"/>
+        <v>1.3487695369447354</v>
       </c>
       <c r="Z64" s="129">
-        <f t="shared" si="20"/>
-        <v>0.29815084603837799</v>
+        <f t="shared" si="22"/>
+        <v>0.29335784497543038</v>
       </c>
       <c r="AA64" s="135">
-        <f t="shared" si="21"/>
-        <v>8.3114056074726148E-2</v>
+        <f t="shared" si="23"/>
+        <v>8.1392103153955578E-2</v>
       </c>
       <c r="AC64" s="158">
         <f t="shared" si="0"/>
@@ -11642,56 +11644,56 @@
       </c>
       <c r="AD64" s="159">
         <f t="shared" si="1"/>
-        <v>2.6111111111111107</v>
+        <v>1.1728395061728394</v>
       </c>
       <c r="AE64" s="160" t="e">
-        <f>(-1 * ((((1 / AD64)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
+        <f t="shared" si="13"/>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="65" spans="17:31">
+    <row r="65" spans="17:31" x14ac:dyDescent="0.2">
       <c r="Q65" s="118">
         <v>0.57999999999999996</v>
       </c>
       <c r="R65" s="117">
-        <f t="shared" si="12"/>
-        <v>2.6666666666666661</v>
+        <f t="shared" si="14"/>
+        <v>1.1975308641975309</v>
       </c>
       <c r="S65" s="129">
-        <f t="shared" si="13"/>
-        <v>2037.7270444667847</v>
+        <f t="shared" si="15"/>
+        <v>105.70414675778086</v>
       </c>
       <c r="T65" s="129">
-        <f t="shared" si="14"/>
-        <v>393.77974480172645</v>
+        <f t="shared" si="16"/>
+        <v>19.51407789249302</v>
       </c>
       <c r="U65" s="129">
-        <f t="shared" si="15"/>
-        <v>80.424140604023052</v>
+        <f t="shared" si="17"/>
+        <v>4.1901302323915548</v>
       </c>
       <c r="V65" s="129">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.368385593142037</v>
       </c>
       <c r="W65" s="129">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.29839751798850311</v>
       </c>
       <c r="X65" s="129">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>8.3207940750375742E-2</v>
       </c>
       <c r="Y65" s="129">
-        <f t="shared" si="19"/>
-        <v>1.3674673040301519</v>
+        <f t="shared" si="21"/>
+        <v>1.3508976427741337</v>
       </c>
       <c r="Z65" s="129">
-        <f t="shared" si="20"/>
-        <v>0.29817157021525803</v>
+        <f t="shared" si="22"/>
+        <v>0.29390332547106568</v>
       </c>
       <c r="AA65" s="135">
-        <f t="shared" si="21"/>
-        <v>8.3121941626953272E-2</v>
+        <f t="shared" si="23"/>
+        <v>8.1587764409679644E-2</v>
       </c>
       <c r="AC65" s="158">
         <f t="shared" si="0"/>
@@ -11699,56 +11701,56 @@
       </c>
       <c r="AD65" s="159">
         <f t="shared" si="1"/>
-        <v>2.6666666666666661</v>
+        <v>1.1975308641975309</v>
       </c>
       <c r="AE65" s="160" t="e">
-        <f>(-1 * ((((1 / AD65)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
+        <f t="shared" si="13"/>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="66" spans="17:31">
+    <row r="66" spans="17:31" x14ac:dyDescent="0.2">
       <c r="Q66" s="118">
         <v>0.59</v>
       </c>
       <c r="R66" s="117">
-        <f t="shared" si="12"/>
-        <v>2.7222222222222219</v>
+        <f t="shared" si="14"/>
+        <v>1.2222222222222221</v>
       </c>
       <c r="S66" s="129">
-        <f t="shared" si="13"/>
-        <v>2222.179241892828</v>
+        <f t="shared" si="15"/>
+        <v>118.57035584815631</v>
       </c>
       <c r="T66" s="129">
-        <f t="shared" si="14"/>
-        <v>429.42413565759352</v>
+        <f t="shared" si="16"/>
+        <v>21.889313056596993</v>
       </c>
       <c r="U66" s="129">
-        <f t="shared" si="15"/>
-        <v>87.704021145822921</v>
+        <f t="shared" si="17"/>
+        <v>4.7001489340172293</v>
       </c>
       <c r="V66" s="129">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.368385593142037</v>
       </c>
       <c r="W66" s="129">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.29839751798850311</v>
       </c>
       <c r="X66" s="129">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>8.3207940750375742E-2</v>
       </c>
       <c r="Y66" s="129">
-        <f t="shared" si="19"/>
-        <v>1.3675434797965111</v>
+        <f t="shared" si="21"/>
+        <v>1.3527736306600466</v>
       </c>
       <c r="Z66" s="129">
-        <f t="shared" si="20"/>
-        <v>0.29819031200820761</v>
+        <f t="shared" si="22"/>
+        <v>0.29438443703351314</v>
       </c>
       <c r="AA66" s="135">
-        <f t="shared" si="21"/>
-        <v>8.3129073226295563E-2</v>
+        <f t="shared" si="23"/>
+        <v>8.1760513434124243E-2</v>
       </c>
       <c r="AC66" s="158">
         <f t="shared" si="0"/>
@@ -11756,56 +11758,56 @@
       </c>
       <c r="AD66" s="159">
         <f t="shared" si="1"/>
-        <v>2.7222222222222219</v>
+        <v>1.2222222222222221</v>
       </c>
       <c r="AE66" s="160" t="e">
-        <f>(-1 * ((((1 / AD66)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
+        <f t="shared" si="13"/>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="67" spans="17:31">
+    <row r="67" spans="17:31" x14ac:dyDescent="0.2">
       <c r="Q67" s="119">
         <v>0.6</v>
       </c>
       <c r="R67" s="130">
         <f>MAX((Q67-rc_vg)/(sc_vg-rc_vg),0)</f>
-        <v>2.7777777777777772</v>
+        <v>1.2469135802469136</v>
       </c>
       <c r="S67" s="131">
-        <f t="shared" si="13"/>
-        <v>2420.6283125120053</v>
+        <f t="shared" si="15"/>
+        <v>132.80698953325199</v>
       </c>
       <c r="T67" s="131">
-        <f t="shared" si="14"/>
-        <v>467.7733466555797</v>
+        <f t="shared" si="16"/>
+        <v>24.517542763558772</v>
       </c>
       <c r="U67" s="131">
-        <f t="shared" si="15"/>
-        <v>95.536324300238149</v>
+        <f t="shared" si="17"/>
+        <v>5.2644914980615525</v>
       </c>
       <c r="V67" s="131">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.368385593142037</v>
       </c>
       <c r="W67" s="131">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.29839751798850311</v>
       </c>
       <c r="X67" s="131">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>8.3207940750375742E-2</v>
       </c>
       <c r="Y67" s="131">
-        <f t="shared" si="19"/>
-        <v>1.3676124793169921</v>
+        <f t="shared" si="21"/>
+        <v>1.3544301327622559</v>
       </c>
       <c r="Z67" s="131">
-        <f t="shared" si="20"/>
-        <v>0.29820728843534156</v>
+        <f t="shared" si="22"/>
+        <v>0.29480945814746984</v>
       </c>
       <c r="AA67" s="136">
-        <f t="shared" si="21"/>
-        <v>8.3135533353668661E-2</v>
+        <f t="shared" si="23"/>
+        <v>8.1913260396115545E-2</v>
       </c>
       <c r="AC67" s="161">
         <f t="shared" si="0"/>
@@ -11813,10 +11815,10 @@
       </c>
       <c r="AD67" s="162">
         <f t="shared" si="1"/>
-        <v>2.7777777777777772</v>
+        <v>1.2469135802469136</v>
       </c>
       <c r="AE67" s="163" t="e">
-        <f>(-1 * ((((1 / AD67)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
+        <f t="shared" si="13"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -11834,7 +11836,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11844,33 +11846,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1432D1FA-6D1A-5B47-9BFC-4C8DE5F35F87}">
   <dimension ref="E1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="9" max="9" width="15.83203125" customWidth="1"/>
     <col min="10" max="10" width="15.1640625" customWidth="1"/>
     <col min="11" max="11" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="5:15">
+    <row r="1" spans="5:15" x14ac:dyDescent="0.2">
       <c r="E1" s="170" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="2" spans="5:15">
+    <row r="2" spans="5:15" x14ac:dyDescent="0.2">
       <c r="E2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="3" spans="5:15">
+    <row r="3" spans="5:15" x14ac:dyDescent="0.2">
       <c r="E3" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="5" spans="5:15" ht="18">
+    <row r="5" spans="5:15" ht="18" x14ac:dyDescent="0.2">
       <c r="I5" t="s">
         <v>166</v>
       </c>
@@ -11893,7 +11895,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="5:15">
+    <row r="6" spans="5:15" x14ac:dyDescent="0.2">
       <c r="I6" s="164"/>
       <c r="J6" s="164">
         <v>0.43</v>
@@ -11914,7 +11916,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="5:15">
+    <row r="7" spans="5:15" x14ac:dyDescent="0.2">
       <c r="I7" s="164" t="s">
         <v>155</v>
       </c>
@@ -11937,7 +11939,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="5:15">
+    <row r="8" spans="5:15" x14ac:dyDescent="0.2">
       <c r="I8" s="164" t="s">
         <v>156</v>
       </c>
@@ -11960,7 +11962,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="5:15">
+    <row r="9" spans="5:15" x14ac:dyDescent="0.2">
       <c r="I9" s="164" t="s">
         <v>157</v>
       </c>
@@ -11983,7 +11985,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="5:15">
+    <row r="10" spans="5:15" x14ac:dyDescent="0.2">
       <c r="I10" s="164" t="s">
         <v>158</v>
       </c>
@@ -12006,7 +12008,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="5:15">
+    <row r="11" spans="5:15" x14ac:dyDescent="0.2">
       <c r="I11" s="164" t="s">
         <v>159</v>
       </c>
@@ -12029,7 +12031,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="5:15">
+    <row r="12" spans="5:15" x14ac:dyDescent="0.2">
       <c r="I12" s="164" t="s">
         <v>160</v>
       </c>
@@ -12052,7 +12054,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="5:15">
+    <row r="13" spans="5:15" x14ac:dyDescent="0.2">
       <c r="I13" s="164" t="s">
         <v>161</v>
       </c>
@@ -12075,7 +12077,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="5:15">
+    <row r="14" spans="5:15" x14ac:dyDescent="0.2">
       <c r="I14" s="164" t="s">
         <v>162</v>
       </c>
@@ -12098,7 +12100,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="5:15">
+    <row r="15" spans="5:15" x14ac:dyDescent="0.2">
       <c r="I15" s="164" t="s">
         <v>163</v>
       </c>
@@ -12121,7 +12123,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="5:15">
+    <row r="16" spans="5:15" x14ac:dyDescent="0.2">
       <c r="I16" s="164" t="s">
         <v>164</v>
       </c>
@@ -12144,7 +12146,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="9:15">
+    <row r="17" spans="9:15" x14ac:dyDescent="0.2">
       <c r="I17" s="164" t="s">
         <v>165</v>
       </c>
@@ -12167,7 +12169,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="9:15" ht="18">
+    <row r="23" spans="9:15" ht="18" x14ac:dyDescent="0.2">
       <c r="I23" s="169"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated functions for developement
</commit_message>
<xml_diff>
--- a/for_development/dev_documentation/soil-root-calibration_V3.xlsx
+++ b/for_development/dev_documentation/soil-root-calibration_V3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jruffault/Dropbox/Mon Mac (MacBook-Pro-de-Julien.local)/Desktop/SurEau-Ecos/for_development/dev_documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBCF6A83-8C74-4548-BC01-F69A26918516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97FF996B-4114-1845-BDE6-C587F2B868B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7400" yWindow="500" windowWidth="31000" windowHeight="17440" xr2:uid="{D9106142-DCBD-4E45-A888-1E539F445614}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{D9106142-DCBD-4E45-A888-1E539F445614}"/>
   </bookViews>
   <sheets>
     <sheet name="WorkSheet" sheetId="1" r:id="rId1"/>
@@ -2685,157 +2685,157 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.5925888793794001E-4</c:v>
+                  <c:v>2.0454398520257967E-13</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.3616134230305676E-3</c:v>
+                  <c:v>1.2347569274838125E-9</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.8715960862765442E-3</c:v>
+                  <c:v>3.0642209572168811E-8</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.3370317102745014E-3</c:v>
+                  <c:v>2.5353030730332247E-7</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>9.1935735207933876E-3</c:v>
+                  <c:v>1.2704850336584736E-6</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.5003057720066113E-2</c:v>
+                  <c:v>4.7486473455361937E-6</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.3480243747916522E-2</c:v>
+                  <c:v>1.4606024170630213E-5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.5520236959888214E-2</c:v>
+                  <c:v>3.9049972626112854E-5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5.2228000126832846E-2</c:v>
+                  <c:v>9.3870019314160969E-5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7.4950331077162757E-2</c:v>
+                  <c:v>2.0750203885895669E-4</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.10531049791441752</c:v>
+                  <c:v>4.2851699766808604E-4</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.14524568383104364</c:v>
+                  <c:v>8.3634458711355345E-4</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.19704739054208348</c:v>
+                  <c:v>1.5562218972464804E-3</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.26340495830866423</c:v>
+                  <c:v>2.7795617716452796E-3</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.34745237470956025</c:v>
+                  <c:v>4.7911668007790953E-3</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.45281856168104484</c:v>
+                  <c:v>8.0049754635572058E-3</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.58368135024671663</c:v>
+                  <c:v>1.3010319402707046E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.74482537467739096</c:v>
+                  <c:v>2.0630998228586515E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.94170414265257341</c:v>
+                  <c:v>3.1999843965140773E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.1805065655457774</c:v>
+                  <c:v>4.8651855079305584E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.4682282635072366</c:v>
+                  <c:v>7.2639434251915228E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.812747993913171</c:v>
+                  <c:v>0.10667376948758543</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.2229095893939594</c:v>
+                  <c:v>0.15429696029076861</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.7086098335157511</c:v>
+                  <c:v>0.22009011565144446</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.2808927488128257</c:v>
+                  <c:v>0.30992334552126366</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.9520508238798979</c:v>
+                  <c:v>0.43125434032024884</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>4.7357337643565272</c:v>
+                  <c:v>0.59348309291227175</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>5.6470654177066297</c:v>
+                  <c:v>0.80837127483281701</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>6.7027695946832884</c:v>
+                  <c:v>1.0905358452516105</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>7.9213055923924749</c:v>
+                  <c:v>1.4580276608530143</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>9.3230143162290542</c:v>
+                  <c:v>1.9330071831962097</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>10.930276002175972</c:v>
+                  <c:v>2.5425308652218259</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>12.767680658793845</c:v>
+                  <c:v>3.3194634612261211</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>14.862212481749824</c:v>
+                  <c:v>4.303533368910303</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>17.243449645369402</c:v>
+                  <c:v>5.5425502059554006</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>19.94378104827738</c:v>
+                  <c:v>7.0938061794239253</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>22.998641787083621</c:v>
+                  <c:v>9.0256854619755629</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>26.446769357223328</c:v>
+                  <c:v>11.419508788604851</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>30.330482838165832</c:v>
+                  <c:v>14.371643883165621</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>34.695987616838806</c:v>
+                  <c:v>17.995916176232406</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>39.59370854492181</c:v>
+                  <c:v>22.426358656651079</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>45.078654820580034</c:v>
+                  <c:v>27.820344693367897</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>51.210820342780124</c:v>
+                  <c:v>34.36215337257147</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>58.055623818019448</c:v>
+                  <c:v>42.267023437842923</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>65.684393518993474</c:v>
+                  <c:v>51.785759441308585</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>74.174902319225055</c:v>
+                  <c:v>63.209962383785772</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>83.611959477491524</c:v>
+                  <c:v>76.877967148800252</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>94.088066646031905</c:v>
+                  <c:v>93.181580669692693</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>105.70414675778086</c:v>
+                  <c:v>112.57372831505542</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>118.57035584815631</c:v>
+                  <c:v>135.57713180653354</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>132.80698953325199</c:v>
+                  <c:v>162.79416054932216</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3096,157 +3096,157 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.5910480274279379E-4</c:v>
+                  <c:v>2.0454398520250109E-13</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.3602598950913313E-3</c:v>
+                  <c:v>1.2347569246185997E-9</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.8655825797312406E-3</c:v>
+                  <c:v>3.0642207807618447E-8</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.316296878539792E-3</c:v>
+                  <c:v>2.5353018650706352E-7</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>9.1322182127808633E-3</c:v>
+                  <c:v>1.2704820002423169E-6</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.4840347305453874E-2</c:v>
+                  <c:v>4.7486049685676018E-6</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.3084141026052558E-2</c:v>
+                  <c:v>1.4605623261418749E-5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.4621539051072632E-2</c:v>
+                  <c:v>3.9047107105590395E-5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5.0307869269171697E-2</c:v>
+                  <c:v>9.385346271504301E-5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7.1058269614329539E-2</c:v>
+                  <c:v>2.0742115360761592E-4</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9.778499721024439E-2</c:v>
+                  <c:v>4.2817218720759057E-4</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.13130813576865469</c:v>
+                  <c:v>8.350321383233855E-4</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.17224423734157626</c:v>
+                  <c:v>1.5516838533916506E-3</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.22088591565340021</c:v>
+                  <c:v>2.7651178904414169E-3</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.27709424360789786</c:v>
+                  <c:v>4.7484121245796578E-3</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.34023115666120018</c:v>
+                  <c:v>7.8863359911596383E-3</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.409156639513995</c:v>
+                  <c:v>1.2699806962644774E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.48230315270739788</c:v>
+                  <c:v>1.9860956384922822E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.55782005427798043</c:v>
+                  <c:v>3.0184630713840487E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.63376089545272862</c:v>
+                  <c:v>4.4576209022731829E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.70827490266880677</c:v>
+                  <c:v>6.391443615834369E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.77976550527831168</c:v>
+                  <c:v>8.8859930015298863E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.84699176825559819</c:v>
+                  <c:v>0.11961293816739084</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.90910640943844057</c:v>
+                  <c:v>0.15569330045970042</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.96563940463757103</c:v>
+                  <c:v>0.19585205581835749</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1.0164447024421746</c:v>
+                  <c:v>0.23820255551380842</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1.0616289552302225</c:v>
+                  <c:v>0.28056326459317776</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1.1014777167099887</c:v>
+                  <c:v>0.32088864396462774</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1.1363891703321813</c:v>
+                  <c:v>0.35761913741145962</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1.166820321044034</c:v>
+                  <c:v>0.38984096647168703</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1.1932467762058712</c:v>
+                  <c:v>0.41725444196353489</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1.2161349505004408</c:v>
+                  <c:v>0.44002475277648928</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1.2359244757316503</c:v>
+                  <c:v>0.45860114884800435</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>1.253018363735048</c:v>
+                  <c:v>0.47356159328931258</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1.2677786885825035</c:v>
+                  <c:v>0.48550455893174055</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1.2805259605188766</c:v>
+                  <c:v>0.49498614224828158</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1.2915408019288817</c:v>
+                  <c:v>0.50249098834064554</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>1.3010669269379471</c:v>
+                  <c:v>0.50842460263644196</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>1.3093147422195068</c:v>
+                  <c:v>0.51311733299329509</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1.3164651252438047</c:v>
+                  <c:v>0.5168336079784428</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1.3226731077108129</c:v>
+                  <c:v>0.5197826905807269</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>1.3280713101470438</c:v>
+                  <c:v>0.52212901569510739</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>1.3327730520587682</c:v>
+                  <c:v>0.52400127125602336</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>1.3368751119396871</c:v>
+                  <c:v>0.52549998173866808</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>1.3404601416348407</c:v>
+                  <c:v>0.52670364858884644</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>1.3435987565710525</c:v>
+                  <c:v>0.52767362627345171</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>1.346351331808286</c:v>
+                  <c:v>0.52845794668938817</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>1.3487695369447354</c:v>
+                  <c:v>0.529094295768477</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>1.3508976427741337</c:v>
+                  <c:v>0.52961231984433843</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>1.3527736306600466</c:v>
+                  <c:v>0.53003540868252186</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>1.3544301327622559</c:v>
+                  <c:v>0.5303820730203862</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3480,184 +3480,184 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>1.368385593142037</c:v>
+                  <c:v>0.53211570172066014</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4296,58 +4296,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>-40.03627388240605</c:v>
+                  <c:v>-15.086374742707315</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-15.812802138851525</c:v>
+                  <c:v>-6.3438934611055888</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-8.573309019436488</c:v>
+                  <c:v>-3.7115976033156328</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-5.4251618951836793</c:v>
+                  <c:v>-2.5138190291476286</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-3.7628840854179857</c:v>
+                  <c:v>-1.8497122268158754</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-2.7733271364219005</c:v>
+                  <c:v>-1.4355601166618484</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-2.1340109821626103</c:v>
+                  <c:v>-1.1562157907434101</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-1.695629994580736</c:v>
+                  <c:v>-0.95690260829654494</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-1.3810808706842324</c:v>
+                  <c:v>-0.80853529907938304</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-1.1471658159994846</c:v>
+                  <c:v>-0.6943676187122968</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.968101443057651</c:v>
+                  <c:v>-0.60413784470221177</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.82769874290523227</c:v>
+                  <c:v>-0.531238660865896</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-0.71536206370457789</c:v>
+                  <c:v>-0.47124061861923627</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-0.62391201418098852</c:v>
+                  <c:v>-0.42107299954196131</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-0.54833885676102501</c:v>
+                  <c:v>-0.37854580116417574</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-0.48505736422050805</c:v>
+                  <c:v>-0.34205869081005458</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-0.43144475917474873</c:v>
+                  <c:v>-0.31041727102801847</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-0.38554494183855909</c:v>
+                  <c:v>-0.2827134117094004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7285,8 +7285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B673C9AC-1A9D-EA45-B245-5C46BCC162EE}">
   <dimension ref="A1:AE67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="64" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="105" zoomScaleNormal="64" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7471,7 +7471,7 @@
         <v>94</v>
       </c>
       <c r="G7" s="138">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="I7" s="71" t="s">
         <v>45</v>
@@ -7493,7 +7493,7 @@
       </c>
       <c r="O7" s="146">
         <f>LAI*fRootToLeaf</f>
-        <v>6</v>
+        <v>2.4</v>
       </c>
       <c r="Q7" s="121" t="s">
         <v>133</v>
@@ -7579,7 +7579,7 @@
       </c>
       <c r="O8" s="147">
         <f>1-(1/n)</f>
-        <v>0.35483870967741937</v>
+        <v>0.41176470588235292</v>
       </c>
       <c r="Q8" s="114">
         <v>0.01</v>
@@ -7602,15 +7602,15 @@
       </c>
       <c r="V8" s="128">
         <f t="shared" ref="V8:V39" si="6">kroot1</f>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W8" s="128">
         <f t="shared" ref="W8:W39" si="7">kroot2</f>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X8" s="128">
         <f t="shared" ref="X8:X39" si="8">kroot3</f>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y8" s="128" t="e">
         <f t="shared" ref="Y8:Y39" si="9">1/((1/kroot1)+(1/S8))</f>
@@ -7674,7 +7674,7 @@
       </c>
       <c r="O9" s="147">
         <f>1-beta^(100*depth1)</f>
-        <v>0.78193462465259256</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="Q9" s="118">
         <v>0.02</v>
@@ -7697,15 +7697,15 @@
       </c>
       <c r="V9" s="129">
         <f t="shared" si="6"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W9" s="129">
         <f t="shared" si="7"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X9" s="129">
         <f t="shared" si="8"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y9" s="129" t="e">
         <f t="shared" si="9"/>
@@ -7749,7 +7749,7 @@
         <v>32</v>
       </c>
       <c r="G10" s="138">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I10" s="73" t="s">
         <v>80</v>
@@ -7769,7 +7769,7 @@
       </c>
       <c r="O10" s="148">
         <f>1-(beta^(100*depth2))-rootP1</f>
-        <v>0.17051286742200178</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="Q10" s="118">
         <v>0.03</v>
@@ -7792,15 +7792,15 @@
       </c>
       <c r="V10" s="129">
         <f t="shared" si="6"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W10" s="129">
         <f t="shared" si="7"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X10" s="129">
         <f t="shared" si="8"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y10" s="129" t="e">
         <f t="shared" si="9"/>
@@ -7844,7 +7844,7 @@
         <v>32</v>
       </c>
       <c r="G11" s="138">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="I11" s="73" t="s">
         <v>81</v>
@@ -7864,7 +7864,7 @@
       </c>
       <c r="O11" s="148">
         <f>1-(beta^(100*depth3))-rootP1-rootP2</f>
-        <v>4.7547394714500424E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Q11" s="118">
         <v>0.04</v>
@@ -7887,15 +7887,15 @@
       </c>
       <c r="V11" s="129">
         <f t="shared" si="6"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W11" s="129">
         <f t="shared" si="7"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X11" s="129">
         <f t="shared" si="8"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y11" s="129" t="e">
         <f t="shared" si="9"/>
@@ -7939,7 +7939,7 @@
         <v>32</v>
       </c>
       <c r="G12" s="138">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="I12" s="73" t="s">
         <v>19</v>
@@ -7959,7 +7959,7 @@
       <c r="N12" s="8"/>
       <c r="O12" s="149">
         <f>RAI/(2*PI()*root_radius)</f>
-        <v>4774.6482927568604</v>
+        <v>1909.8593171027439</v>
       </c>
       <c r="Q12" s="118">
         <v>0.05</v>
@@ -7982,15 +7982,15 @@
       </c>
       <c r="V12" s="129">
         <f t="shared" si="6"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W12" s="129">
         <f t="shared" si="7"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X12" s="129">
         <f t="shared" si="8"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y12" s="129" t="e">
         <f t="shared" si="9"/>
@@ -8044,7 +8044,7 @@
       </c>
       <c r="O13" s="149">
         <f>La*rootP1</f>
-        <v>3733.4628206449775</v>
+        <v>1016.2661307078673</v>
       </c>
       <c r="Q13" s="118">
         <v>0.06</v>
@@ -8067,15 +8067,15 @@
       </c>
       <c r="V13" s="129">
         <f t="shared" si="6"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W13" s="129">
         <f t="shared" si="7"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X13" s="129">
         <f t="shared" si="8"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y13" s="129" t="e">
         <f t="shared" si="9"/>
@@ -8131,7 +8131,7 @@
       </c>
       <c r="O14" s="149">
         <f>La*rootP2</f>
-        <v>814.13897132953764</v>
+        <v>741.72634948149835</v>
       </c>
       <c r="Q14" s="118">
         <v>7.0000000000000007E-2</v>
@@ -8154,15 +8154,15 @@
       </c>
       <c r="V14" s="129">
         <f t="shared" si="6"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W14" s="129">
         <f t="shared" si="7"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X14" s="129">
         <f t="shared" si="8"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y14" s="129" t="e">
         <f t="shared" si="9"/>
@@ -8228,7 +8228,7 @@
       </c>
       <c r="O15" s="149">
         <f>La*rootP3</f>
-        <v>227.02208699862601</v>
+        <v>151.79048012434265</v>
       </c>
       <c r="Q15" s="118">
         <v>0.08</v>
@@ -8251,15 +8251,15 @@
       </c>
       <c r="V15" s="129">
         <f t="shared" si="6"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W15" s="129">
         <f t="shared" si="7"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X15" s="129">
         <f t="shared" si="8"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y15" s="129" t="e">
         <f t="shared" si="9"/>
@@ -8321,7 +8321,7 @@
       <c r="N16" s="8"/>
       <c r="O16" s="149">
         <f>La_1/(depth1*(1-(RFC_1/100)))</f>
-        <v>29867.70256515982</v>
+        <v>14114.807370942603</v>
       </c>
       <c r="Q16" s="118">
         <v>0.09</v>
@@ -8344,15 +8344,15 @@
       </c>
       <c r="V16" s="129">
         <f t="shared" si="6"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W16" s="129">
         <f t="shared" si="7"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X16" s="129">
         <f t="shared" si="8"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y16" s="129" t="e">
         <f t="shared" si="9"/>
@@ -8394,7 +8394,7 @@
       </c>
       <c r="F17" s="49"/>
       <c r="G17" s="139">
-        <v>1.55</v>
+        <v>1.7</v>
       </c>
       <c r="I17" s="73" t="s">
         <v>74</v>
@@ -8416,50 +8416,50 @@
       </c>
       <c r="O17" s="149">
         <f>La_2/((depth2-depth1)*(1-(RFC_2/100)))</f>
-        <v>10855.186284393834</v>
+        <v>8830.0755890654582</v>
       </c>
       <c r="Q17" s="118">
         <v>0.1</v>
       </c>
       <c r="R17" s="117">
         <f t="shared" si="2"/>
-        <v>1.2345679012345689E-2</v>
+        <v>4.975124378109457E-3</v>
       </c>
       <c r="S17" s="129">
         <f t="shared" si="3"/>
-        <v>4.5925888793794001E-4</v>
+        <v>2.0454398520257967E-13</v>
       </c>
       <c r="T17" s="129">
         <f t="shared" si="4"/>
-        <v>8.4783936930846957E-5</v>
+        <v>1.3899522216623486E-13</v>
       </c>
       <c r="U17" s="129">
         <f t="shared" si="5"/>
-        <v>1.8205099893128233E-5</v>
+        <v>2.0248335047652808E-14</v>
       </c>
       <c r="V17" s="129">
         <f t="shared" si="6"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W17" s="129">
         <f t="shared" si="7"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X17" s="129">
         <f t="shared" si="8"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y17" s="129">
         <f t="shared" si="9"/>
-        <v>4.5910480274279379E-4</v>
+        <v>2.0454398520250109E-13</v>
       </c>
       <c r="Z17" s="129">
         <f t="shared" si="10"/>
-        <v>8.475985404246421E-5</v>
+        <v>1.389952221661851E-13</v>
       </c>
       <c r="AA17" s="135">
         <f t="shared" si="11"/>
-        <v>1.8201117663040167E-5</v>
+        <v>2.0248335047647649E-14</v>
       </c>
       <c r="AC17" s="158">
         <f t="shared" si="0"/>
@@ -8467,11 +8467,11 @@
       </c>
       <c r="AD17" s="159">
         <f t="shared" si="1"/>
-        <v>1.2345679012345689E-2</v>
+        <v>4.975124378109457E-3</v>
       </c>
       <c r="AE17" s="160">
         <f t="shared" si="12"/>
-        <v>-295.10161713880905</v>
+        <v>-195.10995583381734</v>
       </c>
     </row>
     <row r="18" spans="1:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -8489,7 +8489,7 @@
       </c>
       <c r="F18" s="49"/>
       <c r="G18" s="139">
-        <v>0.5</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="I18" s="73" t="s">
         <v>75</v>
@@ -8511,50 +8511,50 @@
       </c>
       <c r="O18" s="149">
         <f>La_3/((depth3-depth2)*(1-(RFC_3/100)))</f>
-        <v>1513.4805799908388</v>
+        <v>562.18696342349153</v>
       </c>
       <c r="Q18" s="118">
         <v>0.11</v>
       </c>
       <c r="R18" s="117">
         <f t="shared" si="2"/>
-        <v>3.7037037037037035E-2</v>
+        <v>2.9850746268656705E-2</v>
       </c>
       <c r="S18" s="129">
         <f t="shared" si="3"/>
-        <v>1.3616134230305676E-3</v>
+        <v>1.2347569274838125E-9</v>
       </c>
       <c r="T18" s="129">
         <f t="shared" si="4"/>
-        <v>2.5136790950471092E-4</v>
+        <v>8.3906311538289872E-10</v>
       </c>
       <c r="U18" s="129">
         <f t="shared" si="5"/>
-        <v>5.3974586084538481E-5</v>
+        <v>1.2223176323342338E-10</v>
       </c>
       <c r="V18" s="129">
         <f t="shared" si="6"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W18" s="129">
         <f t="shared" si="7"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X18" s="129">
         <f t="shared" si="8"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y18" s="129">
         <f t="shared" si="9"/>
-        <v>1.3602598950913313E-3</v>
+        <v>1.2347569246185997E-9</v>
       </c>
       <c r="Z18" s="129">
         <f t="shared" si="10"/>
-        <v>2.511563372239747E-4</v>
+        <v>8.3906311357011121E-10</v>
       </c>
       <c r="AA18" s="135">
         <f t="shared" si="11"/>
-        <v>5.3939597027041723E-5</v>
+        <v>1.2223176304543759E-10</v>
       </c>
       <c r="AC18" s="158">
         <f t="shared" si="0"/>
@@ -8562,11 +8562,11 @@
       </c>
       <c r="AD18" s="159">
         <f t="shared" si="1"/>
-        <v>3.7037037037037035E-2</v>
+        <v>2.9850746268656705E-2</v>
       </c>
       <c r="AE18" s="160">
         <f t="shared" si="12"/>
-        <v>-40.03627388240605</v>
+        <v>-15.086374742707315</v>
       </c>
     </row>
     <row r="19" spans="1:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -8598,50 +8598,50 @@
       <c r="N19" s="8"/>
       <c r="O19" s="149">
         <f>2*PI()*La_1/LN((1/SQRT(PI()*Lv_1))/root_radius)</f>
-        <v>8400.1862183303838</v>
+        <v>2016.0107985664499</v>
       </c>
       <c r="Q19" s="118">
         <v>0.12</v>
       </c>
       <c r="R19" s="117">
         <f t="shared" si="2"/>
-        <v>6.1728395061728378E-2</v>
+        <v>5.4726368159203953E-2</v>
       </c>
       <c r="S19" s="129">
         <f t="shared" si="3"/>
-        <v>2.8715960862765442E-3</v>
+        <v>3.0642209572168811E-8</v>
       </c>
       <c r="T19" s="129">
         <f t="shared" si="4"/>
-        <v>5.3012631407720761E-4</v>
+        <v>2.0822517576988215E-8</v>
       </c>
       <c r="U19" s="129">
         <f t="shared" si="5"/>
-        <v>1.1383055391286166E-4</v>
+        <v>3.0333511171358711E-9</v>
       </c>
       <c r="V19" s="129">
         <f t="shared" si="6"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W19" s="129">
         <f t="shared" si="7"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X19" s="129">
         <f t="shared" si="8"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y19" s="129">
         <f t="shared" si="9"/>
-        <v>2.8655825797312406E-3</v>
+        <v>3.0642207807618447E-8</v>
       </c>
       <c r="Z19" s="129">
         <f t="shared" si="10"/>
-        <v>5.2918617383178876E-4</v>
+        <v>2.0822516460577174E-8</v>
       </c>
       <c r="AA19" s="135">
         <f t="shared" si="11"/>
-        <v>1.1367504359663485E-4</v>
+        <v>3.0333510013642288E-9</v>
       </c>
       <c r="AC19" s="158">
         <f t="shared" si="0"/>
@@ -8649,11 +8649,11 @@
       </c>
       <c r="AD19" s="159">
         <f t="shared" si="1"/>
-        <v>6.1728395061728378E-2</v>
+        <v>5.4726368159203953E-2</v>
       </c>
       <c r="AE19" s="160">
         <f t="shared" si="12"/>
-        <v>-15.812802138851525</v>
+        <v>-6.3438934611055888</v>
       </c>
     </row>
     <row r="20" spans="1:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -8689,50 +8689,50 @@
       </c>
       <c r="O20" s="149">
         <f>2*PI()*La_2/LN((1/SQRT(PI()*Lv_2))/root_radius)</f>
-        <v>1550.7611877476247</v>
+        <v>1369.9540886462507</v>
       </c>
       <c r="Q20" s="118">
         <v>0.13</v>
       </c>
       <c r="R20" s="117">
         <f t="shared" si="2"/>
-        <v>8.6419753086419762E-2</v>
+        <v>7.9601990049751242E-2</v>
       </c>
       <c r="S20" s="129">
         <f t="shared" si="3"/>
-        <v>5.3370317102745014E-3</v>
+        <v>2.5353030730332247E-7</v>
       </c>
       <c r="T20" s="129">
         <f t="shared" si="4"/>
-        <v>9.8527120934671923E-4</v>
+        <v>1.7228324438187715E-7</v>
       </c>
       <c r="U20" s="129">
         <f t="shared" si="5"/>
-        <v>2.1156083849480076E-4</v>
+        <v>2.5097617032971093E-8</v>
       </c>
       <c r="V20" s="129">
         <f t="shared" si="6"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W20" s="129">
         <f t="shared" si="7"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X20" s="129">
         <f t="shared" si="8"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y20" s="129">
         <f t="shared" si="9"/>
-        <v>5.316296878539792E-3</v>
+        <v>2.5353018650706352E-7</v>
       </c>
       <c r="Z20" s="129">
         <f t="shared" si="10"/>
-        <v>9.8202867373347116E-4</v>
+        <v>1.7228316795544933E-7</v>
       </c>
       <c r="AA20" s="135">
         <f t="shared" si="11"/>
-        <v>2.1102429742787839E-4</v>
+        <v>2.5097609107562125E-8</v>
       </c>
       <c r="AC20" s="158">
         <f t="shared" si="0"/>
@@ -8740,11 +8740,11 @@
       </c>
       <c r="AD20" s="159">
         <f t="shared" si="1"/>
-        <v>8.6419753086419762E-2</v>
+        <v>7.9601990049751242E-2</v>
       </c>
       <c r="AE20" s="160">
         <f t="shared" si="12"/>
-        <v>-8.573309019436488</v>
+        <v>-3.7115976033156328</v>
       </c>
     </row>
     <row r="21" spans="1:31" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -8764,7 +8764,7 @@
         <v>141</v>
       </c>
       <c r="G21" s="140">
-        <v>9.5000000000000001E-2</v>
+        <v>9.8000000000000004E-2</v>
       </c>
       <c r="I21" s="73" t="s">
         <v>78</v>
@@ -8780,50 +8780,50 @@
       </c>
       <c r="O21" s="149">
         <f>2*PI()*La_3/LN((1/SQRT(PI()*Lv_3))/root_radius)</f>
-        <v>332.98480060389988</v>
+        <v>199.57009280243918</v>
       </c>
       <c r="Q21" s="118">
         <v>0.14000000000000001</v>
       </c>
       <c r="R21" s="117">
         <f t="shared" si="2"/>
-        <v>0.11111111111111113</v>
+        <v>0.10447761194029853</v>
       </c>
       <c r="S21" s="129">
         <f t="shared" si="3"/>
-        <v>9.1935735207933876E-3</v>
+        <v>1.2704850336584736E-6</v>
       </c>
       <c r="T21" s="129">
         <f t="shared" si="4"/>
-        <v>1.6972286830546463E-3</v>
+        <v>8.6334168827961583E-7</v>
       </c>
       <c r="U21" s="129">
         <f t="shared" si="5"/>
-        <v>3.6443480728777771E-4</v>
+        <v>1.2576858033281728E-7</v>
       </c>
       <c r="V21" s="129">
         <f t="shared" si="6"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W21" s="129">
         <f t="shared" si="7"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X21" s="129">
         <f t="shared" si="8"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y21" s="129">
         <f t="shared" si="9"/>
-        <v>9.1322182127808633E-3</v>
+        <v>1.2704820002423169E-6</v>
       </c>
       <c r="Z21" s="129">
         <f t="shared" si="10"/>
-        <v>1.6876297639314931E-3</v>
+        <v>8.6333976907124437E-7</v>
       </c>
       <c r="AA21" s="135">
         <f t="shared" si="11"/>
-        <v>3.6284561315662317E-4</v>
+        <v>1.2576838131109826E-7</v>
       </c>
       <c r="AC21" s="158">
         <f t="shared" si="0"/>
@@ -8831,11 +8831,11 @@
       </c>
       <c r="AD21" s="159">
         <f t="shared" si="1"/>
-        <v>0.11111111111111113</v>
+        <v>0.10447761194029853</v>
       </c>
       <c r="AE21" s="160">
         <f t="shared" si="12"/>
-        <v>-5.4251618951836793</v>
+        <v>-2.5138190291476286</v>
       </c>
     </row>
     <row r="22" spans="1:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -8861,50 +8861,50 @@
       <c r="N22" s="3"/>
       <c r="O22" s="147">
         <f>KRootTotal*rootP1</f>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="Q22" s="118">
         <v>0.15</v>
       </c>
       <c r="R22" s="117">
         <f t="shared" si="2"/>
-        <v>0.13580246913580243</v>
+        <v>0.12935323383084574</v>
       </c>
       <c r="S22" s="129">
         <f t="shared" si="3"/>
-        <v>1.5003057720066113E-2</v>
+        <v>4.7486473455361937E-6</v>
       </c>
       <c r="T22" s="129">
         <f t="shared" si="4"/>
-        <v>2.7697195044373989E-3</v>
+        <v>3.2268819448697255E-6</v>
       </c>
       <c r="U22" s="129">
         <f t="shared" si="5"/>
-        <v>5.9472374225032069E-4</v>
+        <v>4.7008081112888831E-7</v>
       </c>
       <c r="V22" s="129">
         <f t="shared" si="6"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W22" s="129">
         <f t="shared" si="7"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X22" s="129">
         <f t="shared" si="8"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y22" s="129">
         <f t="shared" si="9"/>
-        <v>1.4840347305453874E-2</v>
+        <v>4.7486049685676018E-6</v>
       </c>
       <c r="Z22" s="129">
         <f t="shared" si="10"/>
-        <v>2.7442474570888195E-3</v>
+        <v>3.2268551334250277E-6</v>
       </c>
       <c r="AA22" s="135">
         <f t="shared" si="11"/>
-        <v>5.9050315652386866E-4</v>
+        <v>4.7007803077983929E-7</v>
       </c>
       <c r="AC22" s="158">
         <f t="shared" si="0"/>
@@ -8912,11 +8912,11 @@
       </c>
       <c r="AD22" s="159">
         <f t="shared" si="1"/>
-        <v>0.13580246913580243</v>
+        <v>0.12935323383084574</v>
       </c>
       <c r="AE22" s="160">
         <f t="shared" si="12"/>
-        <v>-3.7628840854179857</v>
+        <v>-1.8497122268158754</v>
       </c>
     </row>
     <row r="23" spans="1:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -8944,50 +8944,50 @@
       <c r="N23" s="3"/>
       <c r="O23" s="147">
         <f>KRootTotal*rootP2</f>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="Q23" s="118">
         <v>0.16</v>
       </c>
       <c r="R23" s="117">
         <f t="shared" si="2"/>
-        <v>0.16049382716049382</v>
+        <v>0.15422885572139303</v>
       </c>
       <c r="S23" s="129">
         <f t="shared" si="3"/>
-        <v>2.3480243747916522E-2</v>
+        <v>1.4606024170630213E-5</v>
       </c>
       <c r="T23" s="129">
         <f t="shared" si="4"/>
-        <v>4.3346956527780455E-3</v>
+        <v>9.9253349960472873E-6</v>
       </c>
       <c r="U23" s="129">
         <f t="shared" si="5"/>
-        <v>9.3076082830994232E-4</v>
+        <v>1.4458878897276214E-6</v>
       </c>
       <c r="V23" s="129">
         <f t="shared" si="6"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W23" s="129">
         <f t="shared" si="7"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X23" s="129">
         <f t="shared" si="8"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y23" s="129">
         <f t="shared" si="9"/>
-        <v>2.3084141026052558E-2</v>
+        <v>1.4605623261418749E-5</v>
       </c>
       <c r="Z23" s="129">
         <f t="shared" si="10"/>
-        <v>4.2726289629593092E-3</v>
+        <v>9.9250813448486128E-6</v>
       </c>
       <c r="AA23" s="135">
         <f t="shared" si="11"/>
-        <v>9.2046454724948354E-4</v>
+        <v>1.4458615859464616E-6</v>
       </c>
       <c r="AC23" s="158">
         <f t="shared" si="0"/>
@@ -8995,11 +8995,11 @@
       </c>
       <c r="AD23" s="159">
         <f t="shared" si="1"/>
-        <v>0.16049382716049382</v>
+        <v>0.15422885572139303</v>
       </c>
       <c r="AE23" s="160">
         <f t="shared" si="12"/>
-        <v>-2.7733271364219005</v>
+        <v>-1.4355601166618484</v>
       </c>
     </row>
     <row r="24" spans="1:31" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -9037,50 +9037,50 @@
       <c r="N24" s="4"/>
       <c r="O24" s="150">
         <f>KRootTotal*rootP3</f>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Q24" s="118">
         <v>0.17</v>
       </c>
       <c r="R24" s="117">
         <f t="shared" si="2"/>
-        <v>0.1851851851851852</v>
+        <v>0.17910447761194032</v>
       </c>
       <c r="S24" s="129">
         <f t="shared" si="3"/>
-        <v>3.5520236959888214E-2</v>
+        <v>3.9049972626112854E-5</v>
       </c>
       <c r="T24" s="129">
         <f t="shared" si="4"/>
-        <v>6.5574028271889514E-3</v>
+        <v>2.6535904320903452E-5</v>
       </c>
       <c r="U24" s="129">
         <f t="shared" si="5"/>
-        <v>1.4080281929562412E-3</v>
+        <v>3.8656572010763356E-6</v>
       </c>
       <c r="V24" s="129">
         <f t="shared" si="6"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W24" s="129">
         <f t="shared" si="7"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X24" s="129">
         <f t="shared" si="8"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y24" s="129">
         <f t="shared" si="9"/>
-        <v>3.4621539051072632E-2</v>
+        <v>3.9047107105590395E-5</v>
       </c>
       <c r="Z24" s="129">
         <f t="shared" si="10"/>
-        <v>6.4163999152732796E-3</v>
+        <v>2.6534091329342642E-5</v>
       </c>
       <c r="AA24" s="135">
         <f t="shared" si="11"/>
-        <v>1.3845982964849576E-3</v>
+        <v>3.8654691904491773E-6</v>
       </c>
       <c r="AC24" s="158">
         <f t="shared" si="0"/>
@@ -9088,11 +9088,11 @@
       </c>
       <c r="AD24" s="159">
         <f t="shared" si="1"/>
-        <v>0.1851851851851852</v>
+        <v>0.17910447761194032</v>
       </c>
       <c r="AE24" s="160">
         <f t="shared" si="12"/>
-        <v>-2.1340109821626103</v>
+        <v>-1.1562157907434101</v>
       </c>
     </row>
     <row r="25" spans="1:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -9117,43 +9117,43 @@
       </c>
       <c r="R25" s="117">
         <f t="shared" si="2"/>
-        <v>0.2098765432098765</v>
+        <v>0.20398009950248752</v>
       </c>
       <c r="S25" s="129">
         <f t="shared" si="3"/>
-        <v>5.2228000126832846E-2</v>
+        <v>9.3870019314160969E-5</v>
       </c>
       <c r="T25" s="129">
         <f t="shared" si="4"/>
-        <v>9.6418285744227887E-3</v>
+        <v>6.3788158700430015E-5</v>
       </c>
       <c r="U25" s="129">
         <f t="shared" si="5"/>
-        <v>2.0703267470694882E-3</v>
+        <v>9.2924345837904392E-6</v>
       </c>
       <c r="V25" s="129">
         <f t="shared" si="6"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W25" s="129">
         <f t="shared" si="7"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X25" s="129">
         <f t="shared" si="8"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y25" s="129">
         <f t="shared" si="9"/>
-        <v>5.0307869269171697E-2</v>
+        <v>9.385346271504301E-5</v>
       </c>
       <c r="Z25" s="129">
         <f t="shared" si="10"/>
-        <v>9.3400331729721342E-3</v>
+        <v>6.3777683400257482E-5</v>
       </c>
       <c r="AA25" s="135">
         <f t="shared" si="11"/>
-        <v>2.0200647874235593E-3</v>
+        <v>9.2913482454850101E-6</v>
       </c>
       <c r="AC25" s="158">
         <f t="shared" si="0"/>
@@ -9161,11 +9161,11 @@
       </c>
       <c r="AD25" s="159">
         <f t="shared" si="1"/>
-        <v>0.2098765432098765</v>
+        <v>0.20398009950248752</v>
       </c>
       <c r="AE25" s="160">
         <f t="shared" si="12"/>
-        <v>-1.695629994580736</v>
+        <v>-0.95690260829654494</v>
       </c>
     </row>
     <row r="26" spans="1:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -9185,50 +9185,50 @@
         <v>55</v>
       </c>
       <c r="G26" s="142">
-        <v>1.75</v>
+        <v>1</v>
       </c>
       <c r="Q26" s="118">
         <v>0.19</v>
       </c>
       <c r="R26" s="117">
         <f t="shared" si="2"/>
-        <v>0.23456790123456789</v>
+        <v>0.22885572139303481</v>
       </c>
       <c r="S26" s="129">
         <f t="shared" si="3"/>
-        <v>7.4950331077162757E-2</v>
+        <v>2.0750203885895669E-4</v>
       </c>
       <c r="T26" s="129">
         <f t="shared" si="4"/>
-        <v>1.383660569210577E-2</v>
+        <v>1.4100532930646958E-4</v>
       </c>
       <c r="U26" s="129">
         <f t="shared" si="5"/>
-        <v>2.971043784060995E-3</v>
+        <v>2.0541160385263866E-5</v>
       </c>
       <c r="V26" s="129">
         <f t="shared" si="6"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W26" s="129">
         <f t="shared" si="7"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X26" s="129">
         <f t="shared" si="8"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y26" s="129">
         <f t="shared" si="9"/>
-        <v>7.1058269614329539E-2</v>
+        <v>2.0742115360761592E-4</v>
       </c>
       <c r="Z26" s="129">
         <f t="shared" si="10"/>
-        <v>1.3223438704391598E-2</v>
+        <v>1.409541527484854E-4</v>
       </c>
       <c r="AA26" s="135">
         <f t="shared" si="11"/>
-        <v>2.8686162465993508E-3</v>
+        <v>2.0535852829572074E-5</v>
       </c>
       <c r="AC26" s="158">
         <f t="shared" si="0"/>
@@ -9236,11 +9236,11 @@
       </c>
       <c r="AD26" s="159">
         <f t="shared" si="1"/>
-        <v>0.23456790123456789</v>
+        <v>0.22885572139303481</v>
       </c>
       <c r="AE26" s="160">
         <f t="shared" si="12"/>
-        <v>-1.3810808706842324</v>
+        <v>-0.80853529907938304</v>
       </c>
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.2">
@@ -9267,43 +9267,43 @@
       </c>
       <c r="R27" s="117">
         <f t="shared" si="2"/>
-        <v>0.25925925925925924</v>
+        <v>0.2537313432835821</v>
       </c>
       <c r="S27" s="129">
         <f t="shared" si="3"/>
-        <v>0.10531049791441752</v>
+        <v>4.2851699766808604E-4</v>
       </c>
       <c r="T27" s="129">
         <f t="shared" si="4"/>
-        <v>1.9441406247838581E-2</v>
+        <v>2.9119318876032337E-4</v>
       </c>
       <c r="U27" s="129">
         <f t="shared" si="5"/>
-        <v>4.1745259257478205E-3</v>
+        <v>4.2419999462727947E-5</v>
       </c>
       <c r="V27" s="129">
         <f t="shared" si="6"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W27" s="129">
         <f t="shared" si="7"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X27" s="129">
         <f t="shared" si="8"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y27" s="129">
         <f t="shared" si="9"/>
-        <v>9.778499721024439E-2</v>
+        <v>4.2817218720759057E-4</v>
       </c>
       <c r="Z27" s="129">
         <f t="shared" si="10"/>
-        <v>1.8252224407377643E-2</v>
+        <v>2.9097501898330599E-4</v>
       </c>
       <c r="AA27" s="135">
         <f t="shared" si="11"/>
-        <v>3.9750961388852991E-3</v>
+        <v>4.2397370407462963E-5</v>
       </c>
       <c r="AC27" s="158">
         <f t="shared" si="0"/>
@@ -9311,11 +9311,11 @@
       </c>
       <c r="AD27" s="159">
         <f t="shared" si="1"/>
-        <v>0.25925925925925924</v>
+        <v>0.2537313432835821</v>
       </c>
       <c r="AE27" s="160">
         <f t="shared" si="12"/>
-        <v>-1.1471658159994846</v>
+        <v>-0.6943676187122968</v>
       </c>
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.2">
@@ -9335,50 +9335,50 @@
         <v>57</v>
       </c>
       <c r="G28" s="143">
-        <v>6</v>
+        <v>2.4</v>
       </c>
       <c r="Q28" s="118">
         <v>0.21</v>
       </c>
       <c r="R28" s="117">
         <f t="shared" si="2"/>
-        <v>0.2839506172839506</v>
+        <v>0.27860696517412931</v>
       </c>
       <c r="S28" s="129">
         <f t="shared" si="3"/>
-        <v>0.14524568383104364</v>
+        <v>8.3634458711355345E-4</v>
       </c>
       <c r="T28" s="129">
         <f t="shared" si="4"/>
-        <v>2.6813854278794076E-2</v>
+        <v>5.6832715749741949E-4</v>
       </c>
       <c r="U28" s="129">
         <f t="shared" si="5"/>
-        <v>5.7575634410959604E-3</v>
+        <v>8.2791901205963724E-5</v>
       </c>
       <c r="V28" s="129">
         <f t="shared" si="6"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W28" s="129">
         <f t="shared" si="7"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X28" s="129">
         <f t="shared" si="8"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y28" s="129">
         <f t="shared" si="9"/>
-        <v>0.13130813576865469</v>
+        <v>8.350321383233855E-4</v>
       </c>
       <c r="Z28" s="129">
         <f t="shared" si="10"/>
-        <v>2.4603037429826512E-2</v>
+        <v>5.6749669616257682E-4</v>
       </c>
       <c r="AA28" s="135">
         <f t="shared" si="11"/>
-        <v>5.3849523141258904E-3</v>
+        <v>8.2705746226506926E-5</v>
       </c>
       <c r="AC28" s="158">
         <f t="shared" si="0"/>
@@ -9386,11 +9386,11 @@
       </c>
       <c r="AD28" s="159">
         <f t="shared" si="1"/>
-        <v>0.2839506172839506</v>
+        <v>0.27860696517412931</v>
       </c>
       <c r="AE28" s="160">
         <f t="shared" si="12"/>
-        <v>-0.968101443057651</v>
+        <v>-0.60413784470221177</v>
       </c>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.2">
@@ -9411,7 +9411,7 @@
         <v>66</v>
       </c>
       <c r="G29" s="144">
-        <v>0.97</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="I29" s="15" t="s">
         <v>137</v>
@@ -9422,43 +9422,43 @@
       </c>
       <c r="R29" s="117">
         <f t="shared" si="2"/>
-        <v>0.30864197530864196</v>
+        <v>0.30348258706467657</v>
       </c>
       <c r="S29" s="129">
         <f t="shared" si="3"/>
-        <v>0.19704739054208348</v>
+        <v>1.5562218972464804E-3</v>
       </c>
       <c r="T29" s="129">
         <f t="shared" si="4"/>
-        <v>3.6376984683126112E-2</v>
+        <v>1.0575104818335477E-3</v>
       </c>
       <c r="U29" s="129">
         <f t="shared" si="5"/>
-        <v>7.8109918451564767E-3</v>
+        <v>1.5405440718646585E-4</v>
       </c>
       <c r="V29" s="129">
         <f t="shared" si="6"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W29" s="129">
         <f t="shared" si="7"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X29" s="129">
         <f t="shared" si="8"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y29" s="129">
         <f t="shared" si="9"/>
-        <v>0.17224423734157626</v>
+        <v>1.5516838533916506E-3</v>
       </c>
       <c r="Z29" s="129">
         <f t="shared" si="10"/>
-        <v>3.242421945137737E-2</v>
+        <v>1.0546387355389163E-3</v>
       </c>
       <c r="AA29" s="135">
         <f t="shared" si="11"/>
-        <v>7.1406742324876607E-3</v>
+        <v>1.5375637436124465E-4</v>
       </c>
       <c r="AC29" s="158">
         <f t="shared" si="0"/>
@@ -9466,11 +9466,11 @@
       </c>
       <c r="AD29" s="159">
         <f t="shared" si="1"/>
-        <v>0.30864197530864196</v>
+        <v>0.30348258706467657</v>
       </c>
       <c r="AE29" s="160">
         <f t="shared" si="12"/>
-        <v>-0.82769874290523227</v>
+        <v>-0.531238660865896</v>
       </c>
     </row>
     <row r="30" spans="1:31" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -9507,43 +9507,43 @@
       </c>
       <c r="R30" s="117">
         <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
+        <v>0.32835820895522388</v>
       </c>
       <c r="S30" s="129">
         <f t="shared" si="3"/>
-        <v>0.26340495830866423</v>
+        <v>2.7795617716452796E-3</v>
       </c>
       <c r="T30" s="129">
         <f t="shared" si="4"/>
-        <v>4.8627277466063906E-2</v>
+        <v>1.8888152863159157E-3</v>
       </c>
       <c r="U30" s="129">
         <f t="shared" si="5"/>
-        <v>1.0441417040147742E-2</v>
+        <v>2.7515596697786065E-4</v>
       </c>
       <c r="V30" s="129">
         <f t="shared" si="6"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W30" s="129">
         <f t="shared" si="7"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X30" s="129">
         <f t="shared" si="8"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y30" s="129">
         <f t="shared" si="9"/>
-        <v>0.22088591565340021</v>
+        <v>2.7651178904414169E-3</v>
       </c>
       <c r="Z30" s="129">
         <f t="shared" si="10"/>
-        <v>4.1813320236684465E-2</v>
+        <v>1.8796735311667903E-3</v>
       </c>
       <c r="AA30" s="135">
         <f t="shared" si="11"/>
-        <v>9.2772532660602303E-3</v>
+        <v>2.7420664452517302E-4</v>
       </c>
       <c r="AC30" s="158">
         <f t="shared" si="0"/>
@@ -9551,11 +9551,11 @@
       </c>
       <c r="AD30" s="159">
         <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
+        <v>0.32835820895522388</v>
       </c>
       <c r="AE30" s="160">
         <f t="shared" si="12"/>
-        <v>-0.71536206370457789</v>
+        <v>-0.47124061861923627</v>
       </c>
     </row>
     <row r="31" spans="1:31" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -9586,50 +9586,50 @@
       </c>
       <c r="O31" s="151">
         <f>1000*(sc_vg-rc_vg)*((depth1*(1-RFC_1/100)+(depth2-depth1)*(1-RFC_2/100))+((depth3-depth2)*(1-RFC_3/100)))</f>
-        <v>141.75000000000006</v>
+        <v>171.25199999999995</v>
       </c>
       <c r="Q31" s="118">
         <v>0.24</v>
       </c>
       <c r="R31" s="117">
         <f t="shared" si="2"/>
-        <v>0.35802469135802462</v>
+        <v>0.35323383084577109</v>
       </c>
       <c r="S31" s="129">
         <f t="shared" si="3"/>
-        <v>0.34745237470956025</v>
+        <v>4.7911668007790953E-3</v>
       </c>
       <c r="T31" s="129">
         <f t="shared" si="4"/>
-        <v>6.4143299122888395E-2</v>
+        <v>3.255775491272575E-3</v>
       </c>
       <c r="U31" s="129">
         <f t="shared" si="5"/>
-        <v>1.3773070823066846E-2</v>
+        <v>4.7428992133542546E-4</v>
       </c>
       <c r="V31" s="129">
         <f t="shared" si="6"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W31" s="129">
         <f t="shared" si="7"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X31" s="129">
         <f t="shared" si="8"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y31" s="129">
         <f t="shared" si="9"/>
-        <v>0.27709424360789786</v>
+        <v>4.7484121245796578E-3</v>
       </c>
       <c r="Z31" s="129">
         <f t="shared" si="10"/>
-        <v>5.279461056652044E-2</v>
+        <v>3.2287084398008193E-3</v>
       </c>
       <c r="AA31" s="135">
         <f t="shared" si="11"/>
-        <v>1.1817043794481364E-2</v>
+        <v>4.7147633247673719E-4</v>
       </c>
       <c r="AC31" s="158">
         <f t="shared" si="0"/>
@@ -9637,11 +9637,11 @@
       </c>
       <c r="AD31" s="159">
         <f t="shared" si="1"/>
-        <v>0.35802469135802462</v>
+        <v>0.35323383084577109</v>
       </c>
       <c r="AE31" s="160">
         <f t="shared" si="12"/>
-        <v>-0.62391201418098852</v>
+        <v>-0.42107299954196131</v>
       </c>
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.2">
@@ -9657,43 +9657,43 @@
       </c>
       <c r="R32" s="117">
         <f t="shared" si="2"/>
-        <v>0.38271604938271603</v>
+        <v>0.37810945273631835</v>
       </c>
       <c r="S32" s="129">
         <f t="shared" si="3"/>
-        <v>0.45281856168104484</v>
+        <v>8.0049754635572058E-3</v>
       </c>
       <c r="T32" s="129">
         <f t="shared" si="4"/>
-        <v>8.3594986146180897E-2</v>
+        <v>5.439677641414997E-3</v>
       </c>
       <c r="U32" s="129">
         <f t="shared" si="5"/>
-        <v>1.7949804272443467E-2</v>
+        <v>7.9243310466360227E-4</v>
       </c>
       <c r="V32" s="129">
         <f t="shared" si="6"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W32" s="129">
         <f t="shared" si="7"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X32" s="129">
         <f t="shared" si="8"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y32" s="129">
         <f t="shared" si="9"/>
-        <v>0.34023115666120018</v>
+        <v>7.8863359911596383E-3</v>
       </c>
       <c r="Z32" s="129">
         <f t="shared" si="10"/>
-        <v>6.5301114844674199E-2</v>
+        <v>5.3645390165769141E-3</v>
       </c>
       <c r="AA32" s="135">
         <f t="shared" si="11"/>
-        <v>1.4764724639180103E-2</v>
+        <v>7.8461010430664311E-4</v>
       </c>
       <c r="AC32" s="158">
         <f t="shared" si="0"/>
@@ -9701,11 +9701,11 @@
       </c>
       <c r="AD32" s="159">
         <f t="shared" si="1"/>
-        <v>0.38271604938271603</v>
+        <v>0.37810945273631835</v>
       </c>
       <c r="AE32" s="160">
         <f t="shared" si="12"/>
-        <v>-0.54833885676102501</v>
+        <v>-0.37854580116417574</v>
       </c>
     </row>
     <row r="33" spans="1:31" x14ac:dyDescent="0.2">
@@ -9729,43 +9729,43 @@
       </c>
       <c r="R33" s="117">
         <f t="shared" si="2"/>
-        <v>0.40740740740740738</v>
+        <v>0.40298507462686567</v>
       </c>
       <c r="S33" s="129">
         <f t="shared" si="3"/>
-        <v>0.58368135024671663</v>
+        <v>1.3010319402707046E-2</v>
       </c>
       <c r="T33" s="129">
         <f t="shared" si="4"/>
-        <v>0.10775360931875183</v>
+        <v>8.8409944396161833E-3</v>
       </c>
       <c r="U33" s="129">
         <f t="shared" si="5"/>
-        <v>2.313722731574732E-2</v>
+        <v>1.2879249716489245E-3</v>
       </c>
       <c r="V33" s="129">
         <f t="shared" si="6"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W33" s="129">
         <f t="shared" si="7"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X33" s="129">
         <f t="shared" si="8"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y33" s="129">
         <f t="shared" si="9"/>
-        <v>0.409156639513995</v>
+        <v>1.2699806962644774E-2</v>
       </c>
       <c r="Z33" s="129">
         <f t="shared" si="10"/>
-        <v>7.9166121704973627E-2</v>
+        <v>8.6442129495175567E-3</v>
       </c>
       <c r="AA33" s="135">
         <f t="shared" si="11"/>
-        <v>1.8103324059064261E-2</v>
+        <v>1.2673870416520067E-3</v>
       </c>
       <c r="AC33" s="158">
         <f t="shared" si="0"/>
@@ -9773,11 +9773,11 @@
       </c>
       <c r="AD33" s="159">
         <f t="shared" si="1"/>
-        <v>0.40740740740740738</v>
+        <v>0.40298507462686567</v>
       </c>
       <c r="AE33" s="160">
         <f t="shared" si="12"/>
-        <v>-0.48505736422050805</v>
+        <v>-0.34205869081005458</v>
       </c>
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.2">
@@ -9793,43 +9793,43 @@
       </c>
       <c r="R34" s="117">
         <f t="shared" si="2"/>
-        <v>0.4320987654320988</v>
+        <v>0.42786069651741293</v>
       </c>
       <c r="S34" s="129">
         <f t="shared" si="3"/>
-        <v>0.74482537467739096</v>
+        <v>2.0630998228586515E-2</v>
       </c>
       <c r="T34" s="129">
         <f t="shared" si="4"/>
-        <v>0.13750246157386459</v>
+        <v>1.40195282665169E-2</v>
       </c>
       <c r="U34" s="129">
         <f t="shared" si="5"/>
-        <v>2.9525003663665384E-2</v>
+        <v>2.0423155639908929E-3</v>
       </c>
       <c r="V34" s="129">
         <f t="shared" si="6"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W34" s="129">
         <f t="shared" si="7"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X34" s="129">
         <f t="shared" si="8"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y34" s="129">
         <f t="shared" si="9"/>
-        <v>0.48230315270739788</v>
+        <v>1.9860956384922822E-2</v>
       </c>
       <c r="Z34" s="129">
         <f t="shared" si="10"/>
-        <v>9.4127999941968729E-2</v>
+        <v>1.353107461586704E-2</v>
       </c>
       <c r="AA34" s="135">
         <f t="shared" si="11"/>
-        <v>2.1792340901502321E-2</v>
+        <v>1.9911493220268412E-3</v>
       </c>
       <c r="AC34" s="158">
         <f t="shared" si="0"/>
@@ -9837,11 +9837,11 @@
       </c>
       <c r="AD34" s="159">
         <f t="shared" si="1"/>
-        <v>0.4320987654320988</v>
+        <v>0.42786069651741293</v>
       </c>
       <c r="AE34" s="160">
         <f t="shared" si="12"/>
-        <v>-0.43144475917474873</v>
+        <v>-0.31041727102801847</v>
       </c>
     </row>
     <row r="35" spans="1:31" x14ac:dyDescent="0.2">
@@ -9857,43 +9857,43 @@
       </c>
       <c r="R35" s="117">
         <f t="shared" si="2"/>
-        <v>0.45679012345679015</v>
+        <v>0.45273631840796025</v>
       </c>
       <c r="S35" s="129">
         <f t="shared" si="3"/>
-        <v>0.94170414265257341</v>
+        <v>3.1999843965140773E-2</v>
       </c>
       <c r="T35" s="129">
         <f t="shared" si="4"/>
-        <v>0.17384831678850846</v>
+        <v>2.1745080486304594E-2</v>
       </c>
       <c r="U35" s="129">
         <f t="shared" si="5"/>
-        <v>3.7329311281787181E-2</v>
+        <v>3.1677468366378991E-3</v>
       </c>
       <c r="V35" s="129">
         <f t="shared" si="6"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W35" s="129">
         <f t="shared" si="7"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X35" s="129">
         <f t="shared" si="8"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y35" s="129">
         <f t="shared" si="9"/>
-        <v>0.55782005427798043</v>
+        <v>3.0184630713840487E-2</v>
       </c>
       <c r="Z35" s="129">
         <f t="shared" si="10"/>
-        <v>0.10984936746062583</v>
+        <v>2.059210660879774E-2</v>
       </c>
       <c r="AA35" s="135">
         <f t="shared" si="11"/>
-        <v>2.5768756704014472E-2</v>
+        <v>3.0463285635928929E-3</v>
       </c>
       <c r="AC35" s="158">
         <f t="shared" si="0"/>
@@ -9901,11 +9901,11 @@
       </c>
       <c r="AD35" s="159">
         <f t="shared" si="1"/>
-        <v>0.45679012345679015</v>
+        <v>0.45273631840796025</v>
       </c>
       <c r="AE35" s="160">
         <f t="shared" si="12"/>
-        <v>-0.38554494183855909</v>
+        <v>-0.2827134117094004</v>
       </c>
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.2">
@@ -9921,43 +9921,43 @@
       </c>
       <c r="R36" s="117">
         <f t="shared" si="2"/>
-        <v>0.4814814814814814</v>
+        <v>0.4776119402985074</v>
       </c>
       <c r="S36" s="129">
         <f t="shared" si="3"/>
-        <v>1.1805065655457774</v>
+        <v>4.8651855079305584E-2</v>
       </c>
       <c r="T36" s="129">
         <f t="shared" si="4"/>
-        <v>0.21793371196162661</v>
+        <v>3.3060739472979897E-2</v>
       </c>
       <c r="U36" s="129">
         <f t="shared" si="5"/>
-        <v>4.679547966235275E-2</v>
+        <v>4.8161722348372647E-3</v>
       </c>
       <c r="V36" s="129">
         <f t="shared" si="6"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W36" s="129">
         <f t="shared" si="7"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X36" s="129">
         <f t="shared" si="8"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y36" s="129">
         <f t="shared" si="9"/>
-        <v>0.63376089545272862</v>
+        <v>4.4576209022731829E-2</v>
       </c>
       <c r="Z36" s="129">
         <f t="shared" si="10"/>
-        <v>0.1259479864149449</v>
+        <v>3.0467145434686337E-2</v>
       </c>
       <c r="AA36" s="135">
         <f t="shared" si="11"/>
-        <v>2.9951177336478972E-2</v>
+        <v>4.5409965687351565E-3</v>
       </c>
       <c r="AC36" s="158">
         <f t="shared" si="0"/>
@@ -9965,7 +9965,7 @@
       </c>
       <c r="AD36" s="159">
         <f t="shared" si="1"/>
-        <v>0.4814814814814814</v>
+        <v>0.4776119402985074</v>
       </c>
       <c r="AE36" s="160">
         <f>MAX(0,(-1*((((1/AD36)^(1/m))-1)^(1/n))/alpha/10000))</f>
@@ -9985,43 +9985,43 @@
       </c>
       <c r="R37" s="117">
         <f t="shared" si="2"/>
-        <v>0.50617283950617276</v>
+        <v>0.50248756218905466</v>
       </c>
       <c r="S37" s="129">
         <f t="shared" si="3"/>
-        <v>1.4682282635072366</v>
+        <v>7.2639434251915228E-2</v>
       </c>
       <c r="T37" s="129">
         <f t="shared" si="4"/>
-        <v>0.27105011086928787</v>
+        <v>4.9361188948553007E-2</v>
       </c>
       <c r="U37" s="129">
         <f t="shared" si="5"/>
-        <v>5.8200816369775706E-2</v>
+        <v>7.1907643773930774E-3</v>
       </c>
       <c r="V37" s="129">
         <f t="shared" si="6"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W37" s="129">
         <f t="shared" si="7"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X37" s="129">
         <f t="shared" si="8"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y37" s="129">
         <f t="shared" si="9"/>
-        <v>0.70827490266880677</v>
+        <v>6.391443615834369E-2</v>
       </c>
       <c r="Z37" s="129">
         <f t="shared" si="10"/>
-        <v>0.14203357119272955</v>
+        <v>4.3794887784780495E-2</v>
       </c>
       <c r="AA37" s="135">
         <f t="shared" si="11"/>
-        <v>3.4246606636992194E-2</v>
+        <v>6.5941537687377932E-3</v>
       </c>
       <c r="AC37" s="158">
         <f t="shared" si="0"/>
@@ -10029,11 +10029,11 @@
       </c>
       <c r="AD37" s="159">
         <f t="shared" si="1"/>
-        <v>0.50617283950617276</v>
+        <v>0.50248756218905466</v>
       </c>
       <c r="AE37" s="160">
         <f t="shared" ref="AE37:AE67" si="13">(-1 * ((((1 / AD37)^(1 / m)) - 1)^(1 / n)) / alpha / 10000)</f>
-        <v>-0.3112880463053686</v>
+        <v>-0.23646180652550242</v>
       </c>
     </row>
     <row r="38" spans="1:31" x14ac:dyDescent="0.2">
@@ -10049,43 +10049,43 @@
       </c>
       <c r="R38" s="117">
         <f t="shared" si="2"/>
-        <v>0.53086419753086411</v>
+        <v>0.52736318407960192</v>
       </c>
       <c r="S38" s="129">
         <f t="shared" si="3"/>
-        <v>1.812747993913171</v>
+        <v>0.10667376948758543</v>
       </c>
       <c r="T38" s="129">
         <f t="shared" si="4"/>
-        <v>0.33465201354627272</v>
+        <v>7.248878168943422E-2</v>
       </c>
       <c r="U38" s="129">
         <f t="shared" si="5"/>
-        <v>7.1857636677282052E-2</v>
+        <v>1.0559910736272639E-2</v>
       </c>
       <c r="V38" s="129">
         <f t="shared" si="6"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W38" s="129">
         <f t="shared" si="7"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X38" s="129">
         <f t="shared" si="8"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y38" s="129">
         <f t="shared" si="9"/>
-        <v>0.77976550527831168</v>
+        <v>8.8859930015298863E-2</v>
       </c>
       <c r="Z38" s="129">
         <f t="shared" si="10"/>
-        <v>0.15774331273883432</v>
+        <v>6.1086899400835649E-2</v>
       </c>
       <c r="AA38" s="135">
         <f t="shared" si="11"/>
-        <v>3.8558692872341267E-2</v>
+        <v>9.3214038786069136E-3</v>
       </c>
       <c r="AC38" s="158">
         <f t="shared" si="0"/>
@@ -10093,11 +10093,11 @@
       </c>
       <c r="AD38" s="159">
         <f t="shared" si="1"/>
-        <v>0.53086419753086411</v>
+        <v>0.52736318407960192</v>
       </c>
       <c r="AE38" s="160">
         <f t="shared" si="13"/>
-        <v>-0.28089442929918113</v>
+        <v>-0.21692546239434651</v>
       </c>
     </row>
     <row r="39" spans="1:31" x14ac:dyDescent="0.2">
@@ -10113,43 +10113,43 @@
       </c>
       <c r="R39" s="117">
         <f t="shared" si="2"/>
-        <v>0.55555555555555558</v>
+        <v>0.55223880597014918</v>
       </c>
       <c r="S39" s="129">
         <f t="shared" si="3"/>
-        <v>2.2229095893939594</v>
+        <v>0.15429696029076861</v>
       </c>
       <c r="T39" s="129">
         <f t="shared" si="4"/>
-        <v>0.41037208289286298</v>
+        <v>0.10485050564527486</v>
       </c>
       <c r="U39" s="129">
         <f t="shared" si="5"/>
-        <v>8.8116511604187417E-2</v>
+        <v>1.5274252849369344E-2</v>
       </c>
       <c r="V39" s="129">
         <f t="shared" si="6"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W39" s="129">
         <f t="shared" si="7"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X39" s="129">
         <f t="shared" si="8"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y39" s="129">
         <f t="shared" si="9"/>
-        <v>0.84699176825559819</v>
+        <v>0.11961293816739084</v>
       </c>
       <c r="Z39" s="129">
         <f t="shared" si="10"/>
-        <v>0.17276984062906914</v>
+        <v>8.2560890575623463E-2</v>
       </c>
       <c r="AA39" s="135">
         <f t="shared" si="11"/>
-        <v>4.2795954552460234E-2</v>
+        <v>1.2811994769166906E-2</v>
       </c>
       <c r="AC39" s="158">
         <f t="shared" si="0"/>
@@ -10157,11 +10157,11 @@
       </c>
       <c r="AD39" s="159">
         <f t="shared" si="1"/>
-        <v>0.55555555555555558</v>
+        <v>0.55223880597014918</v>
       </c>
       <c r="AE39" s="160">
         <f t="shared" si="13"/>
-        <v>-0.25398636654803403</v>
+        <v>-0.19928354534487142</v>
       </c>
     </row>
     <row r="40" spans="1:31" x14ac:dyDescent="0.2">
@@ -10177,43 +10177,43 @@
       </c>
       <c r="R40" s="117">
         <f t="shared" ref="R40:R66" si="14">MAX((Q40-rc_vg)/(sc_vg-rc_vg),0)</f>
-        <v>0.58024691358024694</v>
+        <v>0.57711442786069655</v>
       </c>
       <c r="S40" s="129">
         <f t="shared" ref="S40:S67" si="15">Bgc_1*Ksat*R40^I*(1-(1-Q40^(1/m))^m)^2</f>
-        <v>2.7086098335157511</v>
+        <v>0.22009011565144446</v>
       </c>
       <c r="T40" s="129">
         <f t="shared" ref="T40:T67" si="16">Bgc_2*Ksat*R40^I*(1-(1-Q40^(1/m))^m)^2</f>
-        <v>0.5000373674338201</v>
+        <v>0.1495593942362429</v>
       </c>
       <c r="U40" s="129">
         <f t="shared" ref="U40:U67" si="17">Bgc_3*Ksat*R40^I*(1-(1-Q40^(1/m))^m)^2</f>
-        <v>0.10736975132275949</v>
+        <v>2.1787286475197214E-2</v>
       </c>
       <c r="V40" s="129">
         <f t="shared" ref="V40:V67" si="18">kroot1</f>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W40" s="129">
         <f t="shared" ref="W40:W67" si="19">kroot2</f>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X40" s="129">
         <f t="shared" ref="X40:X67" si="20">kroot3</f>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y40" s="129">
         <f t="shared" ref="Y40:Y67" si="21">1/((1/kroot1)+(1/S40))</f>
-        <v>0.90910640943844057</v>
+        <v>0.15569330045970042</v>
       </c>
       <c r="Z40" s="129">
         <f t="shared" ref="Z40:Z67" si="22">1/((1/kroot2)+(1/T40))</f>
-        <v>0.18687799351957696</v>
+        <v>0.10797747467631082</v>
       </c>
       <c r="AA40" s="135">
         <f t="shared" ref="AA40:AA67" si="23">1/((1/kroot3)+(1/U40))</f>
-        <v>4.6878602680413779E-2</v>
+        <v>1.7099706900215877E-2</v>
       </c>
       <c r="AC40" s="158">
         <f t="shared" si="0"/>
@@ -10221,11 +10221,11 @@
       </c>
       <c r="AD40" s="159">
         <f t="shared" si="1"/>
-        <v>0.58024691358024694</v>
+        <v>0.57711442786069655</v>
       </c>
       <c r="AE40" s="160">
         <f t="shared" si="13"/>
-        <v>-0.22999826025010989</v>
+        <v>-0.18324882767461098</v>
       </c>
     </row>
     <row r="41" spans="1:31" x14ac:dyDescent="0.2">
@@ -10241,43 +10241,43 @@
       </c>
       <c r="R41" s="117">
         <f t="shared" si="14"/>
-        <v>0.60493827160493829</v>
+        <v>0.60199004975124382</v>
       </c>
       <c r="S41" s="129">
         <f t="shared" si="15"/>
-        <v>3.2808927488128257</v>
+        <v>0.30992334552126366</v>
       </c>
       <c r="T41" s="129">
         <f t="shared" si="16"/>
-        <v>0.60568670786358014</v>
+        <v>0.21060440483041645</v>
       </c>
       <c r="U41" s="129">
         <f t="shared" si="17"/>
-        <v>0.13005514275174745</v>
+        <v>3.06801088919278E-2</v>
       </c>
       <c r="V41" s="129">
         <f t="shared" si="18"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W41" s="129">
         <f t="shared" si="19"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X41" s="129">
         <f t="shared" si="20"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y41" s="129">
         <f t="shared" si="21"/>
-        <v>0.96563940463757103</v>
+        <v>0.19585205581835749</v>
       </c>
       <c r="Z41" s="129">
         <f t="shared" si="22"/>
-        <v>0.1999099255766574</v>
+        <v>0.13655376676496517</v>
       </c>
       <c r="AA41" s="135">
         <f t="shared" si="23"/>
-        <v>5.0743056110136957E-2</v>
+        <v>2.2135345452348645E-2</v>
       </c>
       <c r="AC41" s="158">
         <f t="shared" si="0"/>
@@ -10285,11 +10285,11 @@
       </c>
       <c r="AD41" s="159">
         <f t="shared" si="1"/>
-        <v>0.60493827160493829</v>
+        <v>0.60199004975124382</v>
       </c>
       <c r="AE41" s="160">
         <f t="shared" si="13"/>
-        <v>-0.20847238432764578</v>
+        <v>-0.16858466505445768</v>
       </c>
     </row>
     <row r="42" spans="1:31" x14ac:dyDescent="0.2">
@@ -10305,43 +10305,43 @@
       </c>
       <c r="R42" s="117">
         <f t="shared" si="14"/>
-        <v>0.62962962962962965</v>
+        <v>0.62686567164179097</v>
       </c>
       <c r="S42" s="129">
         <f t="shared" si="15"/>
-        <v>3.9520508238798979</v>
+        <v>0.43125434032024884</v>
       </c>
       <c r="T42" s="129">
         <f t="shared" si="16"/>
-        <v>0.72958942461362519</v>
+        <v>0.29305331458952166</v>
       </c>
       <c r="U42" s="129">
         <f t="shared" si="17"/>
-        <v>0.15665996221541953</v>
+        <v>4.2690976050508464E-2</v>
       </c>
       <c r="V42" s="129">
         <f t="shared" si="18"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W42" s="129">
         <f t="shared" si="19"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X42" s="129">
         <f t="shared" si="20"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y42" s="129">
         <f t="shared" si="21"/>
-        <v>1.0164447024421746</v>
+        <v>0.23820255551380842</v>
       </c>
       <c r="Z42" s="129">
         <f t="shared" si="22"/>
-        <v>0.2117805824500899</v>
+        <v>0.16702207910636874</v>
       </c>
       <c r="AA42" s="135">
         <f t="shared" si="23"/>
-        <v>5.4343881331365744E-2</v>
+        <v>2.7772870035292559E-2</v>
       </c>
       <c r="AC42" s="158">
         <f t="shared" si="0"/>
@@ -10349,11 +10349,11 @@
       </c>
       <c r="AD42" s="159">
         <f t="shared" si="1"/>
-        <v>0.62962962962962965</v>
+        <v>0.62686567164179097</v>
       </c>
       <c r="AE42" s="160">
         <f t="shared" si="13"/>
-        <v>-0.18903439682681863</v>
+        <v>-0.15509389831232107</v>
       </c>
     </row>
     <row r="43" spans="1:31" x14ac:dyDescent="0.2">
@@ -10369,43 +10369,43 @@
       </c>
       <c r="R43" s="117">
         <f t="shared" si="14"/>
-        <v>0.65432098765432101</v>
+        <v>0.65174129353233834</v>
       </c>
       <c r="S43" s="129">
         <f t="shared" si="15"/>
-        <v>4.7357337643565272</v>
+        <v>0.59348309291227175</v>
       </c>
       <c r="T43" s="129">
         <f t="shared" si="16"/>
-        <v>0.87426539440809503</v>
+        <v>0.40329376720389154</v>
       </c>
       <c r="U43" s="129">
         <f t="shared" si="17"/>
-        <v>0.18772528635095465</v>
+        <v>5.8750417415126134E-2</v>
       </c>
       <c r="V43" s="129">
         <f t="shared" si="18"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W43" s="129">
         <f t="shared" si="19"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X43" s="129">
         <f t="shared" si="20"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y43" s="129">
         <f t="shared" si="21"/>
-        <v>1.0616289552302225</v>
+        <v>0.28056326459317776</v>
       </c>
       <c r="Z43" s="129">
         <f t="shared" si="22"/>
-        <v>0.22246684959231097</v>
+        <v>0.19784483292033972</v>
       </c>
       <c r="AA43" s="135">
         <f t="shared" si="23"/>
-        <v>5.7653447202308299E-2</v>
+        <v>3.3779945698134785E-2</v>
       </c>
       <c r="AC43" s="158">
         <f t="shared" si="0"/>
@@ -10413,11 +10413,11 @@
       </c>
       <c r="AD43" s="159">
         <f t="shared" si="1"/>
-        <v>0.65432098765432101</v>
+        <v>0.65174129353233834</v>
       </c>
       <c r="AE43" s="160">
         <f t="shared" si="13"/>
-        <v>-0.17137497238380819</v>
+        <v>-0.14261037001108476</v>
       </c>
     </row>
     <row r="44" spans="1:31" x14ac:dyDescent="0.2">
@@ -10433,43 +10433,43 @@
       </c>
       <c r="R44" s="117">
         <f t="shared" si="14"/>
-        <v>0.67901234567901236</v>
+        <v>0.6766169154228856</v>
       </c>
       <c r="S44" s="129">
         <f t="shared" si="15"/>
-        <v>5.6470654177066297</v>
+        <v>0.80837127483281701</v>
       </c>
       <c r="T44" s="129">
         <f t="shared" si="16"/>
-        <v>1.0425066357864452</v>
+        <v>0.54931825458914951</v>
       </c>
       <c r="U44" s="129">
         <f t="shared" si="17"/>
-        <v>0.22385062702645242</v>
+        <v>8.0022751094353251E-2</v>
       </c>
       <c r="V44" s="129">
         <f t="shared" si="18"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W44" s="129">
         <f t="shared" si="19"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X44" s="129">
         <f t="shared" si="20"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y44" s="129">
         <f t="shared" si="21"/>
-        <v>1.1014777167099887</v>
+        <v>0.32088864396462774</v>
       </c>
       <c r="Z44" s="129">
         <f t="shared" si="22"/>
-        <v>0.23199375714472595</v>
+        <v>0.22751459964280202</v>
       </c>
       <c r="AA44" s="135">
         <f t="shared" si="23"/>
-        <v>6.0659925060580294E-2</v>
+        <v>3.9874548847800888E-2</v>
       </c>
       <c r="AC44" s="158">
         <f t="shared" si="0"/>
@@ -10477,11 +10477,11 @@
       </c>
       <c r="AD44" s="159">
         <f t="shared" si="1"/>
-        <v>0.67901234567901236</v>
+        <v>0.6766169154228856</v>
       </c>
       <c r="AE44" s="160">
         <f t="shared" si="13"/>
-        <v>-0.15523581232288602</v>
+        <v>-0.13099231557230459</v>
       </c>
     </row>
     <row r="45" spans="1:31" x14ac:dyDescent="0.2">
@@ -10497,43 +10497,43 @@
       </c>
       <c r="R45" s="117">
         <f t="shared" si="14"/>
-        <v>0.70370370370370372</v>
+        <v>0.70149253731343286</v>
       </c>
       <c r="S45" s="129">
         <f t="shared" si="15"/>
-        <v>6.7027695946832884</v>
+        <v>1.0905358452516105</v>
       </c>
       <c r="T45" s="129">
         <f t="shared" si="16"/>
-        <v>1.2374005370461543</v>
+        <v>0.74105954247868366</v>
       </c>
       <c r="U45" s="129">
         <f t="shared" si="17"/>
-        <v>0.26569891892505126</v>
+        <v>0.10795494746159555</v>
       </c>
       <c r="V45" s="129">
         <f t="shared" si="18"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W45" s="129">
         <f t="shared" si="19"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X45" s="129">
         <f t="shared" si="20"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y45" s="129">
         <f t="shared" si="21"/>
-        <v>1.1363891703321813</v>
+        <v>0.35761913741145962</v>
       </c>
       <c r="Z45" s="129">
         <f t="shared" si="22"/>
-        <v>0.24042044317075323</v>
+        <v>0.25482230548177232</v>
       </c>
       <c r="AA45" s="135">
         <f t="shared" si="23"/>
-        <v>6.3364360115822638E-2</v>
+        <v>4.5776372290832118E-2</v>
       </c>
       <c r="AC45" s="158">
         <f t="shared" si="0"/>
@@ -10541,11 +10541,11 @@
       </c>
       <c r="AD45" s="159">
         <f t="shared" si="1"/>
-        <v>0.70370370370370372</v>
+        <v>0.70149253731343286</v>
       </c>
       <c r="AE45" s="160">
         <f t="shared" si="13"/>
-        <v>-0.14039880681261674</v>
+        <v>-0.12011709268749189</v>
       </c>
     </row>
     <row r="46" spans="1:31" x14ac:dyDescent="0.2">
@@ -10561,43 +10561,43 @@
       </c>
       <c r="R46" s="117">
         <f t="shared" si="14"/>
-        <v>0.72839506172839508</v>
+        <v>0.72636815920398012</v>
       </c>
       <c r="S46" s="129">
         <f t="shared" si="15"/>
-        <v>7.9213055923924749</v>
+        <v>1.4580276608530143</v>
       </c>
       <c r="T46" s="129">
         <f t="shared" si="16"/>
-        <v>1.4623548752008533</v>
+        <v>0.9907838572914659</v>
       </c>
       <c r="U46" s="129">
         <f t="shared" si="17"/>
-        <v>0.31400189170206605</v>
+        <v>0.1443339072349559</v>
       </c>
       <c r="V46" s="129">
         <f t="shared" si="18"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W46" s="129">
         <f t="shared" si="19"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X46" s="129">
         <f t="shared" si="20"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y46" s="129">
         <f t="shared" si="21"/>
-        <v>1.166820321044034</v>
+        <v>0.38984096647168703</v>
       </c>
       <c r="Z46" s="129">
         <f t="shared" si="22"/>
-        <v>0.24782761441426257</v>
+        <v>0.27900338694769261</v>
       </c>
       <c r="AA46" s="135">
         <f t="shared" si="23"/>
-        <v>6.5777452282427248E-2</v>
+        <v>5.1254225716573586E-2</v>
       </c>
       <c r="AC46" s="158">
         <f t="shared" si="0"/>
@@ -10605,11 +10605,11 @@
       </c>
       <c r="AD46" s="159">
         <f t="shared" si="1"/>
-        <v>0.72839506172839508</v>
+        <v>0.72636815920398012</v>
       </c>
       <c r="AE46" s="160">
         <f t="shared" si="13"/>
-        <v>-0.12667746234775107</v>
+        <v>-0.10987684197311723</v>
       </c>
     </row>
     <row r="47" spans="1:31" x14ac:dyDescent="0.2">
@@ -10625,43 +10625,43 @@
       </c>
       <c r="R47" s="117">
         <f t="shared" si="14"/>
-        <v>0.75308641975308654</v>
+        <v>0.75124378109452739</v>
       </c>
       <c r="S47" s="129">
         <f t="shared" si="15"/>
-        <v>9.3230143162290542</v>
+        <v>1.9330071831962097</v>
       </c>
       <c r="T47" s="129">
         <f t="shared" si="16"/>
-        <v>1.7211247915998102</v>
+        <v>1.3135500543376355</v>
       </c>
       <c r="U47" s="129">
         <f t="shared" si="17"/>
-        <v>0.36956586228321364</v>
+        <v>0.19135335148629351</v>
       </c>
       <c r="V47" s="129">
         <f t="shared" si="18"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W47" s="129">
         <f t="shared" si="19"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X47" s="129">
         <f t="shared" si="20"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y47" s="129">
         <f t="shared" si="21"/>
-        <v>1.1932467762058712</v>
+        <v>0.41725444196353489</v>
       </c>
       <c r="Z47" s="129">
         <f t="shared" si="22"/>
-        <v>0.25430734957642431</v>
+        <v>0.29974404521447434</v>
       </c>
       <c r="AA47" s="135">
         <f t="shared" si="23"/>
-        <v>6.7916505253158135E-2</v>
+        <v>5.6154090862684865E-2</v>
       </c>
       <c r="AC47" s="158">
         <f t="shared" si="0"/>
@@ -10669,11 +10669,11 @@
       </c>
       <c r="AD47" s="159">
         <f t="shared" si="1"/>
-        <v>0.75308641975308654</v>
+        <v>0.75124378109452739</v>
       </c>
       <c r="AE47" s="160">
         <f t="shared" si="13"/>
-        <v>-0.1139099244926758</v>
+        <v>-0.10017474475282803</v>
       </c>
     </row>
     <row r="48" spans="1:31" x14ac:dyDescent="0.2">
@@ -10688,43 +10688,43 @@
       </c>
       <c r="R48" s="117">
         <f t="shared" si="14"/>
-        <v>0.77777777777777757</v>
+        <v>0.77611940298507442</v>
       </c>
       <c r="S48" s="129">
         <f t="shared" si="15"/>
-        <v>10.930276002175972</v>
+        <v>2.5425308652218259</v>
       </c>
       <c r="T48" s="129">
         <f t="shared" si="16"/>
-        <v>2.0178419090943427</v>
+        <v>1.7277439966079235</v>
       </c>
       <c r="U48" s="129">
         <f t="shared" si="17"/>
-        <v>0.43327798700319359</v>
+        <v>0.25169166806358295</v>
       </c>
       <c r="V48" s="129">
         <f t="shared" si="18"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W48" s="129">
         <f t="shared" si="19"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X48" s="129">
         <f t="shared" si="20"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y48" s="129">
         <f t="shared" si="21"/>
-        <v>1.2161349505004408</v>
+        <v>0.44002475277648928</v>
       </c>
       <c r="Z48" s="129">
         <f t="shared" si="22"/>
-        <v>0.25995543048210035</v>
+        <v>0.31709053337958748</v>
       </c>
       <c r="AA48" s="135">
         <f t="shared" si="23"/>
-        <v>6.980280997743922E-2</v>
+        <v>6.0403534039305359E-2</v>
       </c>
       <c r="AC48" s="158">
         <f t="shared" si="0"/>
@@ -10732,11 +10732,11 @@
       </c>
       <c r="AD48" s="159">
         <f t="shared" si="1"/>
-        <v>0.77777777777777757</v>
+        <v>0.77611940298507442</v>
       </c>
       <c r="AE48" s="160">
         <f t="shared" si="13"/>
-        <v>-0.10195304955261535</v>
+        <v>-9.0921565565677445E-2</v>
       </c>
     </row>
     <row r="49" spans="17:31" x14ac:dyDescent="0.2">
@@ -10745,43 +10745,43 @@
       </c>
       <c r="R49" s="117">
         <f t="shared" si="14"/>
-        <v>0.80246913580246892</v>
+        <v>0.80099502487562169</v>
       </c>
       <c r="S49" s="129">
         <f t="shared" si="15"/>
-        <v>12.767680658793845</v>
+        <v>3.3194634612261211</v>
       </c>
       <c r="T49" s="129">
         <f t="shared" si="16"/>
-        <v>2.3570457973905348</v>
+        <v>2.2556985032283641</v>
       </c>
       <c r="U49" s="129">
         <f t="shared" si="17"/>
-        <v>0.50611301795494612</v>
+        <v>0.32860222350111951</v>
       </c>
       <c r="V49" s="129">
         <f t="shared" si="18"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W49" s="129">
         <f t="shared" si="19"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X49" s="129">
         <f t="shared" si="20"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y49" s="129">
         <f t="shared" si="21"/>
-        <v>1.2359244757316503</v>
+        <v>0.45860114884800435</v>
       </c>
       <c r="Z49" s="129">
         <f t="shared" si="22"/>
-        <v>0.26486598740526063</v>
+        <v>0.33132268309242324</v>
       </c>
       <c r="AA49" s="135">
         <f t="shared" si="23"/>
-        <v>7.1459569507770701E-2</v>
+        <v>6.3998359433168672E-2</v>
       </c>
       <c r="AC49" s="158">
         <f t="shared" si="0"/>
@@ -10789,11 +10789,11 @@
       </c>
       <c r="AD49" s="159">
         <f t="shared" si="1"/>
-        <v>0.80246913580246892</v>
+        <v>0.80099502487562169</v>
       </c>
       <c r="AE49" s="160">
         <f t="shared" si="13"/>
-        <v>-9.0677015761655322E-2</v>
+        <v>-8.2032126539623051E-2</v>
       </c>
     </row>
     <row r="50" spans="17:31" x14ac:dyDescent="0.2">
@@ -10802,43 +10802,43 @@
       </c>
       <c r="R50" s="117">
         <f t="shared" si="14"/>
-        <v>0.82716049382716039</v>
+        <v>0.82587064676616906</v>
       </c>
       <c r="S50" s="129">
         <f t="shared" si="15"/>
-        <v>14.862212481749824</v>
+        <v>4.303533368910303</v>
       </c>
       <c r="T50" s="129">
         <f t="shared" si="16"/>
-        <v>2.7437180178770948</v>
+        <v>2.9244104935134931</v>
       </c>
       <c r="U50" s="129">
         <f t="shared" si="17"/>
-        <v>0.58914061321272659</v>
+        <v>0.42601783404262555</v>
       </c>
       <c r="V50" s="129">
         <f t="shared" si="18"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W50" s="129">
         <f t="shared" si="19"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X50" s="129">
         <f t="shared" si="20"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y50" s="129">
         <f t="shared" si="21"/>
-        <v>1.253018363735048</v>
+        <v>0.47356159328931258</v>
       </c>
       <c r="Z50" s="129">
         <f t="shared" si="22"/>
-        <v>0.26912805807091206</v>
+        <v>0.34283755974815244</v>
       </c>
       <c r="AA50" s="135">
         <f t="shared" si="23"/>
-        <v>7.2910363157462535E-2</v>
+        <v>6.6981358170934271E-2</v>
       </c>
       <c r="AC50" s="158">
         <f t="shared" si="0"/>
@@ -10846,11 +10846,11 @@
       </c>
       <c r="AD50" s="159">
         <f t="shared" si="1"/>
-        <v>0.82716049382716039</v>
+        <v>0.82587064676616906</v>
       </c>
       <c r="AE50" s="160">
         <f t="shared" si="13"/>
-        <v>-7.9959889996252656E-2</v>
+        <v>-7.3421218367957439E-2</v>
       </c>
     </row>
     <row r="51" spans="17:31" x14ac:dyDescent="0.2">
@@ -10859,43 +10859,43 @@
       </c>
       <c r="R51" s="117">
         <f t="shared" si="14"/>
-        <v>0.85185185185185175</v>
+        <v>0.85074626865671632</v>
       </c>
       <c r="S51" s="129">
         <f t="shared" si="15"/>
-        <v>17.243449645369402</v>
+        <v>5.5425502059554006</v>
       </c>
       <c r="T51" s="129">
         <f t="shared" si="16"/>
-        <v>3.1833190072105726</v>
+        <v>3.7663683753951114</v>
       </c>
       <c r="U51" s="129">
         <f t="shared" si="17"/>
-        <v>0.6835332566029656</v>
+        <v>0.54867129667720305</v>
       </c>
       <c r="V51" s="129">
         <f t="shared" si="18"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W51" s="129">
         <f t="shared" si="19"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X51" s="129">
         <f t="shared" si="20"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y51" s="129">
         <f t="shared" si="21"/>
-        <v>1.2677786885825035</v>
+        <v>0.48550455893174055</v>
       </c>
       <c r="Z51" s="129">
         <f t="shared" si="22"/>
-        <v>0.27282361554777873</v>
+        <v>0.35206411080944089</v>
       </c>
       <c r="AA51" s="135">
         <f t="shared" si="23"/>
-        <v>7.4178086312115504E-2</v>
+        <v>6.9421340826677683E-2</v>
       </c>
       <c r="AC51" s="158">
         <f t="shared" si="0"/>
@@ -10903,11 +10903,11 @@
       </c>
       <c r="AD51" s="159">
         <f t="shared" si="1"/>
-        <v>0.85185185185185175</v>
+        <v>0.85074626865671632</v>
       </c>
       <c r="AE51" s="160">
         <f t="shared" si="13"/>
-        <v>-6.9681292615027479E-2</v>
+        <v>-6.4998100771817696E-2</v>
       </c>
     </row>
     <row r="52" spans="17:31" x14ac:dyDescent="0.2">
@@ -10916,43 +10916,43 @@
       </c>
       <c r="R52" s="117">
         <f t="shared" si="14"/>
-        <v>0.87654320987654311</v>
+        <v>0.87562189054726358</v>
       </c>
       <c r="S52" s="129">
         <f t="shared" si="15"/>
-        <v>19.94378104827738</v>
+        <v>7.0938061794239253</v>
       </c>
       <c r="T52" s="129">
         <f t="shared" si="16"/>
-        <v>3.6818280908006389</v>
+        <v>4.8205043278916362</v>
       </c>
       <c r="U52" s="129">
         <f t="shared" si="17"/>
-        <v>0.79057484953808987</v>
+        <v>0.70223411429980287</v>
       </c>
       <c r="V52" s="129">
         <f t="shared" si="18"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W52" s="129">
         <f t="shared" si="19"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X52" s="129">
         <f t="shared" si="20"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y52" s="129">
         <f t="shared" si="21"/>
-        <v>1.2805259605188766</v>
+        <v>0.49498614224828158</v>
       </c>
       <c r="Z52" s="129">
         <f t="shared" si="22"/>
-        <v>0.27602665575770935</v>
+        <v>0.35941084431036469</v>
       </c>
       <c r="AA52" s="135">
         <f t="shared" si="23"/>
-        <v>7.5284276561896665E-2</v>
+        <v>7.1396779386914758E-2</v>
       </c>
       <c r="AC52" s="158">
         <f t="shared" si="0"/>
@@ -10960,11 +10960,11 @@
       </c>
       <c r="AD52" s="159">
         <f t="shared" si="1"/>
-        <v>0.87654320987654311</v>
+        <v>0.87562189054726358</v>
       </c>
       <c r="AE52" s="160">
         <f t="shared" si="13"/>
-        <v>-5.9713577299716769E-2</v>
+        <v>-5.6657887658762368E-2</v>
       </c>
     </row>
     <row r="53" spans="17:31" x14ac:dyDescent="0.2">
@@ -10973,43 +10973,43 @@
       </c>
       <c r="R53" s="117">
         <f t="shared" si="14"/>
-        <v>0.90123456790123446</v>
+        <v>0.90049751243781084</v>
       </c>
       <c r="S53" s="129">
         <f t="shared" si="15"/>
-        <v>22.998641787083621</v>
+        <v>9.0256854619755629</v>
       </c>
       <c r="T53" s="129">
         <f t="shared" si="16"/>
-        <v>4.2457869536859842</v>
+        <v>6.1332879319202185</v>
       </c>
       <c r="U53" s="129">
         <f t="shared" si="17"/>
-        <v>0.91167004523319917</v>
+        <v>0.89347581200107262</v>
       </c>
       <c r="V53" s="129">
         <f t="shared" si="18"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W53" s="129">
         <f t="shared" si="19"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X53" s="129">
         <f t="shared" si="20"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y53" s="129">
         <f t="shared" si="21"/>
-        <v>1.2915408019288817</v>
+        <v>0.50249098834064554</v>
       </c>
       <c r="Z53" s="129">
         <f t="shared" si="22"/>
-        <v>0.27880300564052873</v>
+        <v>0.36523960676762079</v>
       </c>
       <c r="AA53" s="135">
         <f t="shared" si="23"/>
-        <v>7.6248734192927256E-2</v>
+        <v>7.298507205045579E-2</v>
       </c>
       <c r="AC53" s="158">
         <f t="shared" si="0"/>
@@ -11017,11 +11017,11 @@
       </c>
       <c r="AD53" s="159">
         <f t="shared" si="1"/>
-        <v>0.90123456790123446</v>
+        <v>0.90049751243781084</v>
       </c>
       <c r="AE53" s="160">
         <f t="shared" si="13"/>
-        <v>-4.9906980966632077E-2</v>
+        <v>-4.8265839243006883E-2</v>
       </c>
     </row>
     <row r="54" spans="17:31" x14ac:dyDescent="0.2">
@@ -11030,43 +11030,43 @@
       </c>
       <c r="R54" s="117">
         <f t="shared" si="14"/>
-        <v>0.92592592592592582</v>
+        <v>0.9253731343283581</v>
       </c>
       <c r="S54" s="129">
         <f t="shared" si="15"/>
-        <v>26.446769357223328</v>
+        <v>11.419508788604851</v>
       </c>
       <c r="T54" s="129">
         <f t="shared" si="16"/>
-        <v>4.882346937857144</v>
+        <v>7.7599796421751961</v>
       </c>
       <c r="U54" s="129">
         <f t="shared" si="17"/>
-        <v>1.0483544045506517</v>
+        <v>1.1304465384415061</v>
       </c>
       <c r="V54" s="129">
         <f t="shared" si="18"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W54" s="129">
         <f t="shared" si="19"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X54" s="129">
         <f t="shared" si="20"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y54" s="129">
         <f t="shared" si="21"/>
-        <v>1.3010669269379471</v>
+        <v>0.50842460263644196</v>
       </c>
       <c r="Z54" s="129">
         <f t="shared" si="22"/>
-        <v>0.28121059060758774</v>
+        <v>0.36985663573764782</v>
       </c>
       <c r="AA54" s="135">
         <f t="shared" si="23"/>
-        <v>7.708935485657227E-2</v>
+        <v>7.4256615079238378E-2</v>
       </c>
       <c r="AC54" s="158">
         <f t="shared" si="0"/>
@@ -11074,11 +11074,11 @@
       </c>
       <c r="AD54" s="159">
         <f t="shared" si="1"/>
-        <v>0.92592592592592582</v>
+        <v>0.9253731343283581</v>
       </c>
       <c r="AE54" s="160">
         <f t="shared" si="13"/>
-        <v>-4.0059166658069092E-2</v>
+        <v>-3.9623591391823025E-2</v>
       </c>
     </row>
     <row r="55" spans="17:31" x14ac:dyDescent="0.2">
@@ -11087,43 +11087,43 @@
       </c>
       <c r="R55" s="117">
         <f t="shared" si="14"/>
-        <v>0.95061728395061729</v>
+        <v>0.95024875621890548</v>
       </c>
       <c r="S55" s="129">
         <f t="shared" si="15"/>
-        <v>30.330482838165832</v>
+        <v>14.371643883165621</v>
       </c>
       <c r="T55" s="129">
         <f t="shared" si="16"/>
-        <v>5.5993205827312851</v>
+        <v>9.7660649002032969</v>
       </c>
       <c r="U55" s="129">
         <f t="shared" si="17"/>
-        <v>1.2023054629488972</v>
+        <v>1.4226859823997282</v>
       </c>
       <c r="V55" s="129">
         <f t="shared" si="18"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W55" s="129">
         <f t="shared" si="19"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X55" s="129">
         <f t="shared" si="20"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y55" s="129">
         <f t="shared" si="21"/>
-        <v>1.3093147422195068</v>
+        <v>0.51311733299329509</v>
       </c>
       <c r="Z55" s="129">
         <f t="shared" si="22"/>
-        <v>0.28329997056065431</v>
+        <v>0.37351350065021371</v>
       </c>
       <c r="AA55" s="135">
         <f t="shared" si="23"/>
-        <v>7.782210705623116E-2</v>
+        <v>7.5272278858699151E-2</v>
       </c>
       <c r="AC55" s="158">
         <f t="shared" si="0"/>
@@ -11131,11 +11131,11 @@
       </c>
       <c r="AD55" s="159">
         <f t="shared" si="1"/>
-        <v>0.95061728395061729</v>
+        <v>0.95024875621890548</v>
       </c>
       <c r="AE55" s="160">
         <f t="shared" si="13"/>
-        <v>-2.9836323237022209E-2</v>
+        <v>-3.037915974337899E-2</v>
       </c>
     </row>
     <row r="56" spans="17:31" x14ac:dyDescent="0.2">
@@ -11144,43 +11144,43 @@
       </c>
       <c r="R56" s="117">
         <f t="shared" si="14"/>
-        <v>0.97530864197530864</v>
+        <v>0.97512437810945274</v>
       </c>
       <c r="S56" s="129">
         <f t="shared" si="15"/>
-        <v>34.695987616838806</v>
+        <v>17.995916176232406</v>
       </c>
       <c r="T56" s="129">
         <f t="shared" si="16"/>
-        <v>6.4052378802454824</v>
+        <v>12.228892306576691</v>
       </c>
       <c r="U56" s="129">
         <f t="shared" si="17"/>
-        <v>1.3753548097704866</v>
+        <v>1.7814620159323715</v>
       </c>
       <c r="V56" s="129">
         <f t="shared" si="18"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W56" s="129">
         <f t="shared" si="19"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X56" s="129">
         <f t="shared" si="20"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y56" s="129">
         <f t="shared" si="21"/>
-        <v>1.3164651252438047</v>
+        <v>0.5168336079784428</v>
       </c>
       <c r="Z56" s="129">
         <f t="shared" si="22"/>
-        <v>0.28511501178818738</v>
+        <v>0.37641283283454952</v>
       </c>
       <c r="AA56" s="135">
         <f t="shared" si="23"/>
-        <v>7.8461102534847768E-2</v>
+        <v>7.6082979244401522E-2</v>
       </c>
       <c r="AC56" s="158">
         <f t="shared" si="0"/>
@@ -11188,11 +11188,11 @@
       </c>
       <c r="AD56" s="159">
         <f t="shared" si="1"/>
-        <v>0.97530864197530864</v>
+        <v>0.97512437810945274</v>
       </c>
       <c r="AE56" s="160">
         <f t="shared" si="13"/>
-        <v>-1.8478166964546325E-2</v>
+        <v>-1.9682470324949668E-2</v>
       </c>
     </row>
     <row r="57" spans="17:31" x14ac:dyDescent="0.2">
@@ -11205,39 +11205,39 @@
       </c>
       <c r="S57" s="129">
         <f t="shared" si="15"/>
-        <v>39.59370854492181</v>
+        <v>22.426358656651079</v>
       </c>
       <c r="T57" s="129">
         <f t="shared" si="16"/>
-        <v>7.3094077791361309</v>
+        <v>15.239542246982523</v>
       </c>
       <c r="U57" s="129">
         <f t="shared" si="17"/>
-        <v>1.569501294653463</v>
+        <v>2.2200429092498828</v>
       </c>
       <c r="V57" s="129">
         <f t="shared" si="18"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W57" s="129">
         <f t="shared" si="19"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X57" s="129">
         <f t="shared" si="20"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y57" s="129">
         <f t="shared" si="21"/>
-        <v>1.3226731077108129</v>
+        <v>0.5197826905807269</v>
       </c>
       <c r="Z57" s="129">
         <f t="shared" si="22"/>
-        <v>0.28669360664164567</v>
+        <v>0.37871575368072741</v>
       </c>
       <c r="AA57" s="135">
         <f t="shared" si="23"/>
-        <v>7.9018721463883237E-2</v>
+        <v>7.6730370122441868E-2</v>
       </c>
       <c r="AC57" s="158">
         <f t="shared" si="0"/>
@@ -11258,43 +11258,43 @@
       </c>
       <c r="R58" s="117">
         <f t="shared" si="14"/>
-        <v>1.0246913580246915</v>
+        <v>1.0248756218905473</v>
       </c>
       <c r="S58" s="129">
         <f t="shared" si="15"/>
-        <v>45.078654820580034</v>
+        <v>27.820344693367897</v>
       </c>
       <c r="T58" s="129">
         <f t="shared" si="16"/>
-        <v>8.3219855458778635</v>
+        <v>18.904955760816645</v>
       </c>
       <c r="U58" s="129">
         <f t="shared" si="17"/>
-        <v>1.7869254915049195</v>
+        <v>2.7540074568049362</v>
       </c>
       <c r="V58" s="129">
         <f t="shared" si="18"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W58" s="129">
         <f t="shared" si="19"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X58" s="129">
         <f t="shared" si="20"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y58" s="129">
         <f t="shared" si="21"/>
-        <v>1.3280713101470438</v>
+        <v>0.52212901569510739</v>
       </c>
       <c r="Z58" s="129">
         <f t="shared" si="22"/>
-        <v>0.28806838550308861</v>
+        <v>0.38054933309889089</v>
       </c>
       <c r="AA58" s="135">
         <f t="shared" si="23"/>
-        <v>7.9505765662489875E-2</v>
+        <v>7.7248025371903839E-2</v>
       </c>
       <c r="AC58" s="158">
         <f t="shared" si="0"/>
@@ -11302,7 +11302,7 @@
       </c>
       <c r="AD58" s="159">
         <f t="shared" si="1"/>
-        <v>1.0246913580246915</v>
+        <v>1.0248756218905473</v>
       </c>
       <c r="AE58" s="160" t="e">
         <f t="shared" si="13"/>
@@ -11315,43 +11315,43 @@
       </c>
       <c r="R59" s="117">
         <f t="shared" si="14"/>
-        <v>1.0493827160493827</v>
+        <v>1.0497512437810945</v>
       </c>
       <c r="S59" s="129">
         <f t="shared" si="15"/>
-        <v>51.210820342780124</v>
+        <v>34.36215337257147</v>
       </c>
       <c r="T59" s="129">
         <f t="shared" si="16"/>
-        <v>9.4540466742277243</v>
+        <v>23.350357319969593</v>
       </c>
       <c r="U59" s="129">
         <f t="shared" si="17"/>
-        <v>2.0300055686137046</v>
+        <v>3.4015979191838146</v>
       </c>
       <c r="V59" s="129">
         <f t="shared" si="18"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W59" s="129">
         <f t="shared" si="19"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X59" s="129">
         <f t="shared" si="20"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y59" s="129">
         <f t="shared" si="21"/>
-        <v>1.3327730520587682</v>
+        <v>0.52400127125602336</v>
       </c>
       <c r="Z59" s="129">
         <f t="shared" si="22"/>
-        <v>0.28926738845515332</v>
+        <v>0.38201329997299865</v>
       </c>
       <c r="AA59" s="135">
         <f t="shared" si="23"/>
-        <v>7.9931621829813129E-2</v>
+        <v>7.766274297227535E-2</v>
       </c>
       <c r="AC59" s="158">
         <f t="shared" si="0"/>
@@ -11359,7 +11359,7 @@
       </c>
       <c r="AD59" s="159">
         <f t="shared" si="1"/>
-        <v>1.0493827160493827</v>
+        <v>1.0497512437810945</v>
       </c>
       <c r="AE59" s="160" t="e">
         <f t="shared" si="13"/>
@@ -11372,43 +11372,43 @@
       </c>
       <c r="R60" s="117">
         <f t="shared" si="14"/>
-        <v>1.0740740740740742</v>
+        <v>1.0746268656716418</v>
       </c>
       <c r="S60" s="129">
         <f t="shared" si="15"/>
-        <v>58.055623818019448</v>
+        <v>42.267023437842923</v>
       </c>
       <c r="T60" s="129">
         <f t="shared" si="16"/>
-        <v>10.71766813347568</v>
+        <v>28.722009631473338</v>
       </c>
       <c r="U60" s="129">
         <f t="shared" si="17"/>
-        <v>2.3013347345555122</v>
+        <v>4.1841213330659404</v>
       </c>
       <c r="V60" s="129">
         <f t="shared" si="18"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W60" s="129">
         <f t="shared" si="19"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X60" s="129">
         <f t="shared" si="20"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y60" s="129">
         <f t="shared" si="21"/>
-        <v>1.3368751119396871</v>
+        <v>0.52549998173866808</v>
       </c>
       <c r="Z60" s="129">
         <f t="shared" si="22"/>
-        <v>0.29031467956334678</v>
+        <v>0.38318573113302018</v>
       </c>
       <c r="AA60" s="135">
         <f t="shared" si="23"/>
-        <v>8.0304423243384646E-2</v>
+        <v>7.7995781080402948E-2</v>
       </c>
       <c r="AC60" s="158">
         <f t="shared" si="0"/>
@@ -11416,7 +11416,7 @@
       </c>
       <c r="AD60" s="159">
         <f t="shared" si="1"/>
-        <v>1.0740740740740742</v>
+        <v>1.0746268656716418</v>
       </c>
       <c r="AE60" s="160" t="e">
         <f t="shared" si="13"/>
@@ -11429,43 +11429,43 @@
       </c>
       <c r="R61" s="117">
         <f t="shared" si="14"/>
-        <v>1.0987654320987654</v>
+        <v>1.099502487562189</v>
       </c>
       <c r="S61" s="129">
         <f t="shared" si="15"/>
-        <v>65.684393518993474</v>
+        <v>51.785759441308585</v>
       </c>
       <c r="T61" s="129">
         <f t="shared" si="16"/>
-        <v>12.126017859904362</v>
+        <v>35.190343687999587</v>
       </c>
       <c r="U61" s="129">
         <f t="shared" si="17"/>
-        <v>2.6037404541083355</v>
+        <v>5.126405485970464</v>
       </c>
       <c r="V61" s="129">
         <f t="shared" si="18"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W61" s="129">
         <f t="shared" si="19"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X61" s="129">
         <f t="shared" si="20"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y61" s="129">
         <f t="shared" si="21"/>
-        <v>1.3404601416348407</v>
+        <v>0.52670364858884644</v>
       </c>
       <c r="Z61" s="129">
         <f t="shared" si="22"/>
-        <v>0.29123089678070507</v>
+        <v>0.38412770546709679</v>
       </c>
       <c r="AA61" s="135">
         <f t="shared" si="23"/>
-        <v>8.0631202984527403E-2</v>
+        <v>7.8263943243275527E-2</v>
       </c>
       <c r="AC61" s="158">
         <f t="shared" si="0"/>
@@ -11473,7 +11473,7 @@
       </c>
       <c r="AD61" s="159">
         <f t="shared" si="1"/>
-        <v>1.0987654320987654</v>
+        <v>1.099502487562189</v>
       </c>
       <c r="AE61" s="160" t="e">
         <f t="shared" si="13"/>
@@ -11486,43 +11486,43 @@
       </c>
       <c r="R62" s="117">
         <f t="shared" si="14"/>
-        <v>1.1234567901234569</v>
+        <v>1.1243781094527365</v>
       </c>
       <c r="S62" s="129">
         <f t="shared" si="15"/>
-        <v>74.174902319225055</v>
+        <v>63.209962383785772</v>
       </c>
       <c r="T62" s="129">
         <f t="shared" si="16"/>
-        <v>13.693453529710952</v>
+        <v>42.953513181784068</v>
       </c>
       <c r="U62" s="129">
         <f t="shared" si="17"/>
-        <v>2.9403056571155499</v>
+        <v>6.2573167107740657</v>
       </c>
       <c r="V62" s="129">
         <f t="shared" si="18"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W62" s="129">
         <f t="shared" si="19"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X62" s="129">
         <f t="shared" si="20"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y62" s="129">
         <f t="shared" si="21"/>
-        <v>1.3435987565710525</v>
+        <v>0.52767362627345171</v>
       </c>
       <c r="Z62" s="129">
         <f t="shared" si="22"/>
-        <v>0.29203373678198868</v>
+        <v>0.38488702710231709</v>
       </c>
       <c r="AA62" s="135">
         <f t="shared" si="23"/>
-        <v>8.0918034923987248E-2</v>
+        <v>7.8480489585325663E-2</v>
       </c>
       <c r="AC62" s="158">
         <f t="shared" si="0"/>
@@ -11530,7 +11530,7 @@
       </c>
       <c r="AD62" s="159">
         <f t="shared" si="1"/>
-        <v>1.1234567901234569</v>
+        <v>1.1243781094527365</v>
       </c>
       <c r="AE62" s="160" t="e">
         <f t="shared" si="13"/>
@@ -11543,43 +11543,43 @@
       </c>
       <c r="R63" s="117">
         <f t="shared" si="14"/>
-        <v>1.1481481481481484</v>
+        <v>1.1492537313432838</v>
       </c>
       <c r="S63" s="129">
         <f t="shared" si="15"/>
-        <v>83.611959477491524</v>
+        <v>76.877967148800252</v>
       </c>
       <c r="T63" s="129">
         <f t="shared" si="16"/>
-        <v>15.435631808528241</v>
+        <v>52.241429211193598</v>
       </c>
       <c r="U63" s="129">
         <f t="shared" si="17"/>
-        <v>3.3143921969205619</v>
+        <v>7.6103476475715075</v>
       </c>
       <c r="V63" s="129">
         <f t="shared" si="18"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W63" s="129">
         <f t="shared" si="19"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X63" s="129">
         <f t="shared" si="20"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y63" s="129">
         <f t="shared" si="21"/>
-        <v>1.346351331808286</v>
+        <v>0.52845794668938817</v>
       </c>
       <c r="Z63" s="129">
         <f t="shared" si="22"/>
-        <v>0.29273837773307998</v>
+        <v>0.38550116161472414</v>
       </c>
       <c r="AA63" s="135">
         <f t="shared" si="23"/>
-        <v>8.1170160810602091E-2</v>
+        <v>7.8655880864763536E-2</v>
       </c>
       <c r="AC63" s="158">
         <f t="shared" si="0"/>
@@ -11587,7 +11587,7 @@
       </c>
       <c r="AD63" s="159">
         <f t="shared" si="1"/>
-        <v>1.1481481481481484</v>
+        <v>1.1492537313432838</v>
       </c>
       <c r="AE63" s="160" t="e">
         <f t="shared" si="13"/>
@@ -11600,43 +11600,43 @@
       </c>
       <c r="R64" s="117">
         <f t="shared" si="14"/>
-        <v>1.1728395061728394</v>
+        <v>1.1741293532338306</v>
       </c>
       <c r="S64" s="129">
         <f t="shared" si="15"/>
-        <v>94.088066646031905</v>
+        <v>93.181580669692693</v>
       </c>
       <c r="T64" s="129">
         <f t="shared" si="16"/>
-        <v>17.369629457319185</v>
+        <v>63.320339115117257</v>
       </c>
       <c r="U64" s="129">
         <f t="shared" si="17"/>
-        <v>3.7296668546429541</v>
+        <v>9.2242842721636293</v>
       </c>
       <c r="V64" s="129">
         <f t="shared" si="18"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W64" s="129">
         <f t="shared" si="19"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X64" s="129">
         <f t="shared" si="20"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y64" s="129">
         <f t="shared" si="21"/>
-        <v>1.3487695369447354</v>
+        <v>0.529094295768477</v>
       </c>
       <c r="Z64" s="129">
         <f t="shared" si="22"/>
-        <v>0.29335784497543038</v>
+        <v>0.38599953084019439</v>
       </c>
       <c r="AA64" s="135">
         <f t="shared" si="23"/>
-        <v>8.1392103153955578E-2</v>
+        <v>7.8798375254022557E-2</v>
       </c>
       <c r="AC64" s="158">
         <f t="shared" si="0"/>
@@ -11644,7 +11644,7 @@
       </c>
       <c r="AD64" s="159">
         <f t="shared" si="1"/>
-        <v>1.1728395061728394</v>
+        <v>1.1741293532338306</v>
       </c>
       <c r="AE64" s="160" t="e">
         <f t="shared" si="13"/>
@@ -11657,43 +11657,43 @@
       </c>
       <c r="R65" s="117">
         <f t="shared" si="14"/>
-        <v>1.1975308641975309</v>
+        <v>1.1990049751243781</v>
       </c>
       <c r="S65" s="129">
         <f t="shared" si="15"/>
-        <v>105.70414675778086</v>
+        <v>112.57372831505542</v>
       </c>
       <c r="T65" s="129">
         <f t="shared" si="16"/>
-        <v>19.51407789249302</v>
+        <v>76.498022475388581</v>
       </c>
       <c r="U65" s="129">
         <f t="shared" si="17"/>
-        <v>4.1901302323915548</v>
+        <v>11.14396283141321</v>
       </c>
       <c r="V65" s="129">
         <f t="shared" si="18"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W65" s="129">
         <f t="shared" si="19"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X65" s="129">
         <f t="shared" si="20"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y65" s="129">
         <f t="shared" si="21"/>
-        <v>1.3508976427741337</v>
+        <v>0.52961231984433843</v>
       </c>
       <c r="Z65" s="129">
         <f t="shared" si="22"/>
-        <v>0.29390332547106568</v>
+        <v>0.38640529667320905</v>
       </c>
       <c r="AA65" s="135">
         <f t="shared" si="23"/>
-        <v>8.1587764409679644E-2</v>
+        <v>7.8914501466367651E-2</v>
       </c>
       <c r="AC65" s="158">
         <f t="shared" si="0"/>
@@ -11701,7 +11701,7 @@
       </c>
       <c r="AD65" s="159">
         <f t="shared" si="1"/>
-        <v>1.1975308641975309</v>
+        <v>1.1990049751243781</v>
       </c>
       <c r="AE65" s="160" t="e">
         <f t="shared" si="13"/>
@@ -11714,43 +11714,43 @@
       </c>
       <c r="R66" s="117">
         <f t="shared" si="14"/>
-        <v>1.2222222222222221</v>
+        <v>1.2238805970149254</v>
       </c>
       <c r="S66" s="129">
         <f t="shared" si="15"/>
-        <v>118.57035584815631</v>
+        <v>135.57713180653354</v>
       </c>
       <c r="T66" s="129">
         <f t="shared" si="16"/>
-        <v>21.889313056596993</v>
+        <v>92.129688083697175</v>
       </c>
       <c r="U66" s="129">
         <f t="shared" si="17"/>
-        <v>4.7001489340172293</v>
+        <v>13.421128892641988</v>
       </c>
       <c r="V66" s="129">
         <f t="shared" si="18"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W66" s="129">
         <f t="shared" si="19"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X66" s="129">
         <f t="shared" si="20"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y66" s="129">
         <f t="shared" si="21"/>
-        <v>1.3527736306600466</v>
+        <v>0.53003540868252186</v>
       </c>
       <c r="Z66" s="129">
         <f t="shared" si="22"/>
-        <v>0.29438443703351314</v>
+        <v>0.38673674356729099</v>
       </c>
       <c r="AA66" s="135">
         <f t="shared" si="23"/>
-        <v>8.1760513434124243E-2</v>
+        <v>7.9009431088519225E-2</v>
       </c>
       <c r="AC66" s="158">
         <f t="shared" si="0"/>
@@ -11758,7 +11758,7 @@
       </c>
       <c r="AD66" s="159">
         <f t="shared" si="1"/>
-        <v>1.2222222222222221</v>
+        <v>1.2238805970149254</v>
       </c>
       <c r="AE66" s="160" t="e">
         <f t="shared" si="13"/>
@@ -11771,43 +11771,43 @@
       </c>
       <c r="R67" s="130">
         <f>MAX((Q67-rc_vg)/(sc_vg-rc_vg),0)</f>
-        <v>1.2469135802469136</v>
+        <v>1.2487562189054726</v>
       </c>
       <c r="S67" s="131">
         <f t="shared" si="15"/>
-        <v>132.80698953325199</v>
+        <v>162.79416054932216</v>
       </c>
       <c r="T67" s="131">
         <f t="shared" si="16"/>
-        <v>24.517542763558772</v>
+        <v>110.6246682859358</v>
       </c>
       <c r="U67" s="131">
         <f t="shared" si="17"/>
-        <v>5.2644914980615525</v>
+        <v>16.115412552167705</v>
       </c>
       <c r="V67" s="131">
         <f t="shared" si="18"/>
-        <v>1.368385593142037</v>
+        <v>0.53211570172066014</v>
       </c>
       <c r="W67" s="131">
         <f t="shared" si="19"/>
-        <v>0.29839751798850311</v>
+        <v>0.38836700841750849</v>
       </c>
       <c r="X67" s="131">
         <f t="shared" si="20"/>
-        <v>8.3207940750375742E-2</v>
+        <v>7.947730954058374E-2</v>
       </c>
       <c r="Y67" s="131">
         <f t="shared" si="21"/>
-        <v>1.3544301327622559</v>
+        <v>0.5303820730203862</v>
       </c>
       <c r="Z67" s="131">
         <f t="shared" si="22"/>
-        <v>0.29480945814746984</v>
+        <v>0.38700834875355788</v>
       </c>
       <c r="AA67" s="136">
         <f t="shared" si="23"/>
-        <v>8.1913260396115545E-2</v>
+        <v>7.9087270288341283E-2</v>
       </c>
       <c r="AC67" s="161">
         <f t="shared" si="0"/>
@@ -11815,7 +11815,7 @@
       </c>
       <c r="AD67" s="162">
         <f t="shared" si="1"/>
-        <v>1.2469135802469136</v>
+        <v>1.2487562189054726</v>
       </c>
       <c r="AE67" s="163" t="e">
         <f t="shared" si="13"/>

</xml_diff>

<commit_message>
major update  : -Rename variables (from trunl to stem) - clean other variable names - corrected a bug in Qsat - updated quickstart
</commit_message>
<xml_diff>
--- a/for_development/dev_documentation/soil-root-calibration_V3.xlsx
+++ b/for_development/dev_documentation/soil-root-calibration_V3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jruffault/Dropbox/Mon Mac (MacBook-Pro-de-Julien.local)/Desktop/SurEau-Ecos/for_development/dev_documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97FF996B-4114-1845-BDE6-C587F2B868B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60DAE097-D080-024B-8F06-AC36D4994A0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{D9106142-DCBD-4E45-A888-1E539F445614}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{D9106142-DCBD-4E45-A888-1E539F445614}"/>
   </bookViews>
   <sheets>
     <sheet name="WorkSheet" sheetId="1" r:id="rId1"/>
@@ -61,12 +61,19 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="173">
   <si>
     <t>LAI</t>
   </si>
@@ -1256,6 +1263,9 @@
   </si>
   <si>
     <t xml:space="preserve"> They also can be estimated using basic soil properties such as soil texture, bulk density, organic carbon content, etc. </t>
+  </si>
+  <si>
+    <t>Sand</t>
   </si>
 </sst>
 </file>
@@ -7285,7 +7295,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B673C9AC-1A9D-EA45-B245-5C46BCC162EE}">
   <dimension ref="A1:AE67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="105" zoomScaleNormal="64" workbookViewId="0">
+    <sheetView topLeftCell="A24" zoomScale="105" zoomScaleNormal="64" workbookViewId="0">
       <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
@@ -11846,8 +11856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1432D1FA-6D1A-5B47-9BFC-4C8DE5F35F87}">
   <dimension ref="E1:O23"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11896,7 +11906,9 @@
       </c>
     </row>
     <row r="6" spans="5:15" x14ac:dyDescent="0.2">
-      <c r="I6" s="164"/>
+      <c r="I6" s="164" t="s">
+        <v>172</v>
+      </c>
       <c r="J6" s="164">
         <v>0.43</v>
       </c>

</xml_diff>